<commit_message>
Added replacement feet for 1390-B
</commit_message>
<xml_diff>
--- a/DetailedBudget.xlsx
+++ b/DetailedBudget.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="134">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -415,6 +415,12 @@
   </si>
   <si>
     <t>ARRIVED?</t>
+  </si>
+  <si>
+    <t>Replacement feet for 1390-B</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#9546k549/=y4zioh</t>
   </si>
 </sst>
 </file>
@@ -1152,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B75" workbookViewId="0">
-      <selection activeCell="I89" sqref="I89"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1190,15 +1196,15 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6">
-        <f>D18+D27+D36+D46+D66+D74+D82+D96+D105</f>
-        <v>11395.05</v>
+        <f>D18+D27+D36+D46+D66+D75+D83+D97+D106</f>
+        <v>11384.059999999998</v>
       </c>
       <c r="E3" s="7">
         <v>0.64</v>
       </c>
       <c r="F3" s="8">
         <f>D3*E3</f>
-        <v>7292.8319999999994</v>
+        <v>7285.7983999999988</v>
       </c>
       <c r="H3" s="9"/>
     </row>
@@ -1228,14 +1234,14 @@
       <c r="C5" s="5"/>
       <c r="D5" s="6">
         <f>D4-D3</f>
-        <v>1104.9500000000007</v>
+        <v>1115.9400000000023</v>
       </c>
       <c r="E5" s="7">
         <v>0.64</v>
       </c>
       <c r="F5" s="8">
         <f>D5*E5</f>
-        <v>707.16800000000046</v>
+        <v>714.20160000000146</v>
       </c>
       <c r="H5" s="9"/>
     </row>
@@ -2150,14 +2156,14 @@
         <v>34</v>
       </c>
       <c r="B72" s="2">
-        <v>59.99</v>
+        <v>49</v>
       </c>
       <c r="C72" s="1">
         <v>1</v>
       </c>
       <c r="D72" s="2">
         <f>C72*B72</f>
-        <v>59.99</v>
+        <v>49</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>51</v>
@@ -2169,415 +2175,410 @@
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
-      <c r="C74" s="10" t="s">
+    <row r="73" spans="1:9">
+      <c r="A73" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B73" s="2">
+        <v>5.96</v>
+      </c>
+      <c r="C73" s="1">
+        <v>2</v>
+      </c>
+      <c r="D73" s="2">
+        <f>C73*B73</f>
+        <v>11.92</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="C75" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D74" s="11">
+      <c r="D75" s="11">
         <f>SUM(D70:D72)</f>
-        <v>195.79000000000002</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="20">
-      <c r="A76" s="5" t="s">
+        <v>184.8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="20">
+      <c r="A77" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:9" s="19" customFormat="1">
-      <c r="A77" s="17" t="s">
+    <row r="78" spans="1:9" s="19" customFormat="1">
+      <c r="A78" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B77" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C77" s="17" t="s">
+      <c r="B78" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D77" s="18" t="s">
+      <c r="D78" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E77" s="18" t="s">
+      <c r="E78" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="F77" s="18" t="s">
+      <c r="F78" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="G77" s="18" t="s">
+      <c r="G78" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H77" s="18" t="s">
+      <c r="H78" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="I77" s="17" t="s">
+      <c r="I78" s="17" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
-      <c r="A78" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B78" s="2">
-        <v>50</v>
-      </c>
-      <c r="C78" s="1">
-        <v>1</v>
-      </c>
-      <c r="D78" s="2">
-        <f>C78*B78</f>
-        <v>50</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="1" t="s">
-        <v>83</v>
+        <v>13</v>
       </c>
       <c r="B79" s="2">
-        <v>15.99</v>
+        <v>50</v>
       </c>
       <c r="C79" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D79" s="2">
         <f>C79*B79</f>
-        <v>95.94</v>
+        <v>50</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B80" s="2">
-        <v>10</v>
+        <v>15.99</v>
       </c>
       <c r="C80" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D80" s="2">
         <f>C80*B80</f>
-        <v>10</v>
+        <v>95.94</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H80" s="2" t="s">
+      <c r="I80" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81" s="2">
+        <v>10</v>
+      </c>
+      <c r="C81" s="1">
+        <v>1</v>
+      </c>
+      <c r="D81" s="2">
+        <f>C81*B81</f>
+        <v>10</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H81" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
-      <c r="C82" s="10" t="s">
+    <row r="83" spans="1:9">
+      <c r="C83" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D82" s="11">
-        <f>SUM(D78:D79)</f>
+      <c r="D83" s="11">
+        <f>SUM(D79:D80)</f>
         <v>145.94</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="20">
-      <c r="A84" s="5" t="s">
+    <row r="85" spans="1:9" ht="20">
+      <c r="A85" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="85" spans="1:9" s="19" customFormat="1">
-      <c r="A85" s="17" t="s">
+    <row r="86" spans="1:9" s="19" customFormat="1">
+      <c r="A86" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B85" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C85" s="17" t="s">
+      <c r="B86" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D85" s="18" t="s">
+      <c r="D86" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E85" s="18" t="s">
+      <c r="E86" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="F85" s="18" t="s">
+      <c r="F86" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="G85" s="18" t="s">
+      <c r="G86" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H85" s="18" t="s">
+      <c r="H86" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="I85" s="17" t="s">
+      <c r="I86" s="17" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B86" s="2">
-        <v>4.41</v>
-      </c>
-      <c r="C86" s="1">
-        <v>200</v>
-      </c>
-      <c r="D86" s="2">
-        <f t="shared" ref="D86:D91" si="2">C86*B86</f>
-        <v>882</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="I86" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B87" s="2">
+        <v>4.41</v>
+      </c>
+      <c r="C87" s="1">
+        <v>200</v>
+      </c>
+      <c r="D87" s="2">
+        <f t="shared" ref="D87:D92" si="2">C87*B87</f>
+        <v>882</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B88" s="2">
         <v>23</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C88" s="1">
         <v>4</v>
       </c>
-      <c r="D87" s="2">
+      <c r="D88" s="2">
         <f t="shared" si="2"/>
         <v>92</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="G88" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I87" s="1" t="s">
+      <c r="I88" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:9">
+      <c r="A89" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B89" s="2">
         <v>7.27</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C89" s="1">
         <v>2</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D89" s="2">
         <f t="shared" si="2"/>
         <v>14.54</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="E89" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="F89" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="G89" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I88" s="1" t="s">
+      <c r="I89" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:9">
+      <c r="A90" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B90" s="2">
         <v>90</v>
       </c>
-      <c r="C89" s="1">
-        <v>1</v>
-      </c>
-      <c r="D89" s="2">
+      <c r="C90" s="1">
+        <v>1</v>
+      </c>
+      <c r="D90" s="2">
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-      <c r="G89" s="2" t="s">
+      <c r="G90" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H89" s="2" t="s">
+      <c r="H90" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="I89" s="1" t="s">
+      <c r="I90" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:9">
+      <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B91" s="2">
         <v>7.5</v>
       </c>
-      <c r="C90" s="1">
+      <c r="C91" s="1">
         <v>4</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D91" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="G90" s="2" t="s">
+      <c r="G91" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I90" s="1" t="s">
+      <c r="I91" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:9">
+      <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B92" s="2">
         <v>121</v>
       </c>
-      <c r="C91" s="1">
-        <v>1</v>
-      </c>
-      <c r="D91" s="2">
+      <c r="C92" s="1">
+        <v>1</v>
+      </c>
+      <c r="D92" s="2">
         <f t="shared" si="2"/>
         <v>121</v>
       </c>
-      <c r="G91" s="2" t="s">
+      <c r="G92" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I91" s="1" t="s">
+      <c r="I92" s="1" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
-      <c r="A92" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B95" s="2">
         <v>5.9</v>
       </c>
-      <c r="C94" s="1">
-        <v>1</v>
-      </c>
-      <c r="D94" s="2">
-        <f>C94*B94</f>
+      <c r="C95" s="1">
+        <v>1</v>
+      </c>
+      <c r="D95" s="2">
+        <f>C95*B95</f>
         <v>5.9</v>
       </c>
-      <c r="E94" s="2" t="s">
+      <c r="E95" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G94" s="2" t="s">
+      <c r="G95" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
-      <c r="A96" s="10"/>
-      <c r="C96" s="10" t="s">
+    <row r="97" spans="1:9">
+      <c r="A97" s="10"/>
+      <c r="C97" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D96" s="11">
-        <f>SUM(D86:D91)</f>
+      <c r="D97" s="11">
+        <f>SUM(D87:D92)</f>
         <v>1229.54</v>
       </c>
-      <c r="I96" s="15"/>
-    </row>
-    <row r="97" spans="1:9">
-      <c r="A97" s="20"/>
-      <c r="B97" s="21"/>
-      <c r="C97" s="20"/>
-      <c r="D97" s="21"/>
-      <c r="E97" s="21"/>
-      <c r="F97" s="21"/>
-      <c r="G97" s="21"/>
-      <c r="H97" s="21"/>
-      <c r="I97" s="20"/>
-    </row>
-    <row r="98" spans="1:9" ht="20">
-      <c r="A98" s="5" t="s">
+      <c r="I97" s="15"/>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" s="20"/>
+      <c r="B98" s="21"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="21"/>
+      <c r="E98" s="21"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="21"/>
+      <c r="H98" s="21"/>
+      <c r="I98" s="20"/>
+    </row>
+    <row r="99" spans="1:9" ht="20">
+      <c r="A99" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:9" s="19" customFormat="1">
-      <c r="A99" s="17" t="s">
+    <row r="100" spans="1:9" s="19" customFormat="1">
+      <c r="A100" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B99" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C99" s="17" t="s">
+      <c r="B100" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D99" s="18" t="s">
+      <c r="D100" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E99" s="18" t="s">
+      <c r="E100" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="F99" s="18" t="s">
+      <c r="F100" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="G99" s="18" t="s">
+      <c r="G100" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H99" s="18" t="s">
+      <c r="H100" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="I99" s="17" t="s">
+      <c r="I100" s="17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:9">
+      <c r="A101" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B100" s="2">
-        <v>0</v>
-      </c>
-      <c r="C100" s="1">
-        <v>1</v>
-      </c>
-      <c r="D100" s="2">
-        <v>0</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" s="15" customFormat="1">
-      <c r="A101" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="B101" s="2">
         <v>0</v>
@@ -2600,62 +2601,88 @@
       <c r="H101" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I101" s="1"/>
-    </row>
-    <row r="102" spans="1:9">
+    </row>
+    <row r="102" spans="1:9" s="15" customFormat="1">
       <c r="A102" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="B102" s="2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C102" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D102" s="2">
-        <f>C102*B102</f>
-        <v>150</v>
+        <v>0</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I102" s="1" t="s">
-        <v>78</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I102" s="1"/>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B103" s="2">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C103" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D103" s="2">
         <f>C103*B103</f>
+        <v>150</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B104" s="2">
         <v>9</v>
       </c>
-      <c r="E103" s="2" t="s">
+      <c r="C104" s="1">
+        <v>1</v>
+      </c>
+      <c r="D104" s="2">
+        <f>C104*B104</f>
+        <v>9</v>
+      </c>
+      <c r="E104" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F103" s="2" t="s">
+      <c r="F104" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G103" s="2" t="s">
+      <c r="G104" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
-      <c r="C105" s="10" t="s">
+    <row r="106" spans="1:9">
+      <c r="C106" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D105" s="11">
-        <f>SUM(D100:D102)</f>
+      <c r="D106" s="11">
+        <f>SUM(D101:D103)</f>
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More budget updates w/ purchases
</commit_message>
<xml_diff>
--- a/DetailedBudget.xlsx
+++ b/DetailedBudget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6560" yWindow="480" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2880" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="132">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -333,33 +333,9 @@
     <t>Tamper-resistant stickers (1800 labels)</t>
   </si>
   <si>
-    <t>http://www.amazon.com/Stanton-STR8150-Torque-Direct-Turntable/dp/B0000C5NYD</t>
-  </si>
-  <si>
-    <t>Turntable (Stanton STR8150)</t>
-  </si>
-  <si>
-    <t>Linear motion shaft</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Linear-Motion-Length-Chrome-Hardened/dp/B0045DWAAG/ref=sr_1_2?s=industrial&amp;ie=UTF8&amp;qid=1436546865&amp;sr=1-2</t>
-  </si>
-  <si>
-    <t>Linear bushing (pack of 10)</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Bushing-Linear-Motion-Double-Sealed/dp/B00G9TWD56/ref=sr_1_5?s=industrial&amp;ie=UTF8&amp;qid=1436546865&amp;sr=1-5</t>
-  </si>
-  <si>
-    <t>Acme screw</t>
-  </si>
-  <si>
     <t>McMaster</t>
   </si>
   <si>
-    <t>http://www.mcmaster.com/#precision-acme-lead-screws/=y2eiw1</t>
-  </si>
-  <si>
     <t>Small speakers</t>
   </si>
   <si>
@@ -369,12 +345,6 @@
     <t>http://www.digikey.com/product-search/en?lang=en&amp;site=us&amp;KeyWords=CMS0401KL-3X</t>
   </si>
   <si>
-    <t>Technics 1200 turntable</t>
-  </si>
-  <si>
-    <t>http://newjersey.craigslist.org/ele/5053966688.html</t>
-  </si>
-  <si>
     <t>0.002" acetate roll</t>
   </si>
   <si>
@@ -421,6 +391,30 @@
   </si>
   <si>
     <t>http://www.mcmaster.com/#9546k549/=y4zioh</t>
+  </si>
+  <si>
+    <t>Power strips</t>
+  </si>
+  <si>
+    <t>Extension cords</t>
+  </si>
+  <si>
+    <t>Buy in UK or borrow?</t>
+  </si>
+  <si>
+    <t>Serial # 3641</t>
+  </si>
+  <si>
+    <t>Aluminum L-extrusion</t>
+  </si>
+  <si>
+    <t>Wire nuts</t>
+  </si>
+  <si>
+    <t>Local hardware store</t>
+  </si>
+  <si>
+    <t>Spade terminal</t>
   </si>
 </sst>
 </file>
@@ -521,9 +515,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="138">
+  <cellStyleXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -691,7 +689,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="138">
+  <cellStyles count="142">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -761,6 +759,8 @@
     <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -829,6 +829,8 @@
     <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1158,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I106"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1196,15 +1198,15 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6">
-        <f>D18+D27+D36+D46+D66+D75+D83+D97+D106</f>
-        <v>11384.059999999998</v>
+        <f>D18+D27+D36+D46+D64+D73+D81+D95+D106</f>
+        <v>11576.339999999998</v>
       </c>
       <c r="E3" s="7">
         <v>0.64</v>
       </c>
       <c r="F3" s="8">
         <f>D3*E3</f>
-        <v>7285.7983999999988</v>
+        <v>7408.8575999999994</v>
       </c>
       <c r="H3" s="9"/>
     </row>
@@ -1234,14 +1236,14 @@
       <c r="C5" s="5"/>
       <c r="D5" s="6">
         <f>D4-D3</f>
-        <v>1115.9400000000023</v>
+        <v>923.66000000000167</v>
       </c>
       <c r="E5" s="7">
         <v>0.64</v>
       </c>
       <c r="F5" s="8">
         <f>D5*E5</f>
-        <v>714.20160000000146</v>
+        <v>591.14240000000109</v>
       </c>
       <c r="H5" s="9"/>
     </row>
@@ -1294,10 +1296,10 @@
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G10" s="18" t="s">
         <v>38</v>
@@ -1438,10 +1440,10 @@
         <v>3</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>38</v>
@@ -1517,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1525,7 +1527,7 @@
         <v>42</v>
       </c>
       <c r="D27" s="11">
-        <f>SUM(D22:D24)</f>
+        <f>SUM(D22:D25)</f>
         <v>513</v>
       </c>
     </row>
@@ -1556,10 +1558,10 @@
         <v>3</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G30" s="18" t="s">
         <v>38</v>
@@ -1594,13 +1596,16 @@
       <c r="G31" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="H31" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="I31" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B32" s="2">
         <v>0.48</v>
@@ -1619,7 +1624,7 @@
         <v>51</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1686,10 +1691,10 @@
         <v>3</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F39" s="18" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G39" s="18" t="s">
         <v>38</v>
@@ -1795,8 +1800,8 @@
         <v>42</v>
       </c>
       <c r="D46" s="11">
-        <f>SUM(D40:D42)</f>
-        <v>425</v>
+        <f>SUM(D40:D44)</f>
+        <v>505</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="20">
@@ -1818,10 +1823,10 @@
         <v>3</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F49" s="18" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G49" s="18" t="s">
         <v>38</v>
@@ -1844,7 +1849,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="2">
-        <f t="shared" ref="D50:D64" si="1">C50*B50</f>
+        <f t="shared" ref="D50:D62" si="1">C50*B50</f>
         <v>1500</v>
       </c>
       <c r="G50" s="2" t="s">
@@ -1890,7 +1895,7 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B54" s="2">
         <v>12.62</v>
@@ -1899,791 +1904,860 @@
         <v>2</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="B55" s="2">
-        <v>600</v>
+        <v>15.99</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="D55" s="2">
+        <f>C55*B55</f>
+        <v>15.99</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="B56" s="2">
-        <v>450</v>
+        <v>3.49</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2">
+        <f>C56*B56</f>
+        <v>3.49</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="B57" s="2">
-        <v>15.18</v>
+        <v>2.99</v>
+      </c>
+      <c r="C57" s="1">
+        <v>2</v>
+      </c>
+      <c r="D57" s="2">
+        <f>C57*B57</f>
+        <v>5.98</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B58" s="2">
-        <v>10.220000000000001</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
+      </c>
+      <c r="B59" s="2">
+        <v>269</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
-        <v>96</v>
+        <v>29</v>
+      </c>
+      <c r="B60" s="2">
+        <v>0</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1</v>
+      </c>
+      <c r="D60" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
-        <v>125</v>
+        <v>46</v>
       </c>
       <c r="B61" s="2">
-        <v>269</v>
+        <v>0</v>
       </c>
       <c r="C61" s="1">
         <v>1</v>
       </c>
+      <c r="D61" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="G61" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>126</v>
+        <v>65</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="B62" s="2">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C62" s="1">
         <v>1</v>
       </c>
       <c r="D62" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F62" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="G62" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B63" s="2">
+        <v>99</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="C64" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D64" s="11">
+        <f>SUM(D50:D62)</f>
+        <v>1615.46</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="20">
+      <c r="A66" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C63" s="1">
-        <v>1</v>
-      </c>
-      <c r="D63" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B64" s="2">
-        <v>50</v>
-      </c>
-      <c r="C64" s="1">
-        <v>1</v>
-      </c>
-      <c r="D64" s="2">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="C66" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D66" s="11">
-        <f>SUM(D50:D63)</f>
-        <v>1540</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="20">
-      <c r="A68" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" s="19" customFormat="1">
-      <c r="A69" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B69" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C69" s="17" t="s">
+      <c r="B67" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D69" s="18" t="s">
+      <c r="D67" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="F69" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="G69" s="18" t="s">
+      <c r="E67" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F67" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="G67" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H69" s="18" t="s">
+      <c r="H67" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="I69" s="17" t="s">
+      <c r="I67" s="17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="J67" s="19"/>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" s="2">
+        <v>56.8</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1</v>
+      </c>
+      <c r="D68" s="2">
+        <f>C68*B68</f>
+        <v>56.8</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69" s="2">
+        <v>79</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
+      <c r="D69" s="2">
+        <f>C69*B69</f>
+        <v>79</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B70" s="2">
-        <v>56.8</v>
+        <v>49</v>
       </c>
       <c r="C70" s="1">
         <v>1</v>
       </c>
       <c r="D70" s="2">
         <f>C70*B70</f>
-        <v>56.8</v>
+        <v>49</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71" s="1" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="B71" s="2">
-        <v>79</v>
+        <v>5.96</v>
       </c>
       <c r="C71" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D71" s="2">
         <f>C71*B71</f>
+        <v>11.92</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" s="19" customFormat="1">
+      <c r="A72" s="1"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="C73" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D73" s="11">
+        <f>SUM(D68:D71)</f>
+        <v>196.72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="20">
+      <c r="A75" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F76" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="G76" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H76" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="I76" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J76" s="19"/>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B77" s="2">
+        <v>50</v>
+      </c>
+      <c r="C77" s="1">
+        <v>1</v>
+      </c>
+      <c r="D77" s="2">
+        <f>C77*B77</f>
+        <v>50</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B78" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="C78" s="1">
+        <v>6</v>
+      </c>
+      <c r="D78" s="2">
+        <f>C78*B78</f>
+        <v>95.94</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G71" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B72" s="2">
-        <v>49</v>
-      </c>
-      <c r="C72" s="1">
-        <v>1</v>
-      </c>
-      <c r="D72" s="2">
-        <f>C72*B72</f>
-        <v>49</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B73" s="2">
-        <v>5.96</v>
-      </c>
-      <c r="C73" s="1">
-        <v>2</v>
-      </c>
-      <c r="D73" s="2">
-        <f>C73*B73</f>
-        <v>11.92</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
-      <c r="C75" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D75" s="11">
-        <f>SUM(D70:D72)</f>
-        <v>184.8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="20">
-      <c r="A77" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" s="19" customFormat="1">
-      <c r="A78" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B78" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C78" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D78" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E78" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="F78" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="G78" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H78" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I78" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
-      <c r="A79" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B79" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C79" s="1">
         <v>1</v>
       </c>
       <c r="D79" s="2">
         <f>C79*B79</f>
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9">
-      <c r="A80" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B80" s="2">
-        <v>15.99</v>
-      </c>
-      <c r="C80" s="1">
-        <v>6</v>
-      </c>
-      <c r="D80" s="2">
-        <f>C80*B80</f>
-        <v>95.94</v>
-      </c>
-      <c r="G80" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I80" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
-      <c r="A81" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B81" s="2">
-        <v>10</v>
-      </c>
-      <c r="C81" s="1">
-        <v>1</v>
-      </c>
-      <c r="D81" s="2">
-        <f>C81*B81</f>
-        <v>10</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H81" s="2" t="s">
+      <c r="H79" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
-      <c r="C83" s="10" t="s">
+    <row r="81" spans="1:10" s="19" customFormat="1">
+      <c r="A81" s="1"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D83" s="11">
-        <f>SUM(D79:D80)</f>
-        <v>145.94</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="20">
-      <c r="A85" s="5" t="s">
+      <c r="D81" s="11">
+        <f>SUM(D77:D79)</f>
+        <v>155.94</v>
+      </c>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+    </row>
+    <row r="83" spans="1:10" ht="20">
+      <c r="A83" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="1:9" s="19" customFormat="1">
-      <c r="A86" s="17" t="s">
+    <row r="84" spans="1:10">
+      <c r="A84" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B86" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C86" s="17" t="s">
+      <c r="B84" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D86" s="18" t="s">
+      <c r="D84" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E86" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="F86" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="G86" s="18" t="s">
+      <c r="E84" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F84" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="G84" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H86" s="18" t="s">
+      <c r="H84" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="I86" s="17" t="s">
+      <c r="I84" s="17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="J84" s="19"/>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85" s="2">
+        <v>4.41</v>
+      </c>
+      <c r="C85" s="1">
+        <v>200</v>
+      </c>
+      <c r="D85" s="2">
+        <f t="shared" ref="D85:D90" si="2">C85*B85</f>
+        <v>882</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B86" s="2">
+        <v>23</v>
+      </c>
+      <c r="C86" s="1">
+        <v>4</v>
+      </c>
+      <c r="D86" s="2">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B87" s="2">
-        <v>4.41</v>
+        <v>7.27</v>
       </c>
       <c r="C87" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="D87" s="2">
-        <f t="shared" ref="D87:D92" si="2">C87*B87</f>
-        <v>882</v>
+        <f t="shared" si="2"/>
+        <v>14.54</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88" s="1" t="s">
-        <v>24</v>
+        <v>103</v>
       </c>
       <c r="B88" s="2">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="C88" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D88" s="2">
         <f t="shared" si="2"/>
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>63</v>
+        <v>101</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" s="19" customFormat="1">
       <c r="A89" s="1" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="B89" s="2">
-        <v>7.27</v>
+        <v>7.5</v>
       </c>
       <c r="C89" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D89" s="2">
         <f t="shared" si="2"/>
-        <v>14.54</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
       <c r="G89" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="H89" s="2"/>
       <c r="I89" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9">
+        <v>90</v>
+      </c>
+      <c r="J89" s="1"/>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B90" s="2">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="C90" s="1">
         <v>1</v>
       </c>
       <c r="D90" s="2">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H90" s="2" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B91" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="C91" s="1">
+        <v>108</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B93" s="2">
+        <v>5.9</v>
+      </c>
+      <c r="C93" s="1">
+        <v>1</v>
+      </c>
+      <c r="D93" s="2">
+        <f>C93*B93</f>
+        <v>5.9</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="10"/>
+      <c r="C95" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D95" s="11">
+        <f>SUM(D85:D93)</f>
+        <v>1235.44</v>
+      </c>
+      <c r="I95" s="15"/>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="20"/>
+      <c r="B96" s="21"/>
+      <c r="C96" s="20"/>
+      <c r="D96" s="21"/>
+      <c r="E96" s="21"/>
+      <c r="F96" s="21"/>
+      <c r="G96" s="21"/>
+      <c r="H96" s="21"/>
+      <c r="I96" s="20"/>
+    </row>
+    <row r="97" spans="1:10" ht="20">
+      <c r="A97" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E98" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F98" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="G98" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H98" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="I98" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D91" s="2">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
-      <c r="A92" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B92" s="2">
-        <v>121</v>
-      </c>
-      <c r="C92" s="1">
-        <v>1</v>
-      </c>
-      <c r="D92" s="2">
-        <f t="shared" si="2"/>
-        <v>121</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9">
-      <c r="A93" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G93" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I93" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9">
-      <c r="A94" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G94" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I94" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9">
-      <c r="A95" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B95" s="2">
-        <v>5.9</v>
-      </c>
-      <c r="C95" s="1">
-        <v>1</v>
-      </c>
-      <c r="D95" s="2">
-        <f>C95*B95</f>
-        <v>5.9</v>
-      </c>
-      <c r="E95" s="2" t="s">
+      <c r="J98" s="19"/>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B99" s="2">
+        <v>0</v>
+      </c>
+      <c r="C99" s="1">
+        <v>1</v>
+      </c>
+      <c r="D99" s="2">
+        <v>0</v>
+      </c>
+      <c r="E99" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G95" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
-      <c r="A97" s="10"/>
-      <c r="C97" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D97" s="11">
-        <f>SUM(D87:D92)</f>
-        <v>1229.54</v>
-      </c>
-      <c r="I97" s="15"/>
-    </row>
-    <row r="98" spans="1:9">
-      <c r="A98" s="20"/>
-      <c r="B98" s="21"/>
-      <c r="C98" s="20"/>
-      <c r="D98" s="21"/>
-      <c r="E98" s="21"/>
-      <c r="F98" s="21"/>
-      <c r="G98" s="21"/>
-      <c r="H98" s="21"/>
-      <c r="I98" s="20"/>
-    </row>
-    <row r="99" spans="1:9" ht="20">
-      <c r="A99" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" s="19" customFormat="1">
-      <c r="A100" s="17" t="s">
+      <c r="F99" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B100" s="2">
         <v>0</v>
       </c>
-      <c r="B100" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C100" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D100" s="18" t="s">
+      <c r="C100" s="1">
+        <v>1</v>
+      </c>
+      <c r="D100" s="2">
+        <v>0</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J100" s="15"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B101" s="2">
+        <v>50</v>
+      </c>
+      <c r="C101" s="1">
         <v>3</v>
       </c>
-      <c r="E100" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="F100" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="G100" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H100" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I100" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9">
-      <c r="A101" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B101" s="2">
-        <v>0</v>
-      </c>
-      <c r="C101" s="1">
-        <v>1</v>
-      </c>
       <c r="D101" s="2">
-        <v>0</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>65</v>
+        <f>C101*B101</f>
+        <v>150</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" s="15" customFormat="1">
+        <v>77</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
       <c r="A102" s="1" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="B102" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C102" s="1">
         <v>1</v>
       </c>
       <c r="D102" s="2">
-        <v>0</v>
+        <f>C102*B102</f>
+        <v>9</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H102" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I102" s="1"/>
-    </row>
-    <row r="103" spans="1:9">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" s="19" customFormat="1">
       <c r="A103" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B103" s="2">
-        <v>50</v>
-      </c>
-      <c r="C103" s="1">
-        <v>3</v>
-      </c>
-      <c r="D103" s="2">
-        <f>C103*B103</f>
-        <v>150</v>
-      </c>
-      <c r="G103" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="B103" s="2"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
       <c r="H103" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I103" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9">
+        <v>126</v>
+      </c>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+    </row>
+    <row r="104" spans="1:10">
       <c r="A104" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B104" s="2">
-        <v>9</v>
-      </c>
-      <c r="C104" s="1">
-        <v>1</v>
-      </c>
-      <c r="D104" s="2">
-        <f>C104*B104</f>
-        <v>9</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9">
+        <v>125</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" s="15" customFormat="1">
+      <c r="A105" s="1"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+      <c r="H105" s="2"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+    </row>
+    <row r="106" spans="1:10">
       <c r="C106" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D106" s="11">
-        <f>SUM(D101:D103)</f>
-        <v>150</v>
+        <f>SUM(D99:D104)</f>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revised prices, shipping info
</commit_message>
<xml_diff>
--- a/DetailedBudget.xlsx
+++ b/DetailedBudget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="8140" yWindow="0" windowWidth="19840" windowHeight="16260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="125">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -117,12 +117,6 @@
     <t>http://ubld.it/products/truerng-hardware-random-number-generator/</t>
   </si>
   <si>
-    <t>DigitalTRNG</t>
-  </si>
-  <si>
-    <t>https://www.tindie.com/products/kidekin/trng/</t>
-  </si>
-  <si>
     <t>Type 1390-B Random Noise Generator</t>
   </si>
   <si>
@@ -201,9 +195,6 @@
     <t>Audio cables</t>
   </si>
   <si>
-    <t>Tindie</t>
-  </si>
-  <si>
     <t>UBLD</t>
   </si>
   <si>
@@ -222,15 +213,9 @@
     <t>Craigslist</t>
   </si>
   <si>
-    <t>Sublet for stay in Brighton</t>
-  </si>
-  <si>
     <t>Airbnb</t>
   </si>
   <si>
-    <t>Approx based on average in Brighton</t>
-  </si>
-  <si>
     <t>Local</t>
   </si>
   <si>
@@ -303,21 +288,9 @@
     <t>Dorado Packaging</t>
   </si>
   <si>
-    <t>…or cutting head parts</t>
-  </si>
-  <si>
-    <t>Surface transducer</t>
-  </si>
-  <si>
     <t>Needle</t>
   </si>
   <si>
-    <t>https://www.sparkfun.com/products/10975</t>
-  </si>
-  <si>
-    <t>Sparkfun</t>
-  </si>
-  <si>
     <t>Hagerman Audio Labs</t>
   </si>
   <si>
@@ -333,24 +306,6 @@
     <t>Tamper-resistant stickers (1800 labels)</t>
   </si>
   <si>
-    <t>McMaster</t>
-  </si>
-  <si>
-    <t>Small speakers</t>
-  </si>
-  <si>
-    <t>Digi-Key</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?lang=en&amp;site=us&amp;KeyWords=CMS0401KL-3X</t>
-  </si>
-  <si>
-    <t>0.002" acetate roll</t>
-  </si>
-  <si>
-    <t>http://www.mcmaster.com/#acetate/=y2f16l</t>
-  </si>
-  <si>
     <t>More acetate film</t>
   </si>
   <si>
@@ -387,27 +342,15 @@
     <t>ARRIVED?</t>
   </si>
   <si>
-    <t>Replacement feet for 1390-B</t>
-  </si>
-  <si>
-    <t>http://www.mcmaster.com/#9546k549/=y4zioh</t>
-  </si>
-  <si>
     <t>Power strips</t>
   </si>
   <si>
     <t>Extension cords</t>
   </si>
   <si>
-    <t>Buy in UK or borrow?</t>
-  </si>
-  <si>
     <t>Serial # 3641</t>
   </si>
   <si>
-    <t>Aluminum L-extrusion</t>
-  </si>
-  <si>
     <t>Wire nuts</t>
   </si>
   <si>
@@ -415,6 +358,42 @@
   </si>
   <si>
     <t>Spade terminal</t>
+  </si>
+  <si>
+    <t>Air pump (as vacuum)</t>
+  </si>
+  <si>
+    <t>Jar/tupperware for swarf</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Tetra-77854-Whisper-Pump-Gallon/dp/B0009YJ4NG/ref=zg_bs_2975471011_3</t>
+  </si>
+  <si>
+    <t>Wire transfer fee</t>
+  </si>
+  <si>
+    <t>Chipboard jackets</t>
+  </si>
+  <si>
+    <t>http://doradopkg.com/Record-Jackets/Blank-Record-Jackets/7-Blank-Jacket.html</t>
+  </si>
+  <si>
+    <t>Bank of America</t>
+  </si>
+  <si>
+    <t>Use US-style, plug into adapter</t>
+  </si>
+  <si>
+    <t>Airbnb in Brighton</t>
+  </si>
+  <si>
+    <t>REQUESTED</t>
+  </si>
+  <si>
+    <t>Bring from home</t>
+  </si>
+  <si>
+    <t>Virgin Atlantic</t>
   </si>
 </sst>
 </file>
@@ -515,9 +494,51 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="142">
+  <cellStyleXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -689,7 +710,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="142">
+  <cellStyles count="184">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -761,6 +782,27 @@
     <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -831,6 +873,27 @@
     <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1160,10 +1223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1187,7 +1250,7 @@
     </row>
     <row r="2" spans="1:9" ht="20">
       <c r="E2" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F2" s="4"/>
     </row>
@@ -1198,15 +1261,15 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6">
-        <f>D18+D27+D36+D46+D64+D73+D81+D95+D106</f>
-        <v>11576.339999999998</v>
+        <f>D19+D28+D37+D47+D65+D72+D80+D94+D105</f>
+        <v>12070.279999999999</v>
       </c>
       <c r="E3" s="7">
         <v>0.64</v>
       </c>
       <c r="F3" s="8">
         <f>D3*E3</f>
-        <v>7408.8575999999994</v>
+        <v>7724.9791999999998</v>
       </c>
       <c r="H3" s="9"/>
     </row>
@@ -1236,14 +1299,14 @@
       <c r="C5" s="5"/>
       <c r="D5" s="6">
         <f>D4-D3</f>
-        <v>923.66000000000167</v>
+        <v>429.72000000000116</v>
       </c>
       <c r="E5" s="7">
         <v>0.64</v>
       </c>
       <c r="F5" s="8">
         <f>D5*E5</f>
-        <v>591.14240000000109</v>
+        <v>275.02080000000075</v>
       </c>
       <c r="H5" s="9"/>
     </row>
@@ -1279,7 +1342,7 @@
     </row>
     <row r="9" spans="1:9" ht="20">
       <c r="A9" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="19" customFormat="1">
@@ -1296,16 +1359,16 @@
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>4</v>
@@ -1313,7 +1376,7 @@
     </row>
     <row r="11" spans="1:9" s="15" customFormat="1">
       <c r="A11" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="2">
         <v>850</v>
@@ -1322,18 +1385,24 @@
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" ref="D11:D16" si="0">C11*B11</f>
+        <f t="shared" ref="D11:D17" si="0">C11*B11</f>
         <v>850</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2">
         <v>100</v>
@@ -1348,7 +1417,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2">
         <v>600</v>
@@ -1363,7 +1432,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B14" s="2">
         <v>600</v>
@@ -1378,28 +1447,28 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="15" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="B15" s="2">
-        <v>2000</v>
+        <v>2025</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>2025</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16" s="2">
         <v>3000</v>
@@ -1412,102 +1481,106 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="C18" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="11">
-        <f>SUM(D11:D16)</f>
-        <v>7150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="20">
-      <c r="A20" s="5" t="s">
+    <row r="17" spans="1:9">
+      <c r="A17" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="2">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="C19" s="10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" s="19" customFormat="1">
-      <c r="A21" s="17" t="s">
+      <c r="D19" s="11">
+        <f>SUM(D11:D17)</f>
+        <v>7190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="20">
+      <c r="A21" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="19" customFormat="1">
+      <c r="A22" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="17" t="s">
+      <c r="B22" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D22" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I21" s="17" t="s">
+      <c r="E22" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" s="17" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="2">
-        <v>310</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2</v>
-      </c>
-      <c r="D22" s="2">
-        <f>C22+B22</f>
-        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B23" s="2">
-        <v>200</v>
+        <v>310</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="2">
-        <f>C23+B23</f>
-        <v>201</v>
+        <f>C23*B23</f>
+        <v>620</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B24" s="2">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="2">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>43</v>
+        <f>C24+B24</f>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
@@ -1519,521 +1592,494 @@
         <v>0</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="C27" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="11">
-        <f>SUM(D22:D25)</f>
-        <v>513</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="20">
-      <c r="A29" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="C28" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="11">
+        <f>SUM(D23:D26)</f>
+        <v>821</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="20">
+      <c r="A30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="10"/>
-    </row>
-    <row r="30" spans="1:9" s="19" customFormat="1">
-      <c r="A30" s="17" t="s">
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="10"/>
+    </row>
+    <row r="31" spans="1:9" s="19" customFormat="1">
+      <c r="A31" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="17" t="s">
+      <c r="B31" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D31" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F30" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="G30" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H30" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I30" s="17" t="s">
+      <c r="E31" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" s="17" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="2">
-        <v>12.9</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2">
-        <f>C31*B31</f>
-        <v>12.9</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
-        <v>117</v>
+        <v>5</v>
       </c>
       <c r="B32" s="2">
-        <v>0.48</v>
+        <v>12.9</v>
       </c>
       <c r="C32" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D32" s="2">
         <f>C32*B32</f>
-        <v>2.88</v>
+        <v>12.9</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>118</v>
+        <v>61</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="C33" s="1">
         <v>6</v>
       </c>
       <c r="D33" s="2">
         <f>C33*B33</f>
-        <v>0</v>
+        <v>2.88</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="2">
-        <v>30</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D34" s="2">
         <f>C34*B34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="2">
         <v>30</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I34" s="1" t="s">
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2">
+        <f>C35*B35</f>
+        <v>30</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
-      <c r="C36" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="11">
-        <f>SUM(D31:D34)</f>
+    <row r="37" spans="1:9">
+      <c r="C37" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="11">
+        <f>SUM(D32:D35)</f>
         <v>45.78</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="20">
-      <c r="A38" s="5" t="s">
+    <row r="39" spans="1:9" ht="20">
+      <c r="A39" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="19" customFormat="1">
-      <c r="A39" s="17" t="s">
+    <row r="40" spans="1:9" s="19" customFormat="1">
+      <c r="A40" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="17" t="s">
+      <c r="B40" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D40" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="G39" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H39" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I39" s="17" t="s">
+      <c r="E40" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I40" s="17" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="2">
-        <v>40</v>
-      </c>
-      <c r="C40" s="1">
-        <v>10</v>
-      </c>
-      <c r="D40" s="2">
-        <f>C40*B40</f>
-        <v>400</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" s="2">
+        <v>40</v>
+      </c>
+      <c r="C41" s="1">
         <v>10</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1</v>
       </c>
       <c r="D41" s="2">
         <f>C41*B41</f>
-        <v>10</v>
+        <v>400</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B42" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C42" s="1">
         <v>1</v>
       </c>
       <c r="D42" s="2">
         <f>C42*B42</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="B43" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
       </c>
       <c r="D43" s="2">
-        <v>0</v>
+        <f>C43*B43</f>
+        <v>15</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="B44" s="2">
+        <v>0</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="2">
         <v>40</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C45" s="1">
         <v>2</v>
       </c>
-      <c r="D44" s="2">
-        <f>C44*B44</f>
+      <c r="D45" s="2">
+        <f>C45*B45</f>
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
-      <c r="C46" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D46" s="11">
-        <f>SUM(D40:D44)</f>
+    <row r="47" spans="1:9">
+      <c r="C47" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" s="11">
+        <f>SUM(D41:D45)</f>
         <v>505</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="20">
-      <c r="A48" s="5" t="s">
+    <row r="49" spans="1:9" ht="20">
+      <c r="A49" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="19" customFormat="1">
-      <c r="A49" s="17" t="s">
+    <row r="50" spans="1:9" s="19" customFormat="1">
+      <c r="A50" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="17" t="s">
+      <c r="B50" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="D50" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E49" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F49" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="G49" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H49" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I49" s="17" t="s">
+      <c r="E50" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G50" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I50" s="17" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" s="2">
-        <v>1500</v>
-      </c>
-      <c r="C50" s="1">
-        <v>1</v>
-      </c>
-      <c r="D50" s="2">
-        <f t="shared" ref="D50:D62" si="1">C50*B50</f>
-        <v>1500</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="B51" s="2">
+        <v>1500</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="2">
+        <f t="shared" ref="D51:D63" si="1">C51*B51</f>
+        <v>1500</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>94</v>
+        <v>45</v>
+      </c>
+      <c r="B52" s="2">
+        <v>280</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" si="1"/>
+        <v>280</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="B53" s="2">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C53" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D53" s="2">
-        <f>C53*B53</f>
-        <v>40</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>51</v>
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B54" s="2">
-        <v>12.62</v>
-      </c>
-      <c r="C54" s="1">
-        <v>2</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B55" s="2">
-        <v>15.99</v>
-      </c>
-      <c r="C55" s="1">
-        <v>1</v>
-      </c>
-      <c r="D55" s="2">
-        <f>C55*B55</f>
-        <v>15.99</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B56" s="2">
-        <v>3.49</v>
-      </c>
-      <c r="C56" s="1">
-        <v>1</v>
-      </c>
-      <c r="D56" s="2">
-        <f>C56*B56</f>
-        <v>3.49</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>130</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="B57" s="2">
-        <v>2.99</v>
+        <v>3.49</v>
       </c>
       <c r="C57" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D57" s="2">
         <f>C57*B57</f>
-        <v>5.98</v>
+        <v>3.49</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>96</v>
+        <v>112</v>
+      </c>
+      <c r="B58" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="C58" s="1">
+        <v>2</v>
+      </c>
+      <c r="D58" s="2">
+        <f>C58*B58</f>
+        <v>5.98</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B59" s="2">
-        <v>269</v>
-      </c>
-      <c r="C59" s="1">
-        <v>1</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="B60" s="2">
-        <v>0</v>
+        <v>269</v>
       </c>
       <c r="C60" s="1">
         <v>1</v>
       </c>
-      <c r="D60" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="G60" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>75</v>
+        <v>61</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B61" s="2">
         <v>0</v>
@@ -2045,126 +2091,135 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="E61" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="G61" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B62" s="2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C62" s="1">
         <v>1</v>
       </c>
       <c r="D62" s="2">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B63" s="2">
         <v>50</v>
       </c>
-      <c r="E62" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="C64" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D64" s="11">
-        <f>SUM(D50:D62)</f>
-        <v>1615.46</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="20">
-      <c r="A66" s="5" t="s">
+      <c r="C63" s="1">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="C65" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D65" s="11">
+        <f>SUM(D51:D63)</f>
+        <v>1852.47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="20">
+      <c r="A67" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
-      <c r="A67" s="17" t="s">
+    <row r="68" spans="1:10">
+      <c r="A68" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B67" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="17" t="s">
+      <c r="B68" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D67" s="18" t="s">
+      <c r="D68" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E67" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F67" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="G67" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H67" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I67" s="17" t="s">
+      <c r="E68" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F68" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G68" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H68" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I68" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J67" s="19"/>
-    </row>
-    <row r="68" spans="1:10">
-      <c r="A68" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" s="2">
-        <v>56.8</v>
-      </c>
-      <c r="C68" s="1">
-        <v>1</v>
-      </c>
-      <c r="D68" s="2">
-        <f>C68*B68</f>
-        <v>56.8</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="J68" s="19"/>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B69" s="2">
-        <v>79</v>
+        <v>56.75</v>
       </c>
       <c r="C69" s="1">
         <v>1</v>
       </c>
       <c r="D69" s="2">
         <f>C69*B69</f>
-        <v>79</v>
+        <v>56.75</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B70" s="2">
         <v>49</v>
@@ -2177,446 +2232,467 @@
         <v>49</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
-      <c r="A71" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B71" s="2">
-        <v>5.96</v>
-      </c>
-      <c r="C71" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" s="19" customFormat="1">
+      <c r="A71" s="1"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="C72" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D72" s="11">
+        <f>SUM(D69:D70)</f>
+        <v>105.75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="20">
+      <c r="A74" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D71" s="2">
-        <f>C71*B71</f>
-        <v>11.92</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" s="19" customFormat="1">
-      <c r="A72" s="1"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="C73" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D73" s="11">
-        <f>SUM(D68:D71)</f>
-        <v>196.72</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="20">
-      <c r="A75" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="D75" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E75" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F75" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G75" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H75" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I75" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J75" s="19"/>
     </row>
     <row r="76" spans="1:10">
-      <c r="A76" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B76" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C76" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D76" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E76" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F76" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="G76" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H76" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I76" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J76" s="19"/>
+      <c r="A76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" s="2">
+        <v>50</v>
+      </c>
+      <c r="C76" s="1">
+        <v>1</v>
+      </c>
+      <c r="D76" s="2">
+        <f>C76*B76</f>
+        <v>50</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="1" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="B77" s="2">
-        <v>50</v>
+        <v>15.99</v>
       </c>
       <c r="C77" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D77" s="2">
         <f>C77*B77</f>
-        <v>50</v>
+        <v>95.94</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B78" s="2">
-        <v>15.99</v>
+        <v>10</v>
       </c>
       <c r="C78" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D78" s="2">
         <f>C78*B78</f>
-        <v>95.94</v>
+        <v>10</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10">
-      <c r="A79" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B79" s="2">
-        <v>10</v>
-      </c>
-      <c r="C79" s="1">
-        <v>1</v>
-      </c>
-      <c r="D79" s="2">
-        <f>C79*B79</f>
-        <v>10</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" s="19" customFormat="1">
-      <c r="A81" s="1"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D81" s="11">
-        <f>SUM(D77:D79)</f>
+        <v>76</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="19" customFormat="1">
+      <c r="A80" s="1"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D80" s="11">
+        <f>SUM(D76:D78)</f>
         <v>155.94</v>
       </c>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-    </row>
-    <row r="83" spans="1:10" ht="20">
-      <c r="A83" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+    </row>
+    <row r="82" spans="1:10" ht="20">
+      <c r="A82" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E83" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F83" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G83" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H83" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I83" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J83" s="19"/>
     </row>
     <row r="84" spans="1:10">
-      <c r="A84" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B84" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C84" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D84" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E84" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F84" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="G84" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H84" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I84" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J84" s="19"/>
+      <c r="A84" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" s="2">
+        <v>4.41</v>
+      </c>
+      <c r="C84" s="1">
+        <v>200</v>
+      </c>
+      <c r="D84" s="2">
+        <f t="shared" ref="D84:D89" si="2">C84*B84</f>
+        <v>882</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B85" s="2">
-        <v>4.41</v>
+        <v>23</v>
       </c>
       <c r="C85" s="1">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="D85" s="2">
-        <f t="shared" ref="D85:D90" si="2">C85*B85</f>
-        <v>882</v>
+        <f t="shared" si="2"/>
+        <v>92</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B86" s="2">
-        <v>23</v>
+        <v>7.27</v>
       </c>
       <c r="C86" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D86" s="2">
         <f t="shared" si="2"/>
-        <v>92</v>
+        <v>14.54</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="1" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="B87" s="2">
-        <v>7.27</v>
+        <v>89.9</v>
       </c>
       <c r="C87" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D87" s="2">
         <f t="shared" si="2"/>
-        <v>14.54</v>
+        <v>89.9</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>64</v>
+        <v>92</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" s="19" customFormat="1">
       <c r="A88" s="1" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="B88" s="2">
-        <v>90</v>
+        <v>7.5</v>
       </c>
       <c r="C88" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D88" s="2">
         <f t="shared" si="2"/>
-        <v>90</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
       <c r="G88" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H88" s="2" t="s">
-        <v>113</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="H88" s="2"/>
       <c r="I88" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" s="19" customFormat="1">
+        <v>85</v>
+      </c>
+      <c r="J88" s="1"/>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B89" s="2">
-        <v>7.5</v>
+        <v>121</v>
       </c>
       <c r="C89" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D89" s="2">
         <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
+        <v>121</v>
+      </c>
       <c r="G89" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H89" s="2"/>
+        <v>88</v>
+      </c>
       <c r="I89" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J89" s="1"/>
+        <v>87</v>
+      </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B90" s="2">
-        <v>121</v>
-      </c>
-      <c r="C90" s="1">
-        <v>1</v>
-      </c>
-      <c r="D90" s="2">
-        <f t="shared" si="2"/>
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
+      </c>
+      <c r="B91" s="2">
+        <v>5.9</v>
+      </c>
+      <c r="C91" s="1">
+        <v>1</v>
+      </c>
+      <c r="D91" s="2">
+        <f>C91*B91</f>
+        <v>5.9</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
+      </c>
+      <c r="B92" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="C92" s="1">
+        <v>200</v>
+      </c>
+      <c r="D92" s="2">
+        <f>C92*B92</f>
+        <v>94</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10">
-      <c r="A93" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B93" s="2">
-        <v>5.9</v>
-      </c>
-      <c r="C93" s="1">
-        <v>1</v>
-      </c>
-      <c r="D93" s="2">
-        <f>C93*B93</f>
-        <v>5.9</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G93" s="2" t="s">
         <v>118</v>
       </c>
     </row>
+    <row r="94" spans="1:10">
+      <c r="A94" s="10"/>
+      <c r="C94" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D94" s="11">
+        <f>SUM(D84:D91)</f>
+        <v>1235.3400000000001</v>
+      </c>
+      <c r="I94" s="15"/>
+    </row>
     <row r="95" spans="1:10">
-      <c r="A95" s="10"/>
-      <c r="C95" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D95" s="11">
-        <f>SUM(D85:D93)</f>
-        <v>1235.44</v>
-      </c>
-      <c r="I95" s="15"/>
-    </row>
-    <row r="96" spans="1:10">
-      <c r="A96" s="20"/>
-      <c r="B96" s="21"/>
-      <c r="C96" s="20"/>
-      <c r="D96" s="21"/>
-      <c r="E96" s="21"/>
-      <c r="F96" s="21"/>
-      <c r="G96" s="21"/>
-      <c r="H96" s="21"/>
-      <c r="I96" s="20"/>
-    </row>
-    <row r="97" spans="1:10" ht="20">
-      <c r="A97" s="5" t="s">
-        <v>85</v>
-      </c>
+      <c r="A95" s="20"/>
+      <c r="B95" s="21"/>
+      <c r="C95" s="20"/>
+      <c r="D95" s="21"/>
+      <c r="E95" s="21"/>
+      <c r="F95" s="21"/>
+      <c r="G95" s="21"/>
+      <c r="H95" s="21"/>
+      <c r="I95" s="20"/>
+    </row>
+    <row r="96" spans="1:10" ht="20">
+      <c r="A96" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D97" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E97" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F97" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G97" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H97" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I97" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J97" s="19"/>
     </row>
     <row r="98" spans="1:10">
-      <c r="A98" s="17" t="s">
+      <c r="A98" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B98" s="2">
         <v>0</v>
       </c>
-      <c r="B98" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C98" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D98" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E98" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F98" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="G98" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H98" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I98" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J98" s="19"/>
+      <c r="C98" s="1">
+        <v>1</v>
+      </c>
+      <c r="D98" s="2">
+        <v>0</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B99" s="2">
         <v>0</v>
@@ -2628,135 +2704,134 @@
         <v>0</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>75</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="J99" s="15"/>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B100" s="2">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C100" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D100" s="2">
-        <v>0</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>65</v>
+        <f>C100*B100</f>
+        <v>150</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="J100" s="15"/>
+        <v>72</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B101" s="2">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="C101" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D101" s="2">
         <f>C101*B101</f>
-        <v>150</v>
+        <v>9</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H101" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I101" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" s="19" customFormat="1">
       <c r="A102" s="1" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="B102" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C102" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D102" s="2">
-        <f>C102*B102</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F102" s="2"/>
       <c r="G102" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" s="19" customFormat="1">
+        <v>123</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+    </row>
+    <row r="103" spans="1:10">
       <c r="A103" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B103" s="2"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-      <c r="G103" s="2"/>
+        <v>108</v>
+      </c>
+      <c r="B103" s="2">
+        <v>0</v>
+      </c>
+      <c r="C103" s="1">
+        <v>2</v>
+      </c>
+      <c r="D103" s="2">
+        <v>0</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="H103" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I103" s="1"/>
-      <c r="J103" s="1"/>
-    </row>
-    <row r="104" spans="1:10">
-      <c r="A104" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H104" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" s="15" customFormat="1">
-      <c r="A105" s="1"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="2"/>
-      <c r="E105" s="2"/>
-      <c r="F105" s="2"/>
-      <c r="G105" s="2"/>
-      <c r="H105" s="2"/>
-      <c r="I105" s="1"/>
-      <c r="J105" s="1"/>
-    </row>
-    <row r="106" spans="1:10">
-      <c r="C106" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D106" s="11">
-        <f>SUM(D99:D104)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" s="15" customFormat="1">
+      <c r="A104" s="1"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="C105" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D105" s="11">
+        <f>SUM(D98:D103)</f>
         <v>159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Arrived parts, actual rent, etc
</commit_message>
<xml_diff>
--- a/DetailedBudget.xlsx
+++ b/DetailedBudget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8140" yWindow="0" windowWidth="19840" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="131">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -93,12 +93,6 @@
     <t>REMAINING</t>
   </si>
   <si>
-    <t>Chipboard jackets (pack of 50)</t>
-  </si>
-  <si>
-    <t>http://www.stumptownprinters.com/store/c-sp-blanks:-blank-disc-packaging-24/#7-jacket-%28chipboard%29-for-vinyl</t>
-  </si>
-  <si>
     <t>http://recordcuttingblanks.com/7-INCH-RECORD-BLANKS.html</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>STOREFRONT</t>
   </si>
   <si>
-    <t>Utilities</t>
-  </si>
-  <si>
     <t>SUBTOTAL</t>
   </si>
   <si>
@@ -162,9 +153,6 @@
     <t>Inverse RIAA filter</t>
   </si>
   <si>
-    <t>Weekly rent</t>
-  </si>
-  <si>
     <t>Vinyl lettering for door/window of shop</t>
   </si>
   <si>
@@ -201,9 +189,6 @@
     <t>Record Cutting Blanks</t>
   </si>
   <si>
-    <t>Stumptown Printers</t>
-  </si>
-  <si>
     <t>Amazon</t>
   </si>
   <si>
@@ -234,15 +219,9 @@
     <t>Already own</t>
   </si>
   <si>
-    <t>Power adapter for 22V</t>
-  </si>
-  <si>
     <t>For lathe, 1390 generator, amplifier</t>
   </si>
   <si>
-    <t>http://www.amazon.com/dp/B00CLY1WPU?psc=1</t>
-  </si>
-  <si>
     <t>Roll surcharge for copper mesh</t>
   </si>
   <si>
@@ -273,24 +252,9 @@
     <t>Stools</t>
   </si>
   <si>
-    <t>Clear re-sealable bags</t>
-  </si>
-  <si>
-    <t>http://www.stumptownprinters.com/store/c-clear-poly-sleeves-122/</t>
-  </si>
-  <si>
-    <t>Record labels (minimum order of 500x)</t>
-  </si>
-  <si>
-    <t>http://doradopkg.com/Center-Labels/10-or-7-Center-Label-Single-Set.html</t>
-  </si>
-  <si>
     <t>Dorado Packaging</t>
   </si>
   <si>
-    <t>Needle</t>
-  </si>
-  <si>
     <t>Hagerman Audio Labs</t>
   </si>
   <si>
@@ -387,13 +351,67 @@
     <t>Airbnb in Brighton</t>
   </si>
   <si>
-    <t>REQUESTED</t>
-  </si>
-  <si>
     <t>Bring from home</t>
   </si>
   <si>
     <t>Virgin Atlantic</t>
+  </si>
+  <si>
+    <t>Fuse and holder</t>
+  </si>
+  <si>
+    <t>Extra needles</t>
+  </si>
+  <si>
+    <t>Power adapter for 220V</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/gp/product/B0022QOSDK?refRID=5V9CW20R4Y973CTXF9TH&amp;ref_=pd_rhf_eetyp_p_img_1</t>
+  </si>
+  <si>
+    <t>PARTIAL</t>
+  </si>
+  <si>
+    <t>Tube fittings</t>
+  </si>
+  <si>
+    <t>2 elbows for jar</t>
+  </si>
+  <si>
+    <t>Clear re-sealable bags (pack of 100)</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/gp/product/B003XX91V0?redirect=true&amp;ref_=pd_hud_ysc_orders</t>
+  </si>
+  <si>
+    <t>Tubing/joints for structure</t>
+  </si>
+  <si>
+    <t>Center labels (pack of 100 sheets = 400 labels)</t>
+  </si>
+  <si>
+    <t>http://www.onlinelabels.com/OL7425.htm?src=dlc-21</t>
+  </si>
+  <si>
+    <t>Circle cutter</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Olfa-1057028-Rotary-Circle-Cutter/dp/B001CEAMCY#Ask</t>
+  </si>
+  <si>
+    <t>Extra blades (2x)</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/9463-RB18-2-Rotary-Blades-2-Pack/dp/B000BNXUFI/ref=sr_1_1?s=hi&amp;ie=UTF8&amp;qid=1438977088&amp;sr=1-1&amp;keywords=olfa+18mm+rotary+blade</t>
+  </si>
+  <si>
+    <t>Food + drink at receptions</t>
+  </si>
+  <si>
+    <t>Daily rent with utilities</t>
+  </si>
+  <si>
+    <t>Travel expenses/fee for musicians</t>
   </si>
 </sst>
 </file>
@@ -477,12 +495,18 @@
       <name val="Open Sans"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -494,7 +518,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="184">
+  <cellStyleXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -679,8 +703,46 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -709,8 +771,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="184">
+  <cellStyles count="222">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -803,6 +867,25 @@
     <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -894,6 +977,25 @@
     <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1223,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J105"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1250,7 +1352,7 @@
     </row>
     <row r="2" spans="1:9" ht="20">
       <c r="E2" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F2" s="4"/>
     </row>
@@ -1261,15 +1363,15 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6">
-        <f>D19+D28+D37+D47+D65+D72+D80+D94+D105</f>
-        <v>12070.279999999999</v>
+        <f>D19+D29+D38+D48+D67+D74+D82+D98+D109</f>
+        <v>11741.19</v>
       </c>
       <c r="E3" s="7">
         <v>0.64</v>
       </c>
       <c r="F3" s="8">
         <f>D3*E3</f>
-        <v>7724.9791999999998</v>
+        <v>7514.3616000000002</v>
       </c>
       <c r="H3" s="9"/>
     </row>
@@ -1299,14 +1401,14 @@
       <c r="C5" s="5"/>
       <c r="D5" s="6">
         <f>D4-D3</f>
-        <v>429.72000000000116</v>
+        <v>758.80999999999949</v>
       </c>
       <c r="E5" s="7">
         <v>0.64</v>
       </c>
       <c r="F5" s="8">
         <f>D5*E5</f>
-        <v>275.02080000000075</v>
+        <v>485.63839999999971</v>
       </c>
       <c r="H5" s="9"/>
     </row>
@@ -1342,7 +1444,7 @@
     </row>
     <row r="9" spans="1:9" ht="20">
       <c r="A9" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="19" customFormat="1">
@@ -1359,16 +1461,16 @@
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>4</v>
@@ -1376,7 +1478,7 @@
     </row>
     <row r="11" spans="1:9" s="15" customFormat="1">
       <c r="A11" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2">
         <v>850</v>
@@ -1389,20 +1491,20 @@
         <v>850</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" s="2">
         <v>100</v>
@@ -1417,7 +1519,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B13" s="2">
         <v>600</v>
@@ -1432,7 +1534,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B14" s="2">
         <v>600</v>
@@ -1447,7 +1549,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="15" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B15" s="2">
         <v>2025</v>
@@ -1460,15 +1562,18 @@
         <v>2025</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>122</v>
+        <v>45</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2">
         <v>3000</v>
@@ -1483,7 +1588,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="15" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B17" s="2">
         <v>15</v>
@@ -1496,18 +1601,18 @@
         <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="C19" s="10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D19" s="11">
         <f>SUM(D11:D17)</f>
@@ -1516,7 +1621,7 @@
     </row>
     <row r="21" spans="1:9" ht="20">
       <c r="A21" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="19" customFormat="1">
@@ -1533,16 +1638,16 @@
         <v>3</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I22" s="17" t="s">
         <v>4</v>
@@ -1550,57 +1655,53 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>47</v>
+        <v>129</v>
       </c>
       <c r="B23" s="2">
-        <v>310</v>
+        <v>48</v>
       </c>
       <c r="C23" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D23" s="2">
         <f>C23*B23</f>
-        <v>620</v>
+        <v>672</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B24" s="2">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="2">
-        <f>C24+B24</f>
-        <v>201</v>
+        <v>0</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="2">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>41</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B26" s="2">
         <v>0</v>
@@ -1612,423 +1713,474 @@
         <v>0</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="C28" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="11">
-        <f>SUM(D23:D26)</f>
-        <v>821</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="20">
-      <c r="A30" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="C29" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="11">
+        <f>SUM(D23:D27)</f>
+        <v>672</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="20">
+      <c r="A31" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="10"/>
-    </row>
-    <row r="31" spans="1:9" s="19" customFormat="1">
-      <c r="A31" s="17" t="s">
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="10"/>
+    </row>
+    <row r="32" spans="1:9" s="19" customFormat="1">
+      <c r="A32" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="17" t="s">
+      <c r="B32" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D32" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="G31" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="H31" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I31" s="17" t="s">
+      <c r="E32" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="17" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="2">
-        <v>12.9</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2">
-        <f>C32*B32</f>
-        <v>12.9</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
       <c r="B33" s="2">
-        <v>0.48</v>
+        <v>12.9</v>
       </c>
       <c r="C33" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D33" s="2">
         <f>C33*B33</f>
-        <v>2.88</v>
+        <v>12.9</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>103</v>
+        <v>56</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="C34" s="1">
         <v>6</v>
       </c>
       <c r="D34" s="2">
         <f>C34*B34</f>
+        <v>2.88</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="22" customFormat="1">
+      <c r="A35" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="23"/>
+      <c r="D35" s="23">
+        <f>C35*B35</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="1" t="s">
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B36" s="2">
         <v>30</v>
       </c>
-      <c r="C35" s="1">
-        <v>1</v>
-      </c>
-      <c r="D35" s="2">
-        <f>C35*B35</f>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2">
+        <f>C36*B36</f>
         <v>30</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I35" s="1" t="s">
+      <c r="E36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
-      <c r="C37" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" s="11">
-        <f>SUM(D32:D35)</f>
+    <row r="38" spans="1:9">
+      <c r="C38" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="11">
+        <f>SUM(D33:D36)</f>
         <v>45.78</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="20">
-      <c r="A39" s="5" t="s">
+    <row r="40" spans="1:9" ht="20">
+      <c r="A40" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="19" customFormat="1">
-      <c r="A40" s="17" t="s">
+    <row r="41" spans="1:9" s="19" customFormat="1">
+      <c r="A41" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="17" t="s">
+      <c r="B41" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="D41" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E40" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F40" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="G40" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="H40" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I40" s="17" t="s">
+      <c r="E41" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I41" s="17" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="2">
-        <v>40</v>
-      </c>
-      <c r="C41" s="1">
-        <v>10</v>
-      </c>
-      <c r="D41" s="2">
-        <f>C41*B41</f>
-        <v>400</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42" s="2">
+        <v>40</v>
+      </c>
+      <c r="C42" s="1">
         <v>10</v>
-      </c>
-      <c r="C42" s="1">
-        <v>1</v>
       </c>
       <c r="D42" s="2">
         <f>C42*B42</f>
-        <v>10</v>
+        <v>400</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B43" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
       </c>
       <c r="D43" s="2">
         <f>C43*B43</f>
+        <v>10</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="22" customFormat="1">
+      <c r="A44" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="23">
         <v>15</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B44" s="2">
-        <v>0</v>
-      </c>
-      <c r="C44" s="1">
-        <v>1</v>
-      </c>
-      <c r="D44" s="2">
-        <v>0</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="C44" s="22">
+        <v>1</v>
+      </c>
+      <c r="D44" s="23">
+        <f>C44*B44</f>
+        <v>15</v>
+      </c>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H44" s="23"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="B45" s="2">
+        <v>0</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="22" customFormat="1">
+      <c r="A46" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" s="23">
         <v>40</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C46" s="22">
         <v>2</v>
       </c>
-      <c r="D45" s="2">
-        <f>C45*B45</f>
+      <c r="D46" s="23">
+        <f>C46*B46</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="C47" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D47" s="11">
-        <f>SUM(D41:D45)</f>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="C48" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" s="11">
+        <f>SUM(D42:D46)</f>
         <v>505</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="20">
-      <c r="A49" s="5" t="s">
+    <row r="50" spans="1:9" ht="20">
+      <c r="A50" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="19" customFormat="1">
-      <c r="A50" s="17" t="s">
+    <row r="51" spans="1:9" s="19" customFormat="1">
+      <c r="A51" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="17" t="s">
+      <c r="B51" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D50" s="18" t="s">
+      <c r="D51" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E50" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F50" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="G50" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="H50" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I50" s="17" t="s">
+      <c r="E51" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H51" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I51" s="17" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B51" s="2">
-        <v>1500</v>
-      </c>
-      <c r="C51" s="1">
-        <v>1</v>
-      </c>
-      <c r="D51" s="2">
-        <f t="shared" ref="D51:D63" si="1">C51*B51</f>
-        <v>1500</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B52" s="2">
+        <v>1500</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" ref="D52:D65" si="1">C52*B52</f>
+        <v>1500</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="2">
         <v>280</v>
       </c>
-      <c r="C52" s="1">
-        <v>1</v>
-      </c>
-      <c r="D52" s="2">
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
+      <c r="D53" s="2">
         <f t="shared" si="1"/>
         <v>280</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B53" s="2">
+      <c r="E53" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54" s="2">
         <v>13</v>
       </c>
-      <c r="C53" s="1">
-        <v>1</v>
-      </c>
-      <c r="D53" s="2">
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+      <c r="D54" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="G53" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="1" t="s">
+      <c r="E54" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="22" customFormat="1">
+      <c r="A55" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="23"/>
+      <c r="H55" s="23"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="B56" s="2">
+        <v>6.24</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2">
+        <f>C56*B56</f>
+        <v>6.24</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B57" s="2">
-        <v>3.49</v>
+        <v>2.36</v>
       </c>
       <c r="C57" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D57" s="2">
         <f>C57*B57</f>
-        <v>3.49</v>
+        <v>4.72</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2036,28 +2188,48 @@
         <v>112</v>
       </c>
       <c r="B58" s="2">
-        <v>2.99</v>
+        <f>1.94+2.29</f>
+        <v>4.2300000000000004</v>
       </c>
       <c r="C58" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D58" s="2">
         <f>C58*B58</f>
-        <v>5.98</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
+      </c>
+      <c r="B59" s="2">
+        <v>3.49</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1</v>
+      </c>
+      <c r="D59" s="2">
+        <f>C59*B59</f>
+        <v>3.49</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2065,774 +2237,877 @@
         <v>100</v>
       </c>
       <c r="B60" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="C60" s="1">
+        <v>2</v>
+      </c>
+      <c r="D60" s="2">
+        <f>C60*B60</f>
+        <v>5.98</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="22" customFormat="1">
+      <c r="A61" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+    </row>
+    <row r="62" spans="1:9" s="22" customFormat="1">
+      <c r="A62" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B62" s="23">
         <v>269</v>
       </c>
-      <c r="C60" s="1">
-        <v>1</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B61" s="2">
+      <c r="C62" s="22">
+        <v>1</v>
+      </c>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="H62" s="23"/>
+      <c r="I62" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" s="2">
         <v>0</v>
       </c>
-      <c r="C61" s="1">
-        <v>1</v>
-      </c>
-      <c r="D61" s="2">
+      <c r="C63" s="1">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B62" s="2">
+      <c r="E63" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="22" customFormat="1">
+      <c r="A64" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64" s="23">
         <v>0</v>
       </c>
-      <c r="C62" s="1">
-        <v>1</v>
-      </c>
-      <c r="D62" s="2">
+      <c r="C64" s="22">
+        <v>1</v>
+      </c>
+      <c r="D64" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G62" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B63" s="2">
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="H64" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B65" s="2">
         <v>50</v>
       </c>
-      <c r="C63" s="1">
-        <v>1</v>
-      </c>
-      <c r="D63" s="2">
+      <c r="C65" s="1">
+        <v>1</v>
+      </c>
+      <c r="D65" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="E65" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="C67" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D67" s="11">
+        <f>SUM(D52:D65)</f>
+        <v>1867.66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="20">
+      <c r="A69" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F70" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="G70" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H70" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I70" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J70" s="19"/>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B71" s="2">
+        <v>56.75</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1</v>
+      </c>
+      <c r="D71" s="2">
+        <f>C71*B71</f>
+        <v>56.75</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" s="2">
         <v>49</v>
       </c>
-      <c r="G63" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
-      <c r="C65" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D65" s="11">
-        <f>SUM(D51:D63)</f>
-        <v>1852.47</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="20">
-      <c r="A67" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
-      <c r="A68" s="17" t="s">
+      <c r="C72" s="1">
+        <v>1</v>
+      </c>
+      <c r="D72" s="2">
+        <f>C72*B72</f>
+        <v>49</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" s="19" customFormat="1">
+      <c r="A73" s="1"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="C74" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D74" s="11">
+        <f>SUM(D71:D72)</f>
+        <v>105.75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="20">
+      <c r="A76" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B68" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" s="17" t="s">
+      <c r="B77" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D68" s="18" t="s">
+      <c r="D77" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E68" s="18" t="s">
+      <c r="E77" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F77" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="G77" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H77" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I77" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J77" s="19"/>
+    </row>
+    <row r="78" spans="1:10" s="22" customFormat="1">
+      <c r="A78" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B78" s="23">
+        <v>50</v>
+      </c>
+      <c r="C78" s="22">
+        <v>1</v>
+      </c>
+      <c r="D78" s="23">
+        <f>C78*B78</f>
+        <v>50</v>
+      </c>
+      <c r="E78" s="23"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="H78" s="23"/>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B79" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="C79" s="1">
+        <v>5</v>
+      </c>
+      <c r="D79" s="2">
+        <f>C79*B79</f>
+        <v>79.95</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B80" s="2">
+        <v>10</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1</v>
+      </c>
+      <c r="D80" s="2">
+        <f>C80*B80</f>
+        <v>10</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" s="19" customFormat="1">
+      <c r="A82" s="1"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D82" s="11">
+        <f>SUM(D78:D80)</f>
+        <v>139.94999999999999</v>
+      </c>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+    </row>
+    <row r="84" spans="1:10" ht="20">
+      <c r="A84" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E85" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F85" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="G85" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H85" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I85" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J85" s="19"/>
+    </row>
+    <row r="86" spans="1:10" s="22" customFormat="1">
+      <c r="A86" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B86" s="23">
+        <v>4.41</v>
+      </c>
+      <c r="C86" s="22">
+        <v>200</v>
+      </c>
+      <c r="D86" s="23">
+        <f t="shared" ref="D86:D91" si="2">C86*B86</f>
+        <v>882</v>
+      </c>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H86" s="23"/>
+      <c r="I86" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F68" s="18" t="s">
+      <c r="B87" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="C87" s="1">
+        <v>200</v>
+      </c>
+      <c r="D87" s="2">
+        <f>C87*B87</f>
+        <v>126</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I87" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G68" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="H68" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I68" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J68" s="19"/>
-    </row>
-    <row r="69" spans="1:10">
-      <c r="A69" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" s="2">
-        <v>56.75</v>
-      </c>
-      <c r="C69" s="1">
-        <v>1</v>
-      </c>
-      <c r="D69" s="2">
-        <f>C69*B69</f>
-        <v>56.75</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
-      <c r="A70" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B70" s="2">
-        <v>49</v>
-      </c>
-      <c r="C70" s="1">
-        <v>1</v>
-      </c>
-      <c r="D70" s="2">
-        <f>C70*B70</f>
-        <v>49</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" s="19" customFormat="1">
-      <c r="A71" s="1"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-    </row>
-    <row r="72" spans="1:10">
-      <c r="C72" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D72" s="11">
-        <f>SUM(D69:D70)</f>
-        <v>105.75</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="20">
-      <c r="A74" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B75" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C75" s="17" t="s">
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B88" s="2">
+        <v>7.27</v>
+      </c>
+      <c r="C88" s="1">
         <v>2</v>
       </c>
-      <c r="D75" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E75" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F75" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="G75" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="H75" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I75" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J75" s="19"/>
-    </row>
-    <row r="76" spans="1:10">
-      <c r="A76" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B76" s="2">
-        <v>50</v>
-      </c>
-      <c r="C76" s="1">
-        <v>1</v>
-      </c>
-      <c r="D76" s="2">
-        <f>C76*B76</f>
-        <v>50</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10">
-      <c r="A77" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B77" s="2">
-        <v>15.99</v>
-      </c>
-      <c r="C77" s="1">
-        <v>6</v>
-      </c>
-      <c r="D77" s="2">
-        <f>C77*B77</f>
-        <v>95.94</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
-      <c r="A78" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B78" s="2">
-        <v>10</v>
-      </c>
-      <c r="C78" s="1">
-        <v>1</v>
-      </c>
-      <c r="D78" s="2">
-        <f>C78*B78</f>
-        <v>10</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H78" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" s="19" customFormat="1">
-      <c r="A80" s="1"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D80" s="11">
-        <f>SUM(D76:D78)</f>
-        <v>155.94</v>
-      </c>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-    </row>
-    <row r="82" spans="1:10" ht="20">
-      <c r="A82" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10">
-      <c r="A83" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B83" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C83" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D83" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E83" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F83" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="G83" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="H83" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I83" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J83" s="19"/>
-    </row>
-    <row r="84" spans="1:10">
-      <c r="A84" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B84" s="2">
-        <v>4.41</v>
-      </c>
-      <c r="C84" s="1">
-        <v>200</v>
-      </c>
-      <c r="D84" s="2">
-        <f t="shared" ref="D84:D89" si="2">C84*B84</f>
-        <v>882</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I84" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
-      <c r="A85" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B85" s="2">
-        <v>23</v>
-      </c>
-      <c r="C85" s="1">
-        <v>4</v>
-      </c>
-      <c r="D85" s="2">
-        <f t="shared" si="2"/>
-        <v>92</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I85" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10">
-      <c r="A86" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B86" s="2">
-        <v>7.27</v>
-      </c>
-      <c r="C86" s="1">
-        <v>2</v>
-      </c>
-      <c r="D86" s="2">
+      <c r="D88" s="2">
         <f t="shared" si="2"/>
         <v>14.54</v>
       </c>
-      <c r="E86" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I86" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10">
-      <c r="A87" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B87" s="2">
+      <c r="E88" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" s="19" customFormat="1">
+      <c r="A89" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B89" s="2">
         <v>89.9</v>
       </c>
-      <c r="C87" s="1">
-        <v>1</v>
-      </c>
-      <c r="D87" s="2">
+      <c r="C89" s="1">
+        <v>1</v>
+      </c>
+      <c r="D89" s="2">
         <f t="shared" si="2"/>
         <v>89.9</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I87" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" s="19" customFormat="1">
-      <c r="A88" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B88" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="C88" s="1">
-        <v>4</v>
-      </c>
-      <c r="D88" s="2">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H88" s="2"/>
-      <c r="I88" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J88" s="1"/>
-    </row>
-    <row r="89" spans="1:10">
-      <c r="A89" s="1" t="s">
+      <c r="E89" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H89" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B89" s="2">
-        <v>121</v>
-      </c>
-      <c r="C89" s="1">
-        <v>1</v>
-      </c>
-      <c r="D89" s="2">
-        <f t="shared" si="2"/>
-        <v>121</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="I89" s="1" t="s">
-        <v>87</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="J89" s="1"/>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="1" t="s">
-        <v>95</v>
+        <v>119</v>
+      </c>
+      <c r="B90" s="2">
+        <v>6.45</v>
+      </c>
+      <c r="C90" s="1">
+        <v>2</v>
+      </c>
+      <c r="D90" s="2">
+        <f t="shared" si="2"/>
+        <v>12.9</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10">
-      <c r="A91" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B91" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" s="22" customFormat="1">
+      <c r="A91" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B91" s="23">
+        <v>18.95</v>
+      </c>
+      <c r="C91" s="22">
+        <v>1</v>
+      </c>
+      <c r="D91" s="23">
+        <f t="shared" si="2"/>
+        <v>18.95</v>
+      </c>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H91" s="23"/>
+      <c r="I91" s="22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" s="22" customFormat="1">
+      <c r="A92" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B92" s="23"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="H92" s="23"/>
+      <c r="I92" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B93" s="2">
         <v>5.9</v>
       </c>
-      <c r="C91" s="1">
-        <v>1</v>
-      </c>
-      <c r="D91" s="2">
-        <f>C91*B91</f>
+      <c r="C93" s="1">
+        <v>1</v>
+      </c>
+      <c r="D93" s="2">
+        <f>C93*B93</f>
         <v>5.9</v>
       </c>
-      <c r="E91" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10">
-      <c r="A92" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B92" s="2">
-        <v>0.47</v>
-      </c>
-      <c r="C92" s="1">
-        <v>200</v>
-      </c>
-      <c r="D92" s="2">
-        <f>C92*B92</f>
+      <c r="E93" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B94" s="2">
+        <v>16.71</v>
+      </c>
+      <c r="C94" s="1">
+        <v>1</v>
+      </c>
+      <c r="D94" s="2">
+        <f>C94*B94</f>
+        <v>16.71</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B95" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="C95" s="1">
+        <v>2</v>
+      </c>
+      <c r="D95" s="2">
+        <f>C95*B95</f>
+        <v>10.4</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="10"/>
+      <c r="C98" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D98" s="11">
+        <f>SUM(D86:D95)</f>
+        <v>1177.3000000000004</v>
+      </c>
+      <c r="I98" s="15"/>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="20"/>
+      <c r="B99" s="21"/>
+      <c r="C99" s="20"/>
+      <c r="D99" s="21"/>
+      <c r="E99" s="21"/>
+      <c r="F99" s="21"/>
+      <c r="G99" s="21"/>
+      <c r="H99" s="21"/>
+      <c r="I99" s="20"/>
+    </row>
+    <row r="100" spans="1:10" ht="20">
+      <c r="A100" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E101" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F101" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="G92" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10">
-      <c r="A94" s="10"/>
-      <c r="C94" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D94" s="11">
-        <f>SUM(D84:D91)</f>
-        <v>1235.3400000000001</v>
-      </c>
-      <c r="I94" s="15"/>
-    </row>
-    <row r="95" spans="1:10">
-      <c r="A95" s="20"/>
-      <c r="B95" s="21"/>
-      <c r="C95" s="20"/>
-      <c r="D95" s="21"/>
-      <c r="E95" s="21"/>
-      <c r="F95" s="21"/>
-      <c r="G95" s="21"/>
-      <c r="H95" s="21"/>
-      <c r="I95" s="20"/>
-    </row>
-    <row r="96" spans="1:10" ht="20">
-      <c r="A96" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10">
-      <c r="A97" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B97" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C97" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D97" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E97" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F97" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="G97" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="H97" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I97" s="17" t="s">
+      <c r="G101" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H101" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I101" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J97" s="19"/>
-    </row>
-    <row r="98" spans="1:10">
-      <c r="A98" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B98" s="2">
-        <v>0</v>
-      </c>
-      <c r="C98" s="1">
-        <v>1</v>
-      </c>
-      <c r="D98" s="2">
-        <v>0</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10">
-      <c r="A99" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B99" s="2">
-        <v>0</v>
-      </c>
-      <c r="C99" s="1">
-        <v>1</v>
-      </c>
-      <c r="D99" s="2">
-        <v>0</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J99" s="15"/>
-    </row>
-    <row r="100" spans="1:10">
-      <c r="A100" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B100" s="2">
-        <v>50</v>
-      </c>
-      <c r="C100" s="1">
-        <v>3</v>
-      </c>
-      <c r="D100" s="2">
-        <f>C100*B100</f>
-        <v>150</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10">
-      <c r="A101" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B101" s="2">
-        <v>9</v>
-      </c>
-      <c r="C101" s="1">
-        <v>1</v>
-      </c>
-      <c r="D101" s="2">
-        <f>C101*B101</f>
-        <v>9</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" s="19" customFormat="1">
+      <c r="J101" s="19"/>
+    </row>
+    <row r="102" spans="1:10">
       <c r="A102" s="1" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="B102" s="2">
         <v>0</v>
       </c>
       <c r="C102" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D102" s="2">
         <v>0</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F102" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="G102" s="2" t="s">
-        <v>123</v>
+        <v>57</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="1" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
       <c r="B103" s="2">
         <v>0</v>
       </c>
       <c r="C103" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D103" s="2">
         <v>0</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>62</v>
+        <v>45</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>123</v>
+        <v>57</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" s="15" customFormat="1">
-      <c r="A104" s="1"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="1"/>
-      <c r="J104" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="J103" s="15"/>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B104" s="2">
+        <v>28.75</v>
+      </c>
+      <c r="C104" s="1">
+        <v>1</v>
+      </c>
+      <c r="D104" s="2">
+        <f>C104*B104</f>
+        <v>28.75</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="105" spans="1:10">
-      <c r="C105" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D105" s="11">
-        <f>SUM(D98:D103)</f>
-        <v>159</v>
+      <c r="A105" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B105" s="2">
+        <v>9</v>
+      </c>
+      <c r="C105" s="1">
+        <v>1</v>
+      </c>
+      <c r="D105" s="2">
+        <f>C105*B105</f>
+        <v>9</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" s="19" customFormat="1">
+      <c r="A106" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B106" s="2">
+        <v>0</v>
+      </c>
+      <c r="C106" s="1">
+        <v>2</v>
+      </c>
+      <c r="D106" s="2">
+        <v>0</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B107" s="2">
+        <v>0</v>
+      </c>
+      <c r="C107" s="1">
+        <v>2</v>
+      </c>
+      <c r="D107" s="2">
+        <v>0</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" s="15" customFormat="1">
+      <c r="A108" s="1"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="C109" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D109" s="11">
+        <f>SUM(D102:D107)</f>
+        <v>37.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bought things, many things
</commit_message>
<xml_diff>
--- a/DetailedBudget.xlsx
+++ b/DetailedBudget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="8300" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="155">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -81,9 +81,6 @@
     <t>FARADAY CAGE</t>
   </si>
   <si>
-    <t>Vinyl blanks</t>
-  </si>
-  <si>
     <t>GRAND TOTAL</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>REMAINING</t>
   </si>
   <si>
-    <t>http://recordcuttingblanks.com/7-INCH-RECORD-BLANKS.html</t>
-  </si>
-  <si>
     <t>Labels with preprinted w info (3-1/3x4", pack of 150)</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>UBLD</t>
   </si>
   <si>
-    <t>Record Cutting Blanks</t>
-  </si>
-  <si>
     <t>Amazon</t>
   </si>
   <si>
@@ -270,9 +261,6 @@
     <t>Tamper-resistant stickers (1800 labels)</t>
   </si>
   <si>
-    <t>More acetate film</t>
-  </si>
-  <si>
     <t>ePlastics</t>
   </si>
   <si>
@@ -412,6 +400,90 @@
   </si>
   <si>
     <t>Travel expenses/fee for musicians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use coupon code R1791537AD </t>
+  </si>
+  <si>
+    <t>Canakit</t>
+  </si>
+  <si>
+    <t>(or use my small 10W)</t>
+  </si>
+  <si>
+    <t>http://www.canakit.com/0-5w-universal-mini-amplifier-kit-ck026-uk026.html</t>
+  </si>
+  <si>
+    <t>VU meter (500uA, 700ohm)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/gp/product/B00ARBSTVO?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o00_s00</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/281255271864</t>
+  </si>
+  <si>
+    <t>Drill bushing (for center holes)</t>
+  </si>
+  <si>
+    <t>7.3mm</t>
+  </si>
+  <si>
+    <t>McMaster Carr</t>
+  </si>
+  <si>
+    <t>9/32"</t>
+  </si>
+  <si>
+    <t>Drill rod (for center holes)</t>
+  </si>
+  <si>
+    <t>7.3mm, 4.25" long</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#2900a351/=ygxi4p</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#8486a41/=ygxihl</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#8491a296/=ygximw</t>
+  </si>
+  <si>
+    <t>9/32", 4.25" long</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#3009a129/=ygxisk</t>
+  </si>
+  <si>
+    <t>Gum rubber vacuum tubing (priced per foot)</t>
+  </si>
+  <si>
+    <t>3/16" ID, 1/8" wall</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#5543k21/=ygxj3d</t>
+  </si>
+  <si>
+    <t>UK-style plug adapters (4-pack)</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/OREI-Hong-Kong-Adapter-Plug/dp/B008Y8PSSE/ref=sr_1_10?ie=UTF8&amp;qid=1439408007&amp;sr=8-10&amp;keywords=us+to+uk+power+adapter</t>
+  </si>
+  <si>
+    <t>http://www.bhphotovideo.com/c/product/822508-REG/Focusrite_SCARLETT_2I2_USB_Scarlett_2i2_Portable.html</t>
+  </si>
+  <si>
+    <t>Focusrite Scarlett 2i2 portable audio interface</t>
+  </si>
+  <si>
+    <t>Acetate film for cutting records</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/gp/product/B005OZE9SA/ref=ox_sc_imb_mini_detail?ie=UTF8&amp;psc=1&amp;smid=ATVPDKIKX0DER</t>
   </si>
 </sst>
 </file>
@@ -518,7 +590,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="222">
+  <cellStyleXfs count="248">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -741,8 +813,34 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -773,8 +871,9 @@
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="222">
+  <cellStyles count="248">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -886,6 +985,19 @@
     <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -996,6 +1108,19 @@
     <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1325,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J109"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1352,32 +1477,32 @@
     </row>
     <row r="2" spans="1:9" ht="20">
       <c r="E2" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:9" s="10" customFormat="1" ht="20">
       <c r="A3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6">
-        <f>D19+D29+D38+D48+D67+D74+D82+D98+D109</f>
-        <v>11741.19</v>
+        <f>D19+D29+D38+D48+D68+D75+D83+D102+D115</f>
+        <v>11756.75</v>
       </c>
       <c r="E3" s="7">
         <v>0.64</v>
       </c>
       <c r="F3" s="8">
         <f>D3*E3</f>
-        <v>7514.3616000000002</v>
+        <v>7524.32</v>
       </c>
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:9" ht="20">
       <c r="A4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="5"/>
@@ -1395,20 +1520,20 @@
     </row>
     <row r="5" spans="1:9" ht="20">
       <c r="A5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6">
         <f>D4-D3</f>
-        <v>758.80999999999949</v>
+        <v>743.25</v>
       </c>
       <c r="E5" s="7">
         <v>0.64</v>
       </c>
       <c r="F5" s="8">
         <f>D5*E5</f>
-        <v>485.63839999999971</v>
+        <v>475.68</v>
       </c>
       <c r="H5" s="9"/>
     </row>
@@ -1444,7 +1569,7 @@
     </row>
     <row r="9" spans="1:9" ht="20">
       <c r="A9" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="19" customFormat="1">
@@ -1461,16 +1586,16 @@
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>4</v>
@@ -1478,7 +1603,7 @@
     </row>
     <row r="11" spans="1:9" s="15" customFormat="1">
       <c r="A11" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2">
         <v>850</v>
@@ -1491,20 +1616,20 @@
         <v>850</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2">
         <v>100</v>
@@ -1519,7 +1644,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" s="2">
         <v>600</v>
@@ -1534,7 +1659,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2">
         <v>600</v>
@@ -1549,7 +1674,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B15" s="2">
         <v>2025</v>
@@ -1562,18 +1687,18 @@
         <v>2025</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2">
         <v>3000</v>
@@ -1588,7 +1713,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B17" s="2">
         <v>15</v>
@@ -1601,18 +1726,18 @@
         <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="C19" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D19" s="11">
         <f>SUM(D11:D17)</f>
@@ -1621,7 +1746,7 @@
     </row>
     <row r="21" spans="1:9" ht="20">
       <c r="A21" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="19" customFormat="1">
@@ -1638,16 +1763,16 @@
         <v>3</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I22" s="17" t="s">
         <v>4</v>
@@ -1655,28 +1780,28 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B23" s="2">
-        <v>48</v>
+        <v>74.7</v>
       </c>
       <c r="C23" s="1">
         <v>14</v>
       </c>
       <c r="D23" s="2">
         <f>C23*B23</f>
-        <v>672</v>
+        <v>1045.8</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" s="2">
         <v>0</v>
@@ -1688,20 +1813,20 @@
         <v>0</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B26" s="2">
         <v>0</v>
@@ -1713,21 +1838,21 @@
         <v>0</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="C29" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D29" s="11">
         <f>SUM(D23:D27)</f>
-        <v>672</v>
+        <v>1045.8</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="20">
@@ -1757,16 +1882,16 @@
         <v>3</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I32" s="17" t="s">
         <v>4</v>
@@ -1787,16 +1912,16 @@
         <v>12.9</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>7</v>
@@ -1804,7 +1929,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B34" s="2">
         <v>0.48</v>
@@ -1817,13 +1942,13 @@
         <v>2.88</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="22" customFormat="1">
@@ -1855,13 +1980,13 @@
         <v>30</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>9</v>
@@ -1869,7 +1994,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="C38" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D38" s="11">
         <f>SUM(D33:D36)</f>
@@ -1895,16 +2020,16 @@
         <v>3</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I41" s="17" t="s">
         <v>4</v>
@@ -1925,10 +2050,10 @@
         <v>400</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1946,7 +2071,7 @@
         <v>10</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="22" customFormat="1">
@@ -1966,13 +2091,13 @@
       <c r="E44" s="23"/>
       <c r="F44" s="23"/>
       <c r="G44" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H44" s="23"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B45" s="2">
         <v>0</v>
@@ -1984,12 +2109,12 @@
         <v>0</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="22" customFormat="1">
       <c r="A46" s="22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B46" s="23">
         <v>40</v>
@@ -2008,7 +2133,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="C48" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D48" s="11">
         <f>SUM(D42:D46)</f>
@@ -2034,16 +2159,16 @@
         <v>3</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F51" s="18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I51" s="17" t="s">
         <v>4</v>
@@ -2051,7 +2176,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B52" s="2">
         <v>1500</v>
@@ -2060,22 +2185,22 @@
         <v>1</v>
       </c>
       <c r="D52" s="2">
-        <f t="shared" ref="D52:D65" si="1">C52*B52</f>
+        <f t="shared" ref="D52:D66" si="1">C52*B52</f>
         <v>1500</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B53" s="2">
         <v>280</v>
@@ -2088,18 +2213,18 @@
         <v>280</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B54" s="2">
         <v>13</v>
@@ -2112,25 +2237,43 @@
         <v>13</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" s="22" customFormat="1">
-      <c r="A55" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B55" s="23"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="23"/>
-      <c r="G55" s="23"/>
-      <c r="H55" s="23"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="2">
+        <v>0</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
@@ -2143,22 +2286,22 @@
         <v>1</v>
       </c>
       <c r="D56" s="2">
-        <f>C56*B56</f>
+        <f t="shared" ref="D56:D62" si="2">C56*B56</f>
         <v>6.24</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B57" s="2">
         <v>2.36</v>
@@ -2167,25 +2310,25 @@
         <v>2</v>
       </c>
       <c r="D57" s="2">
-        <f>C57*B57</f>
+        <f t="shared" si="2"/>
         <v>4.72</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B58" s="2">
         <f>1.94+2.29</f>
@@ -2195,22 +2338,22 @@
         <v>1</v>
       </c>
       <c r="D58" s="2">
-        <f>C58*B58</f>
+        <f t="shared" si="2"/>
         <v>4.2300000000000004</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B59" s="2">
         <v>3.49</v>
@@ -2219,22 +2362,22 @@
         <v>1</v>
       </c>
       <c r="D59" s="2">
-        <f>C59*B59</f>
+        <f t="shared" si="2"/>
         <v>3.49</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B60" s="2">
         <v>2.99</v>
@@ -2243,33 +2386,46 @@
         <v>2</v>
       </c>
       <c r="D60" s="2">
-        <f>C60*B60</f>
+        <f t="shared" si="2"/>
         <v>5.98</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" s="22" customFormat="1">
-      <c r="A61" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B61" s="23"/>
-      <c r="D61" s="23"/>
-      <c r="E61" s="23"/>
-      <c r="F61" s="23"/>
-      <c r="G61" s="23"/>
-      <c r="H61" s="23"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" s="2">
+        <v>10</v>
+      </c>
+      <c r="C61" s="1">
+        <v>3</v>
+      </c>
+      <c r="D61" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="62" spans="1:9" s="22" customFormat="1">
       <c r="A62" s="22" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B62" s="23">
         <v>269</v>
@@ -2277,20 +2433,23 @@
       <c r="C62" s="22">
         <v>1</v>
       </c>
-      <c r="D62" s="23"/>
+      <c r="D62" s="23">
+        <f t="shared" si="2"/>
+        <v>269</v>
+      </c>
       <c r="E62" s="23"/>
       <c r="F62" s="23"/>
       <c r="G62" s="23" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H62" s="23"/>
       <c r="I62" s="22" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B63" s="2">
         <v>0</v>
@@ -2303,367 +2462,372 @@
         <v>0</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="22" customFormat="1">
       <c r="A64" s="22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B64" s="23">
-        <v>0</v>
+        <v>14.95</v>
       </c>
       <c r="C64" s="22">
         <v>1</v>
       </c>
       <c r="D64" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E64" s="23"/>
+        <v>14.95</v>
+      </c>
+      <c r="E64" s="23" t="s">
+        <v>132</v>
+      </c>
       <c r="F64" s="23"/>
       <c r="G64" s="23" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="H64" s="23" t="s">
-        <v>65</v>
+        <v>129</v>
+      </c>
+      <c r="I64" s="22" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="1" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
       <c r="B65" s="2">
-        <v>50</v>
+        <v>10.57</v>
       </c>
       <c r="C65" s="1">
         <v>1</v>
       </c>
       <c r="D65" s="2">
         <f t="shared" si="1"/>
+        <v>10.57</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B66" s="2">
         <v>50</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
-      <c r="C67" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D67" s="11">
-        <f>SUM(D52:D65)</f>
-        <v>1867.66</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="20">
-      <c r="A69" s="5" t="s">
+      <c r="C66" s="1">
+        <v>1</v>
+      </c>
+      <c r="D66" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="C68" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D68" s="11">
+        <f>SUM(D52:D66)</f>
+        <v>2192.1799999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="20">
+      <c r="A70" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
-      <c r="A70" s="17" t="s">
+    <row r="71" spans="1:10">
+      <c r="A71" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B70" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C70" s="17" t="s">
+      <c r="B71" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D70" s="18" t="s">
+      <c r="D71" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E70" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="F70" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="G70" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H70" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="I70" s="17" t="s">
+      <c r="E71" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="F71" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G71" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H71" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I71" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J70" s="19"/>
-    </row>
-    <row r="71" spans="1:10">
-      <c r="A71" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B71" s="2">
-        <v>56.75</v>
-      </c>
-      <c r="C71" s="1">
-        <v>1</v>
-      </c>
-      <c r="D71" s="2">
-        <f>C71*B71</f>
-        <v>56.75</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="J71" s="19"/>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B72" s="2">
-        <v>49</v>
+        <v>56.75</v>
       </c>
       <c r="C72" s="1">
         <v>1</v>
       </c>
       <c r="D72" s="2">
         <f>C72*B72</f>
+        <v>56.75</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B73" s="2">
         <v>49</v>
       </c>
-      <c r="E72" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G72" s="2" t="s">
+      <c r="C73" s="1">
+        <v>1</v>
+      </c>
+      <c r="D73" s="2">
+        <f>C73*B73</f>
+        <v>49</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" s="19" customFormat="1">
+      <c r="A74" s="1"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="C75" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" s="19" customFormat="1">
-      <c r="A73" s="1"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-    </row>
-    <row r="74" spans="1:10">
-      <c r="C74" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D74" s="11">
-        <f>SUM(D71:D72)</f>
+      <c r="D75" s="11">
+        <f>SUM(D72:D73)</f>
         <v>105.75</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="20">
-      <c r="A76" s="5" t="s">
+    <row r="77" spans="1:10" ht="20">
+      <c r="A77" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
-      <c r="A77" s="17" t="s">
+    <row r="78" spans="1:10">
+      <c r="A78" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B77" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C77" s="17" t="s">
+      <c r="B78" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D77" s="18" t="s">
+      <c r="D78" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E77" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="F77" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="G77" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H77" s="18" t="s">
+      <c r="E78" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="F78" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G78" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H78" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I78" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J78" s="19"/>
+    </row>
+    <row r="79" spans="1:10" s="22" customFormat="1">
+      <c r="A79" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B79" s="23">
         <v>50</v>
       </c>
-      <c r="I77" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J77" s="19"/>
-    </row>
-    <row r="78" spans="1:10" s="22" customFormat="1">
-      <c r="A78" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="B78" s="23">
+      <c r="C79" s="22">
+        <v>1</v>
+      </c>
+      <c r="D79" s="23">
+        <f>C79*B79</f>
         <v>50</v>
       </c>
-      <c r="C78" s="22">
-        <v>1</v>
-      </c>
-      <c r="D78" s="23">
-        <f>C78*B78</f>
-        <v>50</v>
-      </c>
-      <c r="E78" s="23"/>
-      <c r="F78" s="23"/>
-      <c r="G78" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="H78" s="23"/>
-    </row>
-    <row r="79" spans="1:10">
-      <c r="A79" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B79" s="2">
-        <v>15.99</v>
-      </c>
-      <c r="C79" s="1">
-        <v>5</v>
-      </c>
-      <c r="D79" s="2">
-        <f>C79*B79</f>
-        <v>79.95</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G79" s="2" t="s">
+      <c r="E79" s="23"/>
+      <c r="F79" s="23"/>
+      <c r="G79" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="I79" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="H79" s="23"/>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B80" s="2">
-        <v>10</v>
+        <v>15.99</v>
       </c>
       <c r="C80" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D80" s="2">
         <f>C80*B80</f>
+        <v>79.95</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B81" s="2">
         <v>10</v>
       </c>
-      <c r="E80" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" s="19" customFormat="1">
-      <c r="A82" s="1"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D82" s="11">
-        <f>SUM(D78:D80)</f>
+      <c r="C81" s="1">
+        <v>1</v>
+      </c>
+      <c r="D81" s="2">
+        <f>C81*B81</f>
+        <v>10</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" s="19" customFormat="1">
+      <c r="A83" s="1"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D83" s="11">
+        <f>SUM(D79:D81)</f>
         <v>139.94999999999999</v>
       </c>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="1"/>
-    </row>
-    <row r="84" spans="1:10" ht="20">
-      <c r="A84" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
-      <c r="A85" s="17" t="s">
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+    </row>
+    <row r="85" spans="1:10" ht="20">
+      <c r="A85" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B85" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C85" s="17" t="s">
+      <c r="B86" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D85" s="18" t="s">
+      <c r="D86" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E85" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="F85" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="G85" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H85" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="I85" s="17" t="s">
+      <c r="E86" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="F86" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G86" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H86" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I86" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J85" s="19"/>
-    </row>
-    <row r="86" spans="1:10" s="22" customFormat="1">
-      <c r="A86" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B86" s="23">
-        <v>4.41</v>
-      </c>
-      <c r="C86" s="22">
-        <v>200</v>
-      </c>
-      <c r="D86" s="23">
-        <f t="shared" ref="D86:D91" si="2">C86*B86</f>
-        <v>882</v>
-      </c>
-      <c r="E86" s="23"/>
-      <c r="F86" s="23"/>
-      <c r="G86" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="H86" s="23"/>
-      <c r="I86" s="22" t="s">
-        <v>24</v>
-      </c>
+      <c r="J86" s="19"/>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B87" s="2">
         <v>0.63</v>
@@ -2676,18 +2840,18 @@
         <v>126</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B88" s="2">
         <v>7.27</v>
@@ -2696,25 +2860,25 @@
         <v>2</v>
       </c>
       <c r="D88" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D88:D91" si="3">C88*B88</f>
         <v>14.54</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="89" spans="1:10" s="19" customFormat="1">
       <c r="A89" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B89" s="2">
         <v>89.9</v>
@@ -2723,93 +2887,100 @@
         <v>1</v>
       </c>
       <c r="D89" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>89.9</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J89" s="1"/>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B90" s="2">
         <v>6.45</v>
       </c>
       <c r="C90" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D90" s="2">
-        <f t="shared" si="2"/>
-        <v>12.9</v>
+        <f t="shared" si="3"/>
+        <v>19.350000000000001</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" s="22" customFormat="1">
-      <c r="A91" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="B91" s="23">
-        <v>18.95</v>
-      </c>
-      <c r="C91" s="22">
-        <v>1</v>
-      </c>
-      <c r="D91" s="23">
-        <f t="shared" si="2"/>
-        <v>18.95</v>
-      </c>
-      <c r="E91" s="23"/>
-      <c r="F91" s="23"/>
-      <c r="G91" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="H91" s="23"/>
-      <c r="I91" s="22" t="s">
-        <v>123</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B91" s="2">
+        <f>18.95+4.95-5</f>
+        <v>18.899999999999999</v>
+      </c>
+      <c r="C91" s="1">
+        <v>1</v>
+      </c>
+      <c r="D91" s="2">
+        <f t="shared" si="3"/>
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="92" spans="1:10" s="22" customFormat="1">
       <c r="A92" s="22" t="s">
-        <v>83</v>
+        <v>153</v>
       </c>
       <c r="B92" s="23"/>
       <c r="D92" s="23"/>
       <c r="E92" s="23"/>
       <c r="F92" s="23"/>
       <c r="G92" s="23" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H92" s="23"/>
       <c r="I92" s="22" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B93" s="2">
         <v>5.9</v>
@@ -2822,18 +2993,18 @@
         <v>5.9</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B94" s="2">
         <v>16.71</v>
@@ -2846,18 +3017,21 @@
         <v>16.71</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B95" s="2">
         <v>5.2</v>
@@ -2870,244 +3044,437 @@
         <v>10.4</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10">
-      <c r="A98" s="10"/>
-      <c r="C98" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D98" s="11">
-        <f>SUM(D86:D95)</f>
-        <v>1177.3000000000004</v>
-      </c>
-      <c r="I98" s="15"/>
-    </row>
-    <row r="99" spans="1:10">
-      <c r="A99" s="20"/>
-      <c r="B99" s="21"/>
-      <c r="C99" s="20"/>
-      <c r="D99" s="21"/>
-      <c r="E99" s="21"/>
-      <c r="F99" s="21"/>
-      <c r="G99" s="21"/>
-      <c r="H99" s="21"/>
-      <c r="I99" s="20"/>
-    </row>
-    <row r="100" spans="1:10" ht="20">
-      <c r="A100" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10">
-      <c r="A101" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" s="22" customFormat="1">
+      <c r="A96" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B96" s="23">
+        <v>8.43</v>
+      </c>
+      <c r="C96" s="22">
         <v>0</v>
       </c>
-      <c r="B101" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C101" s="17" t="s">
+      <c r="D96" s="23">
+        <f>C96*B96</f>
+        <v>0</v>
+      </c>
+      <c r="E96" s="23"/>
+      <c r="F96" s="23"/>
+      <c r="G96" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H96" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="I96" s="22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" s="22" customFormat="1">
+      <c r="A97" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B97" s="23">
+        <v>5.84</v>
+      </c>
+      <c r="C97" s="22">
+        <v>0</v>
+      </c>
+      <c r="D97" s="23">
+        <f>C97*B97</f>
+        <v>0</v>
+      </c>
+      <c r="E97" s="23"/>
+      <c r="F97" s="23"/>
+      <c r="G97" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H97" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="I97" s="22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" s="22" customFormat="1">
+      <c r="A98" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B98" s="23">
+        <v>9.5</v>
+      </c>
+      <c r="C98" s="22">
         <v>2</v>
       </c>
-      <c r="D101" s="18" t="s">
+      <c r="D98" s="23">
+        <f>C98*B98</f>
+        <v>19</v>
+      </c>
+      <c r="E98" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F98" s="23"/>
+      <c r="G98" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H98" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="I98" s="22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" s="22" customFormat="1">
+      <c r="A99" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B99" s="23">
+        <v>5.26</v>
+      </c>
+      <c r="C99" s="22">
+        <v>1</v>
+      </c>
+      <c r="D99" s="23">
+        <f>C99*B99</f>
+        <v>5.26</v>
+      </c>
+      <c r="E99" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F99" s="23"/>
+      <c r="G99" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H99" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="I99" s="22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" s="22" customFormat="1">
+      <c r="A100" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="B100" s="23">
+        <v>3.72</v>
+      </c>
+      <c r="C100" s="22">
+        <v>5</v>
+      </c>
+      <c r="D100" s="23">
+        <f>C100*B100</f>
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E100" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F100" s="23"/>
+      <c r="G100" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H100" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="I100" s="22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="10"/>
+      <c r="C102" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D102" s="11">
+        <f>SUM(D87:D100)</f>
+        <v>344.55999999999995</v>
+      </c>
+      <c r="I102" s="15"/>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="20"/>
+      <c r="B103" s="21"/>
+      <c r="C103" s="20"/>
+      <c r="D103" s="21"/>
+      <c r="E103" s="21"/>
+      <c r="F103" s="21"/>
+      <c r="G103" s="21"/>
+      <c r="H103" s="21"/>
+      <c r="I103" s="20"/>
+    </row>
+    <row r="104" spans="1:10" ht="20">
+      <c r="A104" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D105" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E101" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="F101" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="G101" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H101" s="18" t="s">
+      <c r="E105" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="F105" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G105" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H105" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I105" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J105" s="19"/>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="I101" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J101" s="19"/>
-    </row>
-    <row r="102" spans="1:10">
-      <c r="A102" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B102" s="2">
-        <v>0</v>
-      </c>
-      <c r="C102" s="1">
-        <v>1</v>
-      </c>
-      <c r="D102" s="2">
-        <v>0</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G102" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H102" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10">
-      <c r="A103" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B103" s="2">
-        <v>0</v>
-      </c>
-      <c r="C103" s="1">
-        <v>1</v>
-      </c>
-      <c r="D103" s="2">
-        <v>0</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G103" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H103" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J103" s="15"/>
-    </row>
-    <row r="104" spans="1:10">
-      <c r="A104" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B104" s="2">
-        <v>28.75</v>
-      </c>
-      <c r="C104" s="1">
-        <v>1</v>
-      </c>
-      <c r="D104" s="2">
-        <f>C104*B104</f>
-        <v>28.75</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H104" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I104" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10">
-      <c r="A105" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B105" s="2">
-        <v>9</v>
-      </c>
-      <c r="C105" s="1">
-        <v>1</v>
-      </c>
-      <c r="D105" s="2">
-        <f>C105*B105</f>
-        <v>9</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" s="19" customFormat="1">
-      <c r="A106" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="B106" s="2">
         <v>0</v>
       </c>
       <c r="C106" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D106" s="2">
         <v>0</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F106" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="G106" s="2" t="s">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I106" s="1"/>
-      <c r="J106" s="1"/>
+        <v>62</v>
+      </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="1" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="B107" s="2">
         <v>0</v>
       </c>
       <c r="C107" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D107" s="2">
         <v>0</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="G107" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J107" s="15"/>
+    </row>
+    <row r="108" spans="1:10" s="22" customFormat="1">
+      <c r="A108" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B108" s="23">
+        <v>149.99</v>
+      </c>
+      <c r="C108" s="22">
+        <v>1</v>
+      </c>
+      <c r="D108" s="23">
+        <f>C108*B108</f>
+        <v>149.99</v>
+      </c>
+      <c r="E108" s="23"/>
+      <c r="F108" s="23"/>
+      <c r="G108" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="H108" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="I108" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="J108" s="24"/>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H107" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" s="15" customFormat="1">
-      <c r="A108" s="1"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="2"/>
-      <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
-      <c r="G108" s="2"/>
-      <c r="H108" s="2"/>
-      <c r="I108" s="1"/>
-      <c r="J108" s="1"/>
-    </row>
-    <row r="109" spans="1:10">
-      <c r="C109" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D109" s="11">
-        <f>SUM(D102:D107)</f>
-        <v>37.75</v>
+      <c r="B109" s="2">
+        <v>28.75</v>
+      </c>
+      <c r="C109" s="1">
+        <v>1</v>
+      </c>
+      <c r="D109" s="2">
+        <f>C109*B109</f>
+        <v>28.75</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" s="22" customFormat="1">
+      <c r="A110" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="B110" s="23">
+        <v>8.99</v>
+      </c>
+      <c r="C110" s="22">
+        <v>1</v>
+      </c>
+      <c r="D110" s="23">
+        <f>C110*B110</f>
+        <v>8.99</v>
+      </c>
+      <c r="E110" s="23"/>
+      <c r="F110" s="23"/>
+      <c r="G110" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="H110" s="23"/>
+      <c r="I110" s="22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" s="19" customFormat="1">
+      <c r="A111" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B111" s="2">
+        <v>0</v>
+      </c>
+      <c r="C111" s="1">
+        <v>2</v>
+      </c>
+      <c r="D111" s="2">
+        <v>0</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F111" s="2"/>
+      <c r="G111" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I111" s="1"/>
+      <c r="J111" s="1"/>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="A112" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B112" s="2">
+        <v>0</v>
+      </c>
+      <c r="C112" s="1">
+        <v>2</v>
+      </c>
+      <c r="D112" s="2">
+        <v>0</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B113" s="2">
+        <v>9</v>
+      </c>
+      <c r="C113" s="1">
+        <v>1</v>
+      </c>
+      <c r="D113" s="2">
+        <f>C113*B113</f>
+        <v>9</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" s="15" customFormat="1">
+      <c r="A114" s="1"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="C115" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D115" s="11">
+        <f>SUM(D106:D112)</f>
+        <v>187.73000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More stuff coming in
</commit_message>
<xml_diff>
--- a/DetailedBudget.xlsx
+++ b/DetailedBudget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8300" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="40260" yWindow="540" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="165">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -474,9 +474,6 @@
     <t>http://www.amazon.com/OREI-Hong-Kong-Adapter-Plug/dp/B008Y8PSSE/ref=sr_1_10?ie=UTF8&amp;qid=1439408007&amp;sr=8-10&amp;keywords=us+to+uk+power+adapter</t>
   </si>
   <si>
-    <t>http://www.bhphotovideo.com/c/product/822508-REG/Focusrite_SCARLETT_2I2_USB_Scarlett_2i2_Portable.html</t>
-  </si>
-  <si>
     <t>Focusrite Scarlett 2i2 portable audio interface</t>
   </si>
   <si>
@@ -484,6 +481,39 @@
   </si>
   <si>
     <t>http://www.amazon.com/gp/product/B005OZE9SA/ref=ox_sc_imb_mini_detail?ie=UTF8&amp;psc=1&amp;smid=ATVPDKIKX0DER</t>
+  </si>
+  <si>
+    <t>3.3k resistor (for VU meter circuit)</t>
+  </si>
+  <si>
+    <t>100uF electrolytic capacitor (for VU meter circuit)</t>
+  </si>
+  <si>
+    <t>1N4001 diodes (for VU meter circuit)</t>
+  </si>
+  <si>
+    <t>Mouser #512-1N4001</t>
+  </si>
+  <si>
+    <t>Jameco #690988</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Fairchild-Semiconductor/1N4001/?qs=%2fha2pyFadug7krNqeDo6XDrkTfSK%2fTaxgQJA3tR2epo%3d</t>
+  </si>
+  <si>
+    <t>Mouser #647-UVR1E101MED1TD</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Nichicon/UVR1E101MED1TD/?qs=%2fha2pyFadugnBgCwIQYWKEIKN1uq8DHA7sJoeVl59RWjDEqjdK97Sw%3d%3d</t>
+  </si>
+  <si>
+    <t>http://www.jameco.com/webapp/wcs/stores/servlet/ProductDisplay?search_type=jamecoall&amp;catalogId=10001&amp;freeText=690988&amp;langId=-1&amp;productId=690988&amp;storeId=10001&amp;ddkey=http:StoreCatalogDrillDownView</t>
+  </si>
+  <si>
+    <t>Jameco</t>
+  </si>
+  <si>
+    <t>Mouser</t>
   </si>
 </sst>
 </file>
@@ -590,9 +620,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="248">
+  <cellStyleXfs count="270">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -873,7 +925,7 @@
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="248">
+  <cellStyles count="270">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -998,6 +1050,17 @@
     <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1121,6 +1184,17 @@
     <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1450,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1488,15 +1562,15 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6">
-        <f>D19+D29+D38+D48+D68+D75+D83+D102+D115</f>
-        <v>11756.75</v>
+        <f>D19+D29+D38+D48+D71+D78+D86+D105+D118</f>
+        <v>11757.788999999999</v>
       </c>
       <c r="E3" s="7">
         <v>0.64</v>
       </c>
       <c r="F3" s="8">
         <f>D3*E3</f>
-        <v>7524.32</v>
+        <v>7524.9849599999998</v>
       </c>
       <c r="H3" s="9"/>
     </row>
@@ -1526,14 +1600,14 @@
       <c r="C5" s="5"/>
       <c r="D5" s="6">
         <f>D4-D3</f>
-        <v>743.25</v>
+        <v>742.21100000000115</v>
       </c>
       <c r="E5" s="7">
         <v>0.64</v>
       </c>
       <c r="F5" s="8">
         <f>D5*E5</f>
-        <v>475.68</v>
+        <v>475.01504000000074</v>
       </c>
       <c r="H5" s="9"/>
     </row>
@@ -2185,7 +2259,7 @@
         <v>1</v>
       </c>
       <c r="D52" s="2">
-        <f t="shared" ref="D52:D66" si="1">C52*B52</f>
+        <f t="shared" ref="D52:D69" si="1">C52*B52</f>
         <v>1500</v>
       </c>
       <c r="E52" s="2" t="s">
@@ -2519,6 +2593,9 @@
       <c r="E65" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="F65" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="G65" s="2" t="s">
         <v>53</v>
       </c>
@@ -2528,612 +2605,613 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="1" t="s">
-        <v>41</v>
+        <v>154</v>
       </c>
       <c r="B66" s="2">
-        <v>50</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="C66" s="1">
         <v>1</v>
       </c>
       <c r="D66" s="2">
         <f t="shared" si="1"/>
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B67" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="C67" s="1">
+        <v>4</v>
+      </c>
+      <c r="D67" s="2">
+        <f t="shared" si="1"/>
+        <v>0.72</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B68" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1</v>
+      </c>
+      <c r="D68" s="2">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B69" s="2">
         <v>50</v>
       </c>
-      <c r="E66" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G66" s="2" t="s">
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
+      <c r="D69" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G69" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I66" s="1" t="s">
+      <c r="I69" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
-      <c r="C68" s="10" t="s">
+    <row r="71" spans="1:10">
+      <c r="C71" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D68" s="11">
-        <f>SUM(D52:D66)</f>
-        <v>2192.1799999999998</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="20">
-      <c r="A70" s="5" t="s">
+      <c r="D71" s="11">
+        <f>SUM(D52:D69)</f>
+        <v>2193.2189999999996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="20">
+      <c r="A73" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
-      <c r="A71" s="17" t="s">
+    <row r="74" spans="1:10">
+      <c r="A74" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B71" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="17" t="s">
+      <c r="B74" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D71" s="18" t="s">
+      <c r="D74" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E71" s="18" t="s">
+      <c r="E74" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F71" s="18" t="s">
+      <c r="F74" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="G71" s="18" t="s">
+      <c r="G74" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H71" s="18" t="s">
+      <c r="H74" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I71" s="17" t="s">
+      <c r="I74" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J71" s="19"/>
-    </row>
-    <row r="72" spans="1:10">
-      <c r="A72" s="1" t="s">
+      <c r="J74" s="19"/>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B75" s="2">
         <v>56.75</v>
       </c>
-      <c r="C72" s="1">
-        <v>1</v>
-      </c>
-      <c r="D72" s="2">
-        <f>C72*B72</f>
+      <c r="C75" s="1">
+        <v>1</v>
+      </c>
+      <c r="D75" s="2">
+        <f>C75*B75</f>
         <v>56.75</v>
       </c>
-      <c r="E72" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G72" s="2" t="s">
+      <c r="E75" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G75" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I72" s="1" t="s">
+      <c r="I75" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
-      <c r="A73" s="1" t="s">
+    <row r="76" spans="1:10">
+      <c r="A76" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B76" s="2">
         <v>49</v>
       </c>
-      <c r="C73" s="1">
-        <v>1</v>
-      </c>
-      <c r="D73" s="2">
-        <f>C73*B73</f>
+      <c r="C76" s="1">
+        <v>1</v>
+      </c>
+      <c r="D76" s="2">
+        <f>C76*B76</f>
         <v>49</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G73" s="2" t="s">
+      <c r="E76" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G76" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="19" customFormat="1">
-      <c r="A74" s="1"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="C75" s="10" t="s">
+    <row r="77" spans="1:10" s="19" customFormat="1">
+      <c r="A77" s="1"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="C78" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D75" s="11">
-        <f>SUM(D72:D73)</f>
+      <c r="D78" s="11">
+        <f>SUM(D75:D76)</f>
         <v>105.75</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="20">
-      <c r="A77" s="5" t="s">
+    <row r="80" spans="1:10" ht="20">
+      <c r="A80" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
-      <c r="A78" s="17" t="s">
+    <row r="81" spans="1:10">
+      <c r="A81" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B78" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C78" s="17" t="s">
+      <c r="B81" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D78" s="18" t="s">
+      <c r="D81" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E78" s="18" t="s">
+      <c r="E81" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F78" s="18" t="s">
+      <c r="F81" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="G78" s="18" t="s">
+      <c r="G81" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H78" s="18" t="s">
+      <c r="H81" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I78" s="17" t="s">
+      <c r="I81" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J78" s="19"/>
-    </row>
-    <row r="79" spans="1:10" s="22" customFormat="1">
-      <c r="A79" s="22" t="s">
+      <c r="J81" s="19"/>
+    </row>
+    <row r="82" spans="1:10" s="22" customFormat="1">
+      <c r="A82" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="B79" s="23">
+      <c r="B82" s="23">
         <v>50</v>
       </c>
-      <c r="C79" s="22">
-        <v>1</v>
-      </c>
-      <c r="D79" s="23">
-        <f>C79*B79</f>
+      <c r="C82" s="22">
+        <v>1</v>
+      </c>
+      <c r="D82" s="23">
+        <f>C82*B82</f>
         <v>50</v>
       </c>
-      <c r="E79" s="23"/>
-      <c r="F79" s="23"/>
-      <c r="G79" s="23" t="s">
+      <c r="E82" s="23"/>
+      <c r="F82" s="23"/>
+      <c r="G82" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="H79" s="23"/>
-    </row>
-    <row r="80" spans="1:10">
-      <c r="A80" s="1" t="s">
+      <c r="H82" s="23"/>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B83" s="2">
         <v>15.99</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C83" s="1">
         <v>5</v>
       </c>
-      <c r="D80" s="2">
-        <f>C80*B80</f>
+      <c r="D83" s="2">
+        <f>C83*B83</f>
         <v>79.95</v>
       </c>
-      <c r="E80" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G80" s="2" t="s">
+      <c r="E83" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G83" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I80" s="1" t="s">
+      <c r="I83" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
-      <c r="A81" s="1" t="s">
+    <row r="84" spans="1:10">
+      <c r="A84" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B84" s="2">
         <v>10</v>
       </c>
-      <c r="C81" s="1">
-        <v>1</v>
-      </c>
-      <c r="D81" s="2">
-        <f>C81*B81</f>
+      <c r="C84" s="1">
+        <v>1</v>
+      </c>
+      <c r="D84" s="2">
+        <f>C84*B84</f>
         <v>10</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G81" s="2" t="s">
+      <c r="E84" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G84" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H81" s="2" t="s">
+      <c r="H84" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="83" spans="1:10" s="19" customFormat="1">
-      <c r="A83" s="1"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="10" t="s">
+    <row r="86" spans="1:10" s="19" customFormat="1">
+      <c r="A86" s="1"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D83" s="11">
-        <f>SUM(D79:D81)</f>
+      <c r="D86" s="11">
+        <f>SUM(D82:D84)</f>
         <v>139.94999999999999</v>
       </c>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
-      <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
-    </row>
-    <row r="85" spans="1:10" ht="20">
-      <c r="A85" s="5" t="s">
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+    </row>
+    <row r="88" spans="1:10" ht="20">
+      <c r="A88" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
-      <c r="A86" s="17" t="s">
+    <row r="89" spans="1:10">
+      <c r="A89" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B86" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C86" s="17" t="s">
+      <c r="B89" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D86" s="18" t="s">
+      <c r="D89" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E86" s="18" t="s">
+      <c r="E89" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F86" s="18" t="s">
+      <c r="F89" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="G86" s="18" t="s">
+      <c r="G89" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H86" s="18" t="s">
+      <c r="H89" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I86" s="17" t="s">
+      <c r="I89" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J86" s="19"/>
-    </row>
-    <row r="87" spans="1:10">
-      <c r="A87" s="1" t="s">
+      <c r="J89" s="19"/>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B90" s="2">
         <v>0.63</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C90" s="1">
         <v>200</v>
       </c>
-      <c r="D87" s="2">
-        <f>C87*B87</f>
+      <c r="D90" s="2">
+        <f>C90*B90</f>
         <v>126</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G87" s="2" t="s">
+      <c r="E90" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G90" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I87" s="1" t="s">
+      <c r="I90" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
-      <c r="A88" s="1" t="s">
+    <row r="91" spans="1:10">
+      <c r="A91" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B91" s="2">
         <v>7.27</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C91" s="1">
         <v>2</v>
       </c>
-      <c r="D88" s="2">
-        <f t="shared" ref="D88:D91" si="3">C88*B88</f>
+      <c r="D91" s="2">
+        <f t="shared" ref="D91:D94" si="3">C91*B91</f>
         <v>14.54</v>
       </c>
-      <c r="E88" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G88" s="2" t="s">
+      <c r="E91" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G91" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I88" s="1" t="s">
+      <c r="I91" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:10" s="19" customFormat="1">
-      <c r="A89" s="1" t="s">
+    <row r="92" spans="1:10" s="19" customFormat="1">
+      <c r="A92" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B92" s="2">
         <v>89.9</v>
       </c>
-      <c r="C89" s="1">
-        <v>1</v>
-      </c>
-      <c r="D89" s="2">
+      <c r="C92" s="1">
+        <v>1</v>
+      </c>
+      <c r="D92" s="2">
         <f t="shared" si="3"/>
         <v>89.9</v>
       </c>
-      <c r="E89" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G89" s="2" t="s">
+      <c r="E92" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G92" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H89" s="2" t="s">
+      <c r="H92" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="I89" s="1" t="s">
+      <c r="I92" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J89" s="1"/>
-    </row>
-    <row r="90" spans="1:10">
-      <c r="A90" s="1" t="s">
+      <c r="J92" s="1"/>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B93" s="2">
         <v>6.45</v>
       </c>
-      <c r="C90" s="1">
+      <c r="C93" s="1">
         <v>3</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D93" s="2">
         <f t="shared" si="3"/>
         <v>19.350000000000001</v>
       </c>
-      <c r="E90" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G90" s="2" t="s">
+      <c r="E93" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G93" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I90" s="1" t="s">
+      <c r="I93" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
-      <c r="A91" s="1" t="s">
+    <row r="94" spans="1:10">
+      <c r="A94" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B94" s="2">
         <f>18.95+4.95-5</f>
         <v>18.899999999999999</v>
       </c>
-      <c r="C91" s="1">
-        <v>1</v>
-      </c>
-      <c r="D91" s="2">
+      <c r="C94" s="1">
+        <v>1</v>
+      </c>
+      <c r="D94" s="2">
         <f t="shared" si="3"/>
         <v>18.899999999999999</v>
       </c>
-      <c r="E91" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G91" s="2" t="s">
+      <c r="E94" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G94" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H91" s="2" t="s">
+      <c r="H94" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="I91" s="1" t="s">
+      <c r="I94" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="92" spans="1:10" s="22" customFormat="1">
-      <c r="A92" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="B92" s="23"/>
-      <c r="D92" s="23"/>
-      <c r="E92" s="23"/>
-      <c r="F92" s="23"/>
-      <c r="G92" s="23" t="s">
+    <row r="95" spans="1:10" s="22" customFormat="1">
+      <c r="A95" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B95" s="23"/>
+      <c r="D95" s="23"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="23"/>
+      <c r="G95" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="H92" s="23"/>
-      <c r="I92" s="22" t="s">
+      <c r="H95" s="23"/>
+      <c r="I95" s="22" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
-      <c r="A93" s="1" t="s">
+    <row r="96" spans="1:10">
+      <c r="A96" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B96" s="2">
         <v>5.9</v>
       </c>
-      <c r="C93" s="1">
-        <v>1</v>
-      </c>
-      <c r="D93" s="2">
-        <f>C93*B93</f>
+      <c r="C96" s="1">
+        <v>1</v>
+      </c>
+      <c r="D96" s="2">
+        <f t="shared" ref="D96:D103" si="4">C96*B96</f>
         <v>5.9</v>
       </c>
-      <c r="E93" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G93" s="2" t="s">
+      <c r="E96" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G96" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
-      <c r="A94" s="1" t="s">
+    <row r="97" spans="1:10">
+      <c r="A97" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B97" s="2">
         <v>16.71</v>
       </c>
-      <c r="C94" s="1">
-        <v>1</v>
-      </c>
-      <c r="D94" s="2">
-        <f>C94*B94</f>
+      <c r="C97" s="1">
+        <v>1</v>
+      </c>
+      <c r="D97" s="2">
+        <f t="shared" si="4"/>
         <v>16.71</v>
       </c>
-      <c r="E94" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G94" s="2" t="s">
+      <c r="E97" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G97" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I94" s="1" t="s">
+      <c r="I97" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
-      <c r="A95" s="1" t="s">
+    <row r="98" spans="1:10">
+      <c r="A98" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B98" s="2">
         <v>5.2</v>
       </c>
-      <c r="C95" s="1">
+      <c r="C98" s="1">
         <v>2</v>
       </c>
-      <c r="D95" s="2">
-        <f>C95*B95</f>
+      <c r="D98" s="2">
+        <f t="shared" si="4"/>
         <v>10.4</v>
       </c>
-      <c r="E95" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G95" s="2" t="s">
+      <c r="E98" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G98" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I95" s="1" t="s">
+      <c r="I98" s="1" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" s="22" customFormat="1">
-      <c r="A96" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B96" s="23">
-        <v>8.43</v>
-      </c>
-      <c r="C96" s="22">
-        <v>0</v>
-      </c>
-      <c r="D96" s="23">
-        <f>C96*B96</f>
-        <v>0</v>
-      </c>
-      <c r="E96" s="23"/>
-      <c r="F96" s="23"/>
-      <c r="G96" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="H96" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="I96" s="22" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" s="22" customFormat="1">
-      <c r="A97" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="B97" s="23">
-        <v>5.84</v>
-      </c>
-      <c r="C97" s="22">
-        <v>0</v>
-      </c>
-      <c r="D97" s="23">
-        <f>C97*B97</f>
-        <v>0</v>
-      </c>
-      <c r="E97" s="23"/>
-      <c r="F97" s="23"/>
-      <c r="G97" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="H97" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="I97" s="22" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" s="22" customFormat="1">
-      <c r="A98" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B98" s="23">
-        <v>9.5</v>
-      </c>
-      <c r="C98" s="22">
-        <v>2</v>
-      </c>
-      <c r="D98" s="23">
-        <f>C98*B98</f>
-        <v>19</v>
-      </c>
-      <c r="E98" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F98" s="23"/>
-      <c r="G98" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="H98" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="I98" s="22" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="99" spans="1:10" s="22" customFormat="1">
@@ -3141,339 +3219,416 @@
         <v>135</v>
       </c>
       <c r="B99" s="23">
-        <v>5.26</v>
+        <v>8.43</v>
       </c>
       <c r="C99" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D99" s="23">
-        <f>C99*B99</f>
-        <v>5.26</v>
-      </c>
-      <c r="E99" s="23" t="s">
-        <v>43</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E99" s="23"/>
       <c r="F99" s="23"/>
       <c r="G99" s="23" t="s">
         <v>137</v>
       </c>
       <c r="H99" s="23" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="I99" s="22" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="100" spans="1:10" s="22" customFormat="1">
       <c r="A100" s="22" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B100" s="23">
-        <v>3.72</v>
+        <v>5.84</v>
       </c>
       <c r="C100" s="22">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D100" s="23">
-        <f>C100*B100</f>
-        <v>18.600000000000001</v>
-      </c>
-      <c r="E100" s="23" t="s">
-        <v>43</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E100" s="23"/>
       <c r="F100" s="23"/>
       <c r="G100" s="23" t="s">
         <v>137</v>
       </c>
       <c r="H100" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="I100" s="22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" s="22" customFormat="1">
+      <c r="A101" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B101" s="23">
+        <v>9.5</v>
+      </c>
+      <c r="C101" s="22">
+        <v>2</v>
+      </c>
+      <c r="D101" s="23">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="E101" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F101" s="23"/>
+      <c r="G101" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H101" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="I101" s="22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" s="22" customFormat="1">
+      <c r="A102" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B102" s="23">
+        <v>5.26</v>
+      </c>
+      <c r="C102" s="22">
+        <v>1</v>
+      </c>
+      <c r="D102" s="23">
+        <f t="shared" si="4"/>
+        <v>5.26</v>
+      </c>
+      <c r="E102" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F102" s="23"/>
+      <c r="G102" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H102" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="I102" s="22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" s="22" customFormat="1">
+      <c r="A103" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="B103" s="23">
+        <v>3.72</v>
+      </c>
+      <c r="C103" s="22">
+        <v>5</v>
+      </c>
+      <c r="D103" s="23">
+        <f t="shared" si="4"/>
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E103" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F103" s="23"/>
+      <c r="G103" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H103" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="I100" s="22" t="s">
+      <c r="I103" s="22" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
-      <c r="A102" s="10"/>
-      <c r="C102" s="10" t="s">
+    <row r="105" spans="1:10">
+      <c r="A105" s="10"/>
+      <c r="C105" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D102" s="11">
-        <f>SUM(D87:D100)</f>
+      <c r="D105" s="11">
+        <f>SUM(D90:D103)</f>
         <v>344.55999999999995</v>
       </c>
-      <c r="I102" s="15"/>
-    </row>
-    <row r="103" spans="1:10">
-      <c r="A103" s="20"/>
-      <c r="B103" s="21"/>
-      <c r="C103" s="20"/>
-      <c r="D103" s="21"/>
-      <c r="E103" s="21"/>
-      <c r="F103" s="21"/>
-      <c r="G103" s="21"/>
-      <c r="H103" s="21"/>
-      <c r="I103" s="20"/>
-    </row>
-    <row r="104" spans="1:10" ht="20">
-      <c r="A104" s="5" t="s">
+      <c r="I105" s="15"/>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106" s="20"/>
+      <c r="B106" s="21"/>
+      <c r="C106" s="20"/>
+      <c r="D106" s="21"/>
+      <c r="E106" s="21"/>
+      <c r="F106" s="21"/>
+      <c r="G106" s="21"/>
+      <c r="H106" s="21"/>
+      <c r="I106" s="20"/>
+    </row>
+    <row r="107" spans="1:10" ht="20">
+      <c r="A107" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
-      <c r="A105" s="17" t="s">
+    <row r="108" spans="1:10">
+      <c r="A108" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B105" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C105" s="17" t="s">
+      <c r="B108" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D105" s="18" t="s">
+      <c r="D108" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E105" s="18" t="s">
+      <c r="E108" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F105" s="18" t="s">
+      <c r="F108" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="G105" s="18" t="s">
+      <c r="G108" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H105" s="18" t="s">
+      <c r="H108" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I105" s="17" t="s">
+      <c r="I108" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J105" s="19"/>
-    </row>
-    <row r="106" spans="1:10">
-      <c r="A106" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B106" s="2">
-        <v>0</v>
-      </c>
-      <c r="C106" s="1">
-        <v>1</v>
-      </c>
-      <c r="D106" s="2">
-        <v>0</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G106" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H106" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10">
-      <c r="A107" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B107" s="2">
-        <v>0</v>
-      </c>
-      <c r="C107" s="1">
-        <v>1</v>
-      </c>
-      <c r="D107" s="2">
-        <v>0</v>
-      </c>
-      <c r="E107" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G107" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H107" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J107" s="15"/>
-    </row>
-    <row r="108" spans="1:10" s="22" customFormat="1">
-      <c r="A108" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="B108" s="23">
-        <v>149.99</v>
-      </c>
-      <c r="C108" s="22">
-        <v>1</v>
-      </c>
-      <c r="D108" s="23">
-        <f>C108*B108</f>
-        <v>149.99</v>
-      </c>
-      <c r="E108" s="23"/>
-      <c r="F108" s="23"/>
-      <c r="G108" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H108" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="I108" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="J108" s="24"/>
+      <c r="J108" s="19"/>
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="1" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B109" s="2">
-        <v>28.75</v>
+        <v>0</v>
       </c>
       <c r="C109" s="1">
         <v>1</v>
       </c>
       <c r="D109" s="2">
-        <f>C109*B109</f>
-        <v>28.75</v>
+        <v>0</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="G109" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="A110" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B110" s="2">
+        <v>0</v>
+      </c>
+      <c r="C110" s="1">
+        <v>1</v>
+      </c>
+      <c r="D110" s="2">
+        <v>0</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J110" s="15"/>
+    </row>
+    <row r="111" spans="1:10" s="22" customFormat="1">
+      <c r="A111" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="B111" s="23">
+        <v>149.99</v>
+      </c>
+      <c r="C111" s="22">
+        <v>1</v>
+      </c>
+      <c r="D111" s="23">
+        <f>C111*B111</f>
+        <v>149.99</v>
+      </c>
+      <c r="E111" s="23"/>
+      <c r="F111" s="23"/>
+      <c r="G111" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="H109" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I109" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" s="22" customFormat="1">
-      <c r="A110" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="B110" s="23">
-        <v>8.99</v>
-      </c>
-      <c r="C110" s="22">
-        <v>1</v>
-      </c>
-      <c r="D110" s="23">
-        <f>C110*B110</f>
-        <v>8.99</v>
-      </c>
-      <c r="E110" s="23"/>
-      <c r="F110" s="23"/>
-      <c r="G110" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H110" s="23"/>
-      <c r="I110" s="22" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" s="19" customFormat="1">
-      <c r="A111" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B111" s="2">
-        <v>0</v>
-      </c>
-      <c r="C111" s="1">
-        <v>2</v>
-      </c>
-      <c r="D111" s="2">
-        <v>0</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F111" s="2"/>
-      <c r="G111" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H111" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I111" s="1"/>
-      <c r="J111" s="1"/>
+      <c r="I111" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="J111" s="24"/>
     </row>
     <row r="112" spans="1:10">
       <c r="A112" s="1" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="B112" s="2">
+        <v>28.75</v>
+      </c>
+      <c r="C112" s="1">
+        <v>1</v>
+      </c>
+      <c r="D112" s="2">
+        <f>C112*B112</f>
+        <v>28.75</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" s="22" customFormat="1">
+      <c r="A113" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="B113" s="23">
+        <v>8.99</v>
+      </c>
+      <c r="C113" s="22">
+        <v>1</v>
+      </c>
+      <c r="D113" s="23">
+        <f>C113*B113</f>
+        <v>8.99</v>
+      </c>
+      <c r="E113" s="23"/>
+      <c r="F113" s="23"/>
+      <c r="G113" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="H113" s="23"/>
+      <c r="I113" s="22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" s="19" customFormat="1">
+      <c r="A114" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B114" s="2">
         <v>0</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C114" s="1">
         <v>2</v>
       </c>
-      <c r="D112" s="2">
+      <c r="D114" s="2">
         <v>0</v>
       </c>
-      <c r="E112" s="2" t="s">
+      <c r="E114" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G112" s="2" t="s">
+      <c r="F114" s="2"/>
+      <c r="G114" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H112" s="2" t="s">
+      <c r="H114" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="113" spans="1:10">
-      <c r="A113" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B113" s="2">
-        <v>9</v>
-      </c>
-      <c r="C113" s="1">
-        <v>1</v>
-      </c>
-      <c r="D113" s="2">
-        <f>C113*B113</f>
-        <v>9</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G113" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" s="15" customFormat="1">
-      <c r="A114" s="1"/>
-      <c r="B114" s="2"/>
-      <c r="C114" s="1"/>
-      <c r="D114" s="2"/>
-      <c r="E114" s="2"/>
-      <c r="F114" s="2"/>
-      <c r="G114" s="2"/>
-      <c r="H114" s="2"/>
       <c r="I114" s="1"/>
       <c r="J114" s="1"/>
     </row>
     <row r="115" spans="1:10">
-      <c r="C115" s="10" t="s">
+      <c r="A115" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B115" s="2">
+        <v>0</v>
+      </c>
+      <c r="C115" s="1">
+        <v>2</v>
+      </c>
+      <c r="D115" s="2">
+        <v>0</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B116" s="2">
+        <v>9</v>
+      </c>
+      <c r="C116" s="1">
+        <v>1</v>
+      </c>
+      <c r="D116" s="2">
+        <f>C116*B116</f>
+        <v>9</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" s="15" customFormat="1">
+      <c r="A117" s="1"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="1"/>
+      <c r="J117" s="1"/>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="C118" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D115" s="11">
-        <f>SUM(D106:D112)</f>
+      <c r="D118" s="11">
+        <f>SUM(D109:D115)</f>
         <v>187.73000000000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More budget updates, new parts
</commit_message>
<xml_diff>
--- a/DetailedBudget.xlsx
+++ b/DetailedBudget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40260" yWindow="540" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="7240" yWindow="0" windowWidth="28560" windowHeight="19700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="172">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Screws</t>
   </si>
   <si>
-    <t>Tubing</t>
-  </si>
-  <si>
     <t>WHITE NOISE BOUTIQUE: DETAILED BUDGET</t>
   </si>
   <si>
@@ -315,9 +312,6 @@
     <t>Air pump (as vacuum)</t>
   </si>
   <si>
-    <t>Jar/tupperware for swarf</t>
-  </si>
-  <si>
     <t>http://www.amazon.com/Tetra-77854-Whisper-Pump-Gallon/dp/B0009YJ4NG/ref=zg_bs_2975471011_3</t>
   </si>
   <si>
@@ -429,27 +423,12 @@
     <t>Drill bushing (for center holes)</t>
   </si>
   <si>
-    <t>7.3mm</t>
-  </si>
-  <si>
     <t>McMaster Carr</t>
   </si>
   <si>
     <t>9/32"</t>
   </si>
   <si>
-    <t>Drill rod (for center holes)</t>
-  </si>
-  <si>
-    <t>7.3mm, 4.25" long</t>
-  </si>
-  <si>
-    <t>http://www.mcmaster.com/#2900a351/=ygxi4p</t>
-  </si>
-  <si>
-    <t>http://www.mcmaster.com/#8486a41/=ygxihl</t>
-  </si>
-  <si>
     <t>http://www.mcmaster.com/#8491a296/=ygximw</t>
   </si>
   <si>
@@ -514,6 +493,48 @@
   </si>
   <si>
     <t>Mouser</t>
+  </si>
+  <si>
+    <t>Lock&amp;Lock twist top container</t>
+  </si>
+  <si>
+    <t>Lock&amp;Lock</t>
+  </si>
+  <si>
+    <t>http://shop.locknlock-usa.com/home/213-twist-top-round-food-container-32-cups-256-oz.html</t>
+  </si>
+  <si>
+    <t>3/16" ID tubing</t>
+  </si>
+  <si>
+    <t>Misc hardware (bolts, etc) for punch</t>
+  </si>
+  <si>
+    <t>Baby powder (for vacuum tubing)</t>
+  </si>
+  <si>
+    <t>Local store</t>
+  </si>
+  <si>
+    <t>12V power adapter (110-240V)</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>2.1mm DC barrel jack</t>
+  </si>
+  <si>
+    <t>Plastic enclosure</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/products/905</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/products/610</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/products/798</t>
   </si>
 </sst>
 </file>
@@ -597,7 +618,7 @@
       <name val="Open Sans"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -607,6 +628,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -892,7 +919,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -923,7 +950,9 @@
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="270">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1524,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J118"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1546,37 +1575,37 @@
   <sheetData>
     <row r="1" spans="1:9" ht="34">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="20">
       <c r="E2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:9" s="10" customFormat="1" ht="20">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6">
-        <f>D19+D29+D38+D48+D71+D78+D86+D105+D118</f>
-        <v>11757.788999999999</v>
+        <f>D19+D29+D38+D48+D75+D82+D90+D108+D121</f>
+        <v>11812.598999999998</v>
       </c>
       <c r="E3" s="7">
         <v>0.64</v>
       </c>
       <c r="F3" s="8">
         <f>D3*E3</f>
-        <v>7524.9849599999998</v>
+        <v>7560.0633599999992</v>
       </c>
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:9" ht="20">
       <c r="A4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="5"/>
@@ -1594,20 +1623,20 @@
     </row>
     <row r="5" spans="1:9" ht="20">
       <c r="A5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6">
         <f>D4-D3</f>
-        <v>742.21100000000115</v>
+        <v>687.40100000000166</v>
       </c>
       <c r="E5" s="7">
         <v>0.64</v>
       </c>
       <c r="F5" s="8">
         <f>D5*E5</f>
-        <v>475.01504000000074</v>
+        <v>439.93664000000109</v>
       </c>
       <c r="H5" s="9"/>
     </row>
@@ -1643,7 +1672,7 @@
     </row>
     <row r="9" spans="1:9" ht="20">
       <c r="A9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="19" customFormat="1">
@@ -1660,16 +1689,16 @@
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>90</v>
-      </c>
       <c r="G10" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>4</v>
@@ -1677,7 +1706,7 @@
     </row>
     <row r="11" spans="1:9" s="15" customFormat="1">
       <c r="A11" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2">
         <v>850</v>
@@ -1690,20 +1719,20 @@
         <v>850</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2">
         <v>100</v>
@@ -1718,7 +1747,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2">
         <v>600</v>
@@ -1733,7 +1762,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="2">
         <v>600</v>
@@ -1748,7 +1777,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B15" s="2">
         <v>2025</v>
@@ -1761,18 +1790,18 @@
         <v>2025</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2">
         <v>3000</v>
@@ -1787,7 +1816,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B17" s="2">
         <v>15</v>
@@ -1800,18 +1829,18 @@
         <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="C19" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="11">
         <f>SUM(D11:D17)</f>
@@ -1820,7 +1849,7 @@
     </row>
     <row r="21" spans="1:9" ht="20">
       <c r="A21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="19" customFormat="1">
@@ -1837,16 +1866,16 @@
         <v>3</v>
       </c>
       <c r="E22" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F22" s="18" t="s">
-        <v>90</v>
-      </c>
       <c r="G22" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I22" s="17" t="s">
         <v>4</v>
@@ -1854,7 +1883,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B23" s="2">
         <v>74.7</v>
@@ -1867,15 +1896,15 @@
         <v>1045.8</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2">
         <v>0</v>
@@ -1887,20 +1916,20 @@
         <v>0</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="2">
         <v>0</v>
@@ -1912,17 +1941,17 @@
         <v>0</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="C29" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="11">
         <f>SUM(D23:D27)</f>
@@ -1931,7 +1960,7 @@
     </row>
     <row r="31" spans="1:9" ht="20">
       <c r="A31" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -1956,16 +1985,16 @@
         <v>3</v>
       </c>
       <c r="E32" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F32" s="18" t="s">
-        <v>90</v>
-      </c>
       <c r="G32" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I32" s="17" t="s">
         <v>4</v>
@@ -1986,16 +2015,16 @@
         <v>12.9</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>7</v>
@@ -2003,7 +2032,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B34" s="2">
         <v>0.48</v>
@@ -2016,13 +2045,13 @@
         <v>2.88</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="22" customFormat="1">
@@ -2054,13 +2083,13 @@
         <v>30</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>9</v>
@@ -2068,7 +2097,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="C38" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D38" s="11">
         <f>SUM(D33:D36)</f>
@@ -2077,7 +2106,7 @@
     </row>
     <row r="40" spans="1:9" ht="20">
       <c r="A40" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="19" customFormat="1">
@@ -2094,16 +2123,16 @@
         <v>3</v>
       </c>
       <c r="E41" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F41" s="18" t="s">
-        <v>90</v>
-      </c>
       <c r="G41" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I41" s="17" t="s">
         <v>4</v>
@@ -2124,10 +2153,10 @@
         <v>400</v>
       </c>
       <c r="G42" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2145,7 +2174,7 @@
         <v>10</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="22" customFormat="1">
@@ -2165,13 +2194,13 @@
       <c r="E44" s="23"/>
       <c r="F44" s="23"/>
       <c r="G44" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H44" s="23"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B45" s="2">
         <v>0</v>
@@ -2183,12 +2212,12 @@
         <v>0</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="22" customFormat="1">
       <c r="A46" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B46" s="23">
         <v>40</v>
@@ -2207,7 +2236,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="C48" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D48" s="11">
         <f>SUM(D42:D46)</f>
@@ -2216,7 +2245,7 @@
     </row>
     <row r="50" spans="1:9" ht="20">
       <c r="A50" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="19" customFormat="1">
@@ -2233,16 +2262,16 @@
         <v>3</v>
       </c>
       <c r="E51" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F51" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F51" s="18" t="s">
-        <v>90</v>
-      </c>
       <c r="G51" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I51" s="17" t="s">
         <v>4</v>
@@ -2250,7 +2279,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B52" s="2">
         <v>1500</v>
@@ -2259,22 +2288,22 @@
         <v>1</v>
       </c>
       <c r="D52" s="2">
-        <f t="shared" ref="D52:D69" si="1">C52*B52</f>
+        <f t="shared" ref="D52:D73" si="1">C52*B52</f>
         <v>1500</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B53" s="2">
         <v>280</v>
@@ -2287,18 +2316,18 @@
         <v>280</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B54" s="2">
         <v>13</v>
@@ -2311,47 +2340,47 @@
         <v>13</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>98</v>
+        <v>158</v>
       </c>
       <c r="B55" s="2">
-        <v>0</v>
+        <v>6.99</v>
       </c>
       <c r="C55" s="1">
         <v>1</v>
       </c>
       <c r="D55" s="2">
-        <v>0</v>
+        <v>6.99</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>13</v>
+        <v>161</v>
       </c>
       <c r="B56" s="2">
         <v>6.24</v>
@@ -2364,18 +2393,18 @@
         <v>6.24</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B57" s="2">
         <v>2.36</v>
@@ -2388,21 +2417,21 @@
         <v>4.72</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B58" s="2">
         <f>1.94+2.29</f>
@@ -2416,18 +2445,18 @@
         <v>4.2300000000000004</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B59" s="2">
         <v>3.49</v>
@@ -2440,18 +2469,18 @@
         <v>3.49</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B60" s="2">
         <v>2.99</v>
@@ -2464,18 +2493,18 @@
         <v>5.98</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B61" s="2">
         <v>10</v>
@@ -2488,18 +2517,21 @@
         <v>30</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="22" customFormat="1">
       <c r="A62" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B62" s="23">
         <v>269</v>
@@ -2514,16 +2546,16 @@
       <c r="E62" s="23"/>
       <c r="F62" s="23"/>
       <c r="G62" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H62" s="23"/>
       <c r="I62" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B63" s="2">
         <v>0</v>
@@ -2536,21 +2568,21 @@
         <v>0</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="22" customFormat="1">
       <c r="A64" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B64" s="23">
         <v>14.95</v>
@@ -2563,22 +2595,22 @@
         <v>14.95</v>
       </c>
       <c r="E64" s="23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F64" s="23"/>
       <c r="G64" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="H64" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="I64" s="22" t="s">
         <v>128</v>
-      </c>
-      <c r="H64" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="I64" s="22" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B65" s="2">
         <v>10.57</v>
@@ -2591,21 +2623,21 @@
         <v>10.57</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B66" s="2">
         <v>9.9000000000000005E-2</v>
@@ -2618,21 +2650,21 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B67" s="2">
         <v>0.18</v>
@@ -2645,21 +2677,21 @@
         <v>0.72</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B68" s="2">
         <v>0.22</v>
@@ -2672,21 +2704,21 @@
         <v>0.22</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B69" s="2">
         <v>50</v>
@@ -2699,936 +2731,1031 @@
         <v>50</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G69" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I69" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
-      <c r="C71" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D71" s="11">
-        <f>SUM(D52:D69)</f>
-        <v>2193.2189999999996</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="20">
-      <c r="A73" s="5" t="s">
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B70" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+      <c r="D70" s="2">
+        <f t="shared" si="1"/>
+        <v>1.99</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" s="24" customFormat="1">
+      <c r="A71" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="B71" s="25">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="C71" s="24">
+        <v>1</v>
+      </c>
+      <c r="D71" s="25">
+        <f t="shared" si="1"/>
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="E71" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F71" s="25"/>
+      <c r="G71" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="H71" s="25"/>
+      <c r="I71" s="24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" s="24" customFormat="1">
+      <c r="A72" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="B72" s="25">
+        <v>2.95</v>
+      </c>
+      <c r="C72" s="24">
+        <v>3</v>
+      </c>
+      <c r="D72" s="25">
+        <f t="shared" si="1"/>
+        <v>8.8500000000000014</v>
+      </c>
+      <c r="E72" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F72" s="25"/>
+      <c r="G72" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="H72" s="25"/>
+      <c r="I72" s="24" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" s="24" customFormat="1">
+      <c r="A73" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="B73" s="25">
+        <v>19.95</v>
+      </c>
+      <c r="C73" s="24">
+        <v>1</v>
+      </c>
+      <c r="D73" s="25">
+        <f t="shared" si="1"/>
+        <v>19.95</v>
+      </c>
+      <c r="E73" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F73" s="25"/>
+      <c r="G73" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="H73" s="25"/>
+      <c r="I73" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="C75" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D75" s="11">
+        <f>SUM(D52:D73)</f>
+        <v>2239.9489999999992</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="20">
+      <c r="A77" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E78" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F78" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="G78" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H78" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I78" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J78" s="19"/>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B79" s="2">
+        <v>56.75</v>
+      </c>
+      <c r="C79" s="1">
+        <v>1</v>
+      </c>
+      <c r="D79" s="2">
+        <f>C79*B79</f>
+        <v>56.75</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B80" s="2">
+        <v>49</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1</v>
+      </c>
+      <c r="D80" s="2">
+        <f>C80*B80</f>
+        <v>49</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" s="19" customFormat="1">
+      <c r="A81" s="1"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="C82" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D82" s="11">
+        <f>SUM(D79:D80)</f>
+        <v>105.75</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="20">
+      <c r="A84" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
-      <c r="A74" s="17" t="s">
+    <row r="85" spans="1:10">
+      <c r="A85" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B74" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C74" s="17" t="s">
+      <c r="B85" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D74" s="18" t="s">
+      <c r="D85" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E74" s="18" t="s">
+      <c r="E85" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F85" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F74" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="G74" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H74" s="18" t="s">
+      <c r="G85" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H85" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I85" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J85" s="19"/>
+    </row>
+    <row r="86" spans="1:10" s="22" customFormat="1">
+      <c r="A86" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B86" s="23">
+        <v>50</v>
+      </c>
+      <c r="C86" s="22">
+        <v>1</v>
+      </c>
+      <c r="D86" s="23">
+        <f>C86*B86</f>
+        <v>50</v>
+      </c>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H86" s="23"/>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B87" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="C87" s="1">
+        <v>5</v>
+      </c>
+      <c r="D87" s="2">
+        <f>C87*B87</f>
+        <v>79.95</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B88" s="2">
+        <v>10</v>
+      </c>
+      <c r="C88" s="1">
+        <v>1</v>
+      </c>
+      <c r="D88" s="2">
+        <f>C88*B88</f>
+        <v>10</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" s="19" customFormat="1">
+      <c r="A90" s="1"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D90" s="11">
+        <f>SUM(D86:D88)</f>
+        <v>139.94999999999999</v>
+      </c>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+    </row>
+    <row r="92" spans="1:10" ht="20">
+      <c r="A92" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I74" s="17" t="s">
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D93" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E93" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F93" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="G93" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H93" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I93" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J74" s="19"/>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="2">
-        <v>56.75</v>
-      </c>
-      <c r="C75" s="1">
-        <v>1</v>
-      </c>
-      <c r="D75" s="2">
-        <f>C75*B75</f>
-        <v>56.75</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G75" s="2" t="s">
+      <c r="J93" s="19"/>
+    </row>
+    <row r="94" spans="1:10" s="24" customFormat="1">
+      <c r="A94" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B94" s="25">
+        <v>0.63</v>
+      </c>
+      <c r="C94" s="24">
+        <v>200</v>
+      </c>
+      <c r="D94" s="25">
+        <f>C94*B94</f>
+        <v>126</v>
+      </c>
+      <c r="E94" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F94" s="25"/>
+      <c r="G94" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="H94" s="25"/>
+      <c r="I94" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B95" s="2">
+        <v>7.27</v>
+      </c>
+      <c r="C95" s="1">
+        <v>2</v>
+      </c>
+      <c r="D95" s="2">
+        <f t="shared" ref="D95:D98" si="3">C95*B95</f>
+        <v>14.54</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G95" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I75" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
-      <c r="A76" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B76" s="2">
-        <v>49</v>
-      </c>
-      <c r="C76" s="1">
-        <v>1</v>
-      </c>
-      <c r="D76" s="2">
-        <f>C76*B76</f>
-        <v>49</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" s="19" customFormat="1">
-      <c r="A77" s="1"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-    </row>
-    <row r="78" spans="1:10">
-      <c r="C78" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D78" s="11">
-        <f>SUM(D75:D76)</f>
-        <v>105.75</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="20">
-      <c r="A80" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10">
-      <c r="A81" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B81" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C81" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D81" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E81" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F81" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="G81" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H81" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I81" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J81" s="19"/>
-    </row>
-    <row r="82" spans="1:10" s="22" customFormat="1">
-      <c r="A82" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="B82" s="23">
-        <v>50</v>
-      </c>
-      <c r="C82" s="22">
-        <v>1</v>
-      </c>
-      <c r="D82" s="23">
-        <f>C82*B82</f>
-        <v>50</v>
-      </c>
-      <c r="E82" s="23"/>
-      <c r="F82" s="23"/>
-      <c r="G82" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="H82" s="23"/>
-    </row>
-    <row r="83" spans="1:10">
-      <c r="A83" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B83" s="2">
-        <v>15.99</v>
-      </c>
-      <c r="C83" s="1">
-        <v>5</v>
-      </c>
-      <c r="D83" s="2">
-        <f>C83*B83</f>
-        <v>79.95</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10">
-      <c r="A84" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B84" s="2">
-        <v>10</v>
-      </c>
-      <c r="C84" s="1">
-        <v>1</v>
-      </c>
-      <c r="D84" s="2">
-        <f>C84*B84</f>
-        <v>10</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" s="19" customFormat="1">
-      <c r="A86" s="1"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D86" s="11">
-        <f>SUM(D82:D84)</f>
-        <v>139.94999999999999</v>
-      </c>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
-      <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="1"/>
-      <c r="J86" s="1"/>
-    </row>
-    <row r="88" spans="1:10" ht="20">
-      <c r="A88" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10">
-      <c r="A89" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B89" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C89" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D89" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E89" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F89" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="G89" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H89" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I89" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J89" s="19"/>
-    </row>
-    <row r="90" spans="1:10">
-      <c r="A90" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B90" s="2">
-        <v>0.63</v>
-      </c>
-      <c r="C90" s="1">
-        <v>200</v>
-      </c>
-      <c r="D90" s="2">
-        <f>C90*B90</f>
-        <v>126</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G90" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I90" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10">
-      <c r="A91" s="1" t="s">
+      <c r="I95" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B91" s="2">
-        <v>7.27</v>
-      </c>
-      <c r="C91" s="1">
-        <v>2</v>
-      </c>
-      <c r="D91" s="2">
-        <f t="shared" ref="D91:D94" si="3">C91*B91</f>
-        <v>14.54</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" s="19" customFormat="1">
-      <c r="A92" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B92" s="2">
+    </row>
+    <row r="96" spans="1:10" s="19" customFormat="1">
+      <c r="A96" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B96" s="2">
         <v>89.9</v>
       </c>
-      <c r="C92" s="1">
-        <v>1</v>
-      </c>
-      <c r="D92" s="2">
+      <c r="C96" s="1">
+        <v>1</v>
+      </c>
+      <c r="D96" s="2">
         <f t="shared" si="3"/>
         <v>89.9</v>
       </c>
-      <c r="E92" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G92" s="2" t="s">
+      <c r="E96" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I96" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H92" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J92" s="1"/>
-    </row>
-    <row r="93" spans="1:10">
-      <c r="A93" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B93" s="2">
+      <c r="J96" s="1"/>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B97" s="2">
         <v>6.45</v>
       </c>
-      <c r="C93" s="1">
+      <c r="C97" s="1">
         <v>3</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D97" s="2">
         <f t="shared" si="3"/>
         <v>19.350000000000001</v>
       </c>
-      <c r="E93" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G93" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I93" s="1" t="s">
+      <c r="E97" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="94" spans="1:10">
-      <c r="A94" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B94" s="2">
+      <c r="B98" s="2">
         <f>18.95+4.95-5</f>
         <v>18.899999999999999</v>
       </c>
-      <c r="C94" s="1">
-        <v>1</v>
-      </c>
-      <c r="D94" s="2">
+      <c r="C98" s="1">
+        <v>1</v>
+      </c>
+      <c r="D98" s="2">
         <f t="shared" si="3"/>
         <v>18.899999999999999</v>
       </c>
-      <c r="E94" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G94" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H94" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="I94" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" s="22" customFormat="1">
-      <c r="A95" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="B95" s="23"/>
-      <c r="D95" s="23"/>
-      <c r="E95" s="23"/>
-      <c r="F95" s="23"/>
-      <c r="G95" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="H95" s="23"/>
-      <c r="I95" s="22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10">
-      <c r="A96" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B96" s="2">
-        <v>5.9</v>
-      </c>
-      <c r="C96" s="1">
-        <v>1</v>
-      </c>
-      <c r="D96" s="2">
-        <f t="shared" ref="D96:D103" si="4">C96*B96</f>
-        <v>5.9</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10">
-      <c r="A97" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B97" s="2">
-        <v>16.71</v>
-      </c>
-      <c r="C97" s="1">
-        <v>1</v>
-      </c>
-      <c r="D97" s="2">
-        <f t="shared" si="4"/>
-        <v>16.71</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10">
-      <c r="A98" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B98" s="2">
-        <v>5.2</v>
-      </c>
-      <c r="C98" s="1">
-        <v>2</v>
-      </c>
-      <c r="D98" s="2">
-        <f t="shared" si="4"/>
-        <v>10.4</v>
-      </c>
       <c r="E98" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>53</v>
+        <v>76</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="99" spans="1:10" s="22" customFormat="1">
       <c r="A99" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B99" s="23">
-        <v>8.43</v>
-      </c>
-      <c r="C99" s="22">
-        <v>0</v>
-      </c>
-      <c r="D99" s="23">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="B99" s="23"/>
+      <c r="D99" s="23"/>
       <c r="E99" s="23"/>
       <c r="F99" s="23"/>
       <c r="G99" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="H99" s="23" t="s">
-        <v>136</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H99" s="23"/>
       <c r="I99" s="22" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" s="22" customFormat="1">
-      <c r="A100" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="B100" s="23">
-        <v>5.84</v>
-      </c>
-      <c r="C100" s="22">
-        <v>0</v>
-      </c>
-      <c r="D100" s="23">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B100" s="2">
+        <v>5.9</v>
+      </c>
+      <c r="C100" s="1">
+        <v>1</v>
+      </c>
+      <c r="D100" s="2">
+        <f t="shared" ref="D100:D106" si="4">C100*B100</f>
+        <v>5.9</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B101" s="2">
+        <v>16.71</v>
+      </c>
+      <c r="C101" s="1">
+        <v>1</v>
+      </c>
+      <c r="D101" s="2">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E100" s="23"/>
-      <c r="F100" s="23"/>
-      <c r="G100" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="H100" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="I100" s="22" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" s="22" customFormat="1">
-      <c r="A101" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B101" s="23">
+        <v>16.71</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B102" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="C102" s="1">
+        <v>2</v>
+      </c>
+      <c r="D102" s="2">
+        <f t="shared" si="4"/>
+        <v>10.4</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B103" s="2">
         <v>9.5</v>
       </c>
-      <c r="C101" s="22">
+      <c r="C103" s="1">
         <v>2</v>
       </c>
-      <c r="D101" s="23">
+      <c r="D103" s="2">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="E101" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F101" s="23"/>
-      <c r="G101" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="H101" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="I101" s="22" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" s="22" customFormat="1">
-      <c r="A102" s="22" t="s">
+      <c r="E103" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H103" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B102" s="23">
+      <c r="I103" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B104" s="2">
         <v>5.26</v>
       </c>
-      <c r="C102" s="22">
-        <v>1</v>
-      </c>
-      <c r="D102" s="23">
+      <c r="C104" s="1">
+        <v>1</v>
+      </c>
+      <c r="D104" s="2">
         <f t="shared" si="4"/>
         <v>5.26</v>
       </c>
-      <c r="E102" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F102" s="23"/>
-      <c r="G102" s="23" t="s">
+      <c r="E104" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H104" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H102" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="I102" s="22" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" s="22" customFormat="1">
-      <c r="A103" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="B103" s="23">
+      <c r="I104" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B105" s="2">
         <v>3.72</v>
       </c>
-      <c r="C103" s="22">
+      <c r="C105" s="1">
         <v>5</v>
       </c>
-      <c r="D103" s="23">
+      <c r="D105" s="2">
         <f t="shared" si="4"/>
         <v>18.600000000000001</v>
       </c>
-      <c r="E103" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F103" s="23"/>
-      <c r="G103" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="H103" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="I103" s="22" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10">
-      <c r="A105" s="10"/>
-      <c r="C105" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D105" s="11">
-        <f>SUM(D90:D103)</f>
-        <v>344.55999999999995</v>
-      </c>
-      <c r="I105" s="15"/>
+      <c r="E105" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="106" spans="1:10">
-      <c r="A106" s="20"/>
-      <c r="B106" s="21"/>
-      <c r="C106" s="20"/>
-      <c r="D106" s="21"/>
-      <c r="E106" s="21"/>
-      <c r="F106" s="21"/>
-      <c r="G106" s="21"/>
-      <c r="H106" s="21"/>
-      <c r="I106" s="20"/>
-    </row>
-    <row r="107" spans="1:10" ht="20">
-      <c r="A107" s="5" t="s">
-        <v>70</v>
+      <c r="A106" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B106" s="2">
+        <v>8.08</v>
+      </c>
+      <c r="C106" s="1">
+        <v>1</v>
+      </c>
+      <c r="D106" s="2">
+        <f t="shared" si="4"/>
+        <v>8.08</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="108" spans="1:10">
-      <c r="A108" s="17" t="s">
+      <c r="A108" s="10"/>
+      <c r="C108" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D108" s="11">
+        <f>SUM(D94:D106)</f>
+        <v>352.63999999999993</v>
+      </c>
+      <c r="I108" s="15"/>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="20"/>
+      <c r="B109" s="21"/>
+      <c r="C109" s="20"/>
+      <c r="D109" s="21"/>
+      <c r="E109" s="21"/>
+      <c r="F109" s="21"/>
+      <c r="G109" s="21"/>
+      <c r="H109" s="21"/>
+      <c r="I109" s="20"/>
+    </row>
+    <row r="110" spans="1:10" ht="20">
+      <c r="A110" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B108" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C108" s="17" t="s">
+      <c r="B111" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C111" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D108" s="18" t="s">
+      <c r="D111" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E108" s="18" t="s">
+      <c r="E111" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F111" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F108" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="G108" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H108" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I108" s="17" t="s">
+      <c r="G111" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H111" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I111" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J108" s="19"/>
-    </row>
-    <row r="109" spans="1:10">
-      <c r="A109" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B109" s="2">
-        <v>0</v>
-      </c>
-      <c r="C109" s="1">
-        <v>1</v>
-      </c>
-      <c r="D109" s="2">
-        <v>0</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G109" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H109" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10">
-      <c r="A110" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B110" s="2">
-        <v>0</v>
-      </c>
-      <c r="C110" s="1">
-        <v>1</v>
-      </c>
-      <c r="D110" s="2">
-        <v>0</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G110" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H110" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J110" s="15"/>
-    </row>
-    <row r="111" spans="1:10" s="22" customFormat="1">
-      <c r="A111" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="B111" s="23">
-        <v>149.99</v>
-      </c>
-      <c r="C111" s="22">
-        <v>1</v>
-      </c>
-      <c r="D111" s="23">
-        <f>C111*B111</f>
-        <v>149.99</v>
-      </c>
-      <c r="E111" s="23"/>
-      <c r="F111" s="23"/>
-      <c r="G111" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="I111" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="J111" s="24"/>
+      <c r="J111" s="19"/>
     </row>
     <row r="112" spans="1:10">
       <c r="A112" s="1" t="s">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="B112" s="2">
-        <v>28.75</v>
+        <v>0</v>
       </c>
       <c r="C112" s="1">
         <v>1</v>
       </c>
       <c r="D112" s="2">
-        <f>C112*B112</f>
-        <v>28.75</v>
+        <v>0</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>53</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I112" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" s="22" customFormat="1">
-      <c r="A113" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="B113" s="23">
-        <v>8.99</v>
-      </c>
-      <c r="C113" s="22">
-        <v>1</v>
-      </c>
-      <c r="D113" s="23">
-        <f>C113*B113</f>
-        <v>8.99</v>
-      </c>
-      <c r="E113" s="23"/>
-      <c r="F113" s="23"/>
-      <c r="G113" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B113" s="2">
+        <v>0</v>
+      </c>
+      <c r="C113" s="1">
+        <v>1</v>
+      </c>
+      <c r="D113" s="2">
+        <v>0</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F113" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H113" s="23"/>
-      <c r="I113" s="22" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" s="19" customFormat="1">
-      <c r="A114" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B114" s="2">
-        <v>0</v>
-      </c>
-      <c r="C114" s="1">
-        <v>2</v>
-      </c>
-      <c r="D114" s="2">
-        <v>0</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F114" s="2"/>
-      <c r="G114" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H114" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I114" s="1"/>
-      <c r="J114" s="1"/>
+      <c r="G113" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J113" s="15"/>
+    </row>
+    <row r="114" spans="1:10" s="24" customFormat="1">
+      <c r="A114" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="B114" s="25">
+        <v>149.99</v>
+      </c>
+      <c r="C114" s="24">
+        <v>1</v>
+      </c>
+      <c r="D114" s="25">
+        <f>C114*B114</f>
+        <v>149.99</v>
+      </c>
+      <c r="E114" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F114" s="25"/>
+      <c r="G114" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="I114" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="J114" s="26"/>
     </row>
     <row r="115" spans="1:10">
       <c r="A115" s="1" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B115" s="2">
+        <v>28.75</v>
+      </c>
+      <c r="C115" s="1">
+        <v>1</v>
+      </c>
+      <c r="D115" s="2">
+        <f>C115*B115</f>
+        <v>28.75</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" s="24" customFormat="1">
+      <c r="A116" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="B116" s="25">
+        <v>8.99</v>
+      </c>
+      <c r="C116" s="24">
+        <v>1</v>
+      </c>
+      <c r="D116" s="25">
+        <f>C116*B116</f>
+        <v>8.99</v>
+      </c>
+      <c r="E116" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F116" s="25"/>
+      <c r="G116" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="H116" s="25"/>
+      <c r="I116" s="24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" s="19" customFormat="1">
+      <c r="A117" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B117" s="2">
         <v>0</v>
       </c>
-      <c r="C115" s="1">
+      <c r="C117" s="1">
         <v>2</v>
       </c>
-      <c r="D115" s="2">
+      <c r="D117" s="2">
         <v>0</v>
       </c>
-      <c r="E115" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G115" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H115" s="2" t="s">
+      <c r="E117" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="116" spans="1:10">
-      <c r="A116" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B116" s="2">
-        <v>9</v>
-      </c>
-      <c r="C116" s="1">
-        <v>1</v>
-      </c>
-      <c r="D116" s="2">
-        <f>C116*B116</f>
-        <v>9</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G116" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" s="15" customFormat="1">
-      <c r="A117" s="1"/>
-      <c r="B117" s="2"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="2"/>
-      <c r="F117" s="2"/>
-      <c r="G117" s="2"/>
-      <c r="H117" s="2"/>
+      <c r="H117" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="I117" s="1"/>
       <c r="J117" s="1"/>
     </row>
     <row r="118" spans="1:10">
-      <c r="C118" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D118" s="11">
-        <f>SUM(D109:D115)</f>
+      <c r="A118" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B118" s="2">
+        <v>0</v>
+      </c>
+      <c r="C118" s="1">
+        <v>2</v>
+      </c>
+      <c r="D118" s="2">
+        <v>0</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B119" s="2">
+        <v>9</v>
+      </c>
+      <c r="C119" s="1">
+        <v>1</v>
+      </c>
+      <c r="D119" s="2">
+        <f>C119*B119</f>
+        <v>9</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" s="15" customFormat="1">
+      <c r="A120" s="1"/>
+      <c r="B120" s="2"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
+      <c r="I120" s="1"/>
+      <c r="J120" s="1"/>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="C121" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D121" s="11">
+        <f>SUM(D112:D118)</f>
         <v>187.73000000000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Most everything is here
</commit_message>
<xml_diff>
--- a/DetailedBudget.xlsx
+++ b/DetailedBudget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="0" windowWidth="28560" windowHeight="19700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="190">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Casino-quality dice (stick of 5, amber color)</t>
   </si>
   <si>
-    <t>Dice cup?</t>
-  </si>
-  <si>
     <t>http://www.amazon.com/Precision-Casino-Matching-Numbers-Brybelly/dp/B005JEA7UU/ref=sr_1_2?ie=UTF8&amp;qid=1436456271&amp;sr=8-2&amp;keywords=casino+dice</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>Wood glue</t>
   </si>
   <si>
-    <t>Screws</t>
-  </si>
-  <si>
     <t>WHITE NOISE BOUTIQUE: DETAILED BUDGET</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>Vinyl cutting lathe (without cutting head)</t>
   </si>
   <si>
-    <t>Amplifier</t>
-  </si>
-  <si>
     <t>Cutting head</t>
   </si>
   <si>
@@ -195,9 +186,6 @@
     <t>Hand and power tools</t>
   </si>
   <si>
-    <t>Shipped or borrowed</t>
-  </si>
-  <si>
     <t>Local lumberyard</t>
   </si>
   <si>
@@ -237,9 +225,6 @@
     <t>1and1</t>
   </si>
   <si>
-    <t>Stools</t>
-  </si>
-  <si>
     <t>Dorado Packaging</t>
   </si>
   <si>
@@ -258,24 +243,12 @@
     <t>Tamper-resistant stickers (1800 labels)</t>
   </si>
   <si>
-    <t>ePlastics</t>
-  </si>
-  <si>
-    <t>http://www.eplastics.com/Acetate_Film</t>
-  </si>
-  <si>
     <t>Use coupon code R1783494DE</t>
   </si>
   <si>
     <t>Through Stevens</t>
   </si>
   <si>
-    <t>Pelican case</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/Pelican-0340-Cube-Camera-Black/dp/B004AICE5C/ref=sr_1_1?ie=UTF8&amp;qid=1437055202&amp;sr=8-1&amp;keywords=0340+Cube+Case</t>
-  </si>
-  <si>
     <t>Felt for dice tray</t>
   </si>
   <si>
@@ -360,9 +333,6 @@
     <t>2 elbows for jar</t>
   </si>
   <si>
-    <t>Clear re-sealable bags (pack of 100)</t>
-  </si>
-  <si>
     <t>http://www.amazon.com/gp/product/B003XX91V0?redirect=true&amp;ref_=pd_hud_ysc_orders</t>
   </si>
   <si>
@@ -402,12 +372,6 @@
     <t>Canakit</t>
   </si>
   <si>
-    <t>(or use my small 10W)</t>
-  </si>
-  <si>
-    <t>http://www.canakit.com/0-5w-universal-mini-amplifier-kit-ck026-uk026.html</t>
-  </si>
-  <si>
     <t>VU meter (500uA, 700ohm)</t>
   </si>
   <si>
@@ -438,9 +402,6 @@
     <t>http://www.mcmaster.com/#3009a129/=ygxisk</t>
   </si>
   <si>
-    <t>Gum rubber vacuum tubing (priced per foot)</t>
-  </si>
-  <si>
     <t>3/16" ID, 1/8" wall</t>
   </si>
   <si>
@@ -456,9 +417,6 @@
     <t>Focusrite Scarlett 2i2 portable audio interface</t>
   </si>
   <si>
-    <t>Acetate film for cutting records</t>
-  </si>
-  <si>
     <t>http://www.amazon.com/gp/product/B005OZE9SA/ref=ox_sc_imb_mini_detail?ie=UTF8&amp;psc=1&amp;smid=ATVPDKIKX0DER</t>
   </si>
   <si>
@@ -535,6 +493,102 @@
   </si>
   <si>
     <t>https://www.adafruit.com/products/798</t>
+  </si>
+  <si>
+    <t>Nylon Y-fitting (pack of 10)</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#5463k721/=yk0tey</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#5546k44/=yk0tqn</t>
+  </si>
+  <si>
+    <t>3/16" ID, 1/16" wall</t>
+  </si>
+  <si>
+    <t>Shaft collar (for spring)</t>
+  </si>
+  <si>
+    <t>5/16" ID, aluminum</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#6157k32/=yk0ste</t>
+  </si>
+  <si>
+    <t>Gum rubber tubing (priced per foot)</t>
+  </si>
+  <si>
+    <t>Gum rubber vacuum tubing (priced per foot) - TOO LARGE</t>
+  </si>
+  <si>
+    <t>Nylon L fitting (pack of 10)</t>
+  </si>
+  <si>
+    <t>3/16" tube to 1/4" male pipe thread</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#2808k52/=yk0st8</t>
+  </si>
+  <si>
+    <t>Approx for now</t>
+  </si>
+  <si>
+    <t>Borrowed</t>
+  </si>
+  <si>
+    <t>10W amplifier</t>
+  </si>
+  <si>
+    <t>http://www.canakit.com/10w-audio-amplifier-kit-ck003-uk003.html</t>
+  </si>
+  <si>
+    <t>Trim-head screws</t>
+  </si>
+  <si>
+    <t>#6 x 2.25", uses #1 square bit</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#91520a160/=yk118o</t>
+  </si>
+  <si>
+    <t>Clear bags (pack of 100)</t>
+  </si>
+  <si>
+    <t>Replacement labels for above (same size, 100 sheets @ 6 per)</t>
+  </si>
+  <si>
+    <t>Acetate sheets (0.01 x 25 x 40")</t>
+  </si>
+  <si>
+    <t>Dick Blick</t>
+  </si>
+  <si>
+    <t>http://www.dickblick.com/products/grafix-clear-acetate-sheets-and-pads/#items</t>
+  </si>
+  <si>
+    <t>WiFi access</t>
+  </si>
+  <si>
+    <t>Paint</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Pelican-1650-Case-Camera-Black/dp/B002E6R7NG/ref=pd_sim_421_5?ie=UTF8&amp;refRID=0NF7WZB5Z45CS8AYB1T6</t>
+  </si>
+  <si>
+    <t>Pelican 1650 case with foam (28.5 x 17.37 x 10.5" interior)</t>
+  </si>
+  <si>
+    <t>Olfa perforation cutter</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Olfa-194B-OLFA-perforation-cutter/dp/B001GLP39A/ref=sr_1_1?rps=1&amp;ie=UTF8&amp;qid=1440373758&amp;sr=8-1&amp;keywords=OLFA+perforation+cutter+28&amp;refinements=p_85%3A2470955011</t>
+  </si>
+  <si>
+    <t>60mm LED rings (for microscope, 2x)</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/gp/product/B007Q946RQ/ref=ox_sc_act_title_3?ie=UTF8&amp;psc=1&amp;smid=A1THAZDOWP300U</t>
   </si>
 </sst>
 </file>
@@ -647,9 +701,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="270">
+  <cellStyleXfs count="294">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -952,9 +1030,11 @@
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="270">
+  <cellStyles count="294">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1090,6 +1170,18 @@
     <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="291" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="293" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1224,6 +1316,18 @@
     <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="274" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="276" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="278" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="282" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="284" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="286" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="288" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="290" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="292" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1553,15 +1657,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J121"/>
+  <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="42.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="2" customWidth="1"/>
@@ -1575,37 +1679,37 @@
   <sheetData>
     <row r="1" spans="1:9" ht="34">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="20">
       <c r="E2" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:9" s="10" customFormat="1" ht="20">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6">
-        <f>D19+D29+D38+D48+D75+D82+D90+D108+D121</f>
-        <v>11812.598999999998</v>
+        <f>D19+D31+D39+D48+D80+D87+D95+D114+D128</f>
+        <v>12455.179</v>
       </c>
       <c r="E3" s="7">
         <v>0.64</v>
       </c>
       <c r="F3" s="8">
         <f>D3*E3</f>
-        <v>7560.0633599999992</v>
+        <v>7971.3145599999998</v>
       </c>
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:9" ht="20">
       <c r="A4" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="5"/>
@@ -1623,20 +1727,20 @@
     </row>
     <row r="5" spans="1:9" ht="20">
       <c r="A5" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6">
         <f>D4-D3</f>
-        <v>687.40100000000166</v>
+        <v>44.820999999999913</v>
       </c>
       <c r="E5" s="7">
         <v>0.64</v>
       </c>
       <c r="F5" s="8">
         <f>D5*E5</f>
-        <v>439.93664000000109</v>
+        <v>28.685439999999943</v>
       </c>
       <c r="H5" s="9"/>
     </row>
@@ -1672,7 +1776,7 @@
     </row>
     <row r="9" spans="1:9" ht="20">
       <c r="A9" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="19" customFormat="1">
@@ -1689,16 +1793,16 @@
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>4</v>
@@ -1706,7 +1810,7 @@
     </row>
     <row r="11" spans="1:9" s="15" customFormat="1">
       <c r="A11" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2">
         <v>850</v>
@@ -1719,20 +1823,20 @@
         <v>850</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2">
         <v>100</v>
@@ -1747,7 +1851,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2">
         <v>600</v>
@@ -1762,7 +1866,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2">
         <v>600</v>
@@ -1777,7 +1881,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="15" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B15" s="2">
         <v>2025</v>
@@ -1790,18 +1894,18 @@
         <v>2025</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2">
         <v>3000</v>
@@ -1813,10 +1917,16 @@
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
+      <c r="E16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="15" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B17" s="2">
         <v>15</v>
@@ -1829,18 +1939,18 @@
         <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="C19" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D19" s="11">
         <f>SUM(D11:D17)</f>
@@ -1849,7 +1959,7 @@
     </row>
     <row r="21" spans="1:9" ht="20">
       <c r="A21" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="19" customFormat="1">
@@ -1866,16 +1976,16 @@
         <v>3</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I22" s="17" t="s">
         <v>4</v>
@@ -1883,7 +1993,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B23" s="2">
         <v>74.7</v>
@@ -1896,15 +2006,12 @@
         <v>1045.8</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24" s="2">
         <v>0</v>
@@ -1915,21 +2022,35 @@
       <c r="D24" s="2">
         <v>0</v>
       </c>
+      <c r="E24" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="G24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="1" t="s">
-        <v>122</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="22" customFormat="1">
+      <c r="A25" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="23">
+        <v>100</v>
+      </c>
+      <c r="C25" s="22">
+        <v>1</v>
+      </c>
+      <c r="D25" s="23">
+        <f>C25*B25</f>
+        <v>100</v>
+      </c>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B26" s="2">
         <v>0</v>
@@ -1940,312 +2061,349 @@
       <c r="D26" s="2">
         <v>0</v>
       </c>
+      <c r="E26" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="G26" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="1" t="s">
-        <v>124</v>
-      </c>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="22" customFormat="1">
+      <c r="A27" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="23">
+        <v>100</v>
+      </c>
+      <c r="C27" s="22">
+        <v>2</v>
+      </c>
+      <c r="D27" s="23">
+        <f>C27*B27</f>
+        <v>200</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="22" customFormat="1">
+      <c r="A28" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B28" s="23">
+        <v>200</v>
+      </c>
+      <c r="C28" s="22">
+        <v>1</v>
+      </c>
+      <c r="D28" s="23">
+        <f>C28*B28</f>
+        <v>200</v>
+      </c>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="C29" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="11">
-        <f>SUM(D23:D27)</f>
-        <v>1045.8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="20">
-      <c r="A31" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="10"/>
-    </row>
-    <row r="32" spans="1:9" s="19" customFormat="1">
-      <c r="A32" s="17" t="s">
+      <c r="A29" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B29" s="2">
+        <v>60</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2">
+        <f>C29*B29</f>
+        <v>60</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="C31" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="11">
+        <f>SUM(D23:D29)</f>
+        <v>1605.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="20">
+      <c r="A33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="10"/>
+    </row>
+    <row r="34" spans="1:9" s="19" customFormat="1">
+      <c r="A34" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="17" t="s">
+      <c r="B34" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D34" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="G32" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H32" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="I32" s="17" t="s">
+      <c r="E34" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34" s="17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="1" t="s">
+    <row r="35" spans="1:9">
+      <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B35" s="2">
         <v>12.9</v>
       </c>
-      <c r="C33" s="1">
-        <v>1</v>
-      </c>
-      <c r="D33" s="2">
-        <f>C33*B33</f>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2">
+        <f>C35*B35</f>
         <v>12.9</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="2">
-        <v>0.48</v>
-      </c>
-      <c r="C34" s="1">
+      <c r="E35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="2">
-        <f>C34*B34</f>
-        <v>2.88</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="22" customFormat="1">
-      <c r="A35" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="23"/>
-      <c r="D35" s="23">
-        <f>C35*B35</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="B36" s="2">
-        <v>30</v>
+        <v>0.48</v>
       </c>
       <c r="C36" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D36" s="2">
         <f>C36*B36</f>
+        <v>2.88</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="2">
         <v>30</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="C38" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D38" s="11">
-        <f>SUM(D33:D36)</f>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2">
+        <f>C37*B37</f>
+        <v>30</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="C39" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="11">
+        <f>SUM(D35:D37)</f>
         <v>45.78</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="20">
-      <c r="A40" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="19" customFormat="1">
-      <c r="A41" s="17" t="s">
+    <row r="41" spans="1:9" ht="20">
+      <c r="A41" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="19" customFormat="1">
+      <c r="A42" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="17" t="s">
+      <c r="B42" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D42" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F41" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="G41" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H41" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="I41" s="17" t="s">
+      <c r="E42" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I42" s="17" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="2">
-        <v>40</v>
-      </c>
-      <c r="C42" s="1">
-        <v>10</v>
-      </c>
-      <c r="D42" s="2">
-        <f>C42*B42</f>
-        <v>400</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B43" s="2">
+        <v>40</v>
+      </c>
+      <c r="C43" s="1">
         <v>10</v>
-      </c>
-      <c r="C43" s="1">
-        <v>1</v>
       </c>
       <c r="D43" s="2">
         <f>C43*B43</f>
+        <v>400</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="22" customFormat="1">
-      <c r="A44" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="23">
-        <v>15</v>
-      </c>
-      <c r="C44" s="22">
-        <v>1</v>
-      </c>
-      <c r="D44" s="23">
+      <c r="B44" s="2">
+        <v>10</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2">
         <f>C44*B44</f>
-        <v>15</v>
-      </c>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="H44" s="23"/>
+        <v>10</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>57</v>
+        <v>174</v>
       </c>
       <c r="B45" s="2">
+        <v>11.21</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2">
+        <f>C45*B45</f>
+        <v>11.21</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="2">
         <v>0</v>
       </c>
-      <c r="C45" s="1">
-        <v>1</v>
-      </c>
-      <c r="D45" s="2">
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46" s="2">
         <v>0</v>
       </c>
-      <c r="G45" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="22" customFormat="1">
-      <c r="A46" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B46" s="23">
-        <v>40</v>
-      </c>
-      <c r="C46" s="22">
-        <v>2</v>
-      </c>
-      <c r="D46" s="23">
-        <f>C46*B46</f>
-        <v>80</v>
-      </c>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
+      <c r="E46" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="48" spans="1:9">
       <c r="C48" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D48" s="11">
-        <f>SUM(D42:D46)</f>
-        <v>505</v>
+        <f>SUM(D43:D46)</f>
+        <v>421.21</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="20">
       <c r="A50" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="19" customFormat="1">
@@ -2262,16 +2420,16 @@
         <v>3</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F51" s="18" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I51" s="17" t="s">
         <v>4</v>
@@ -2279,7 +2437,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B52" s="2">
         <v>1500</v>
@@ -2288,22 +2446,22 @@
         <v>1</v>
       </c>
       <c r="D52" s="2">
-        <f t="shared" ref="D52:D73" si="1">C52*B52</f>
+        <f t="shared" ref="D52:D78" si="1">C52*B52</f>
         <v>1500</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B53" s="2">
         <v>280</v>
@@ -2316,18 +2474,18 @@
         <v>280</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B54" s="2">
         <v>13</v>
@@ -2340,21 +2498,21 @@
         <v>13</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B55" s="2">
         <v>6.99</v>
@@ -2366,21 +2524,21 @@
         <v>6.99</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B56" s="2">
         <v>6.24</v>
@@ -2393,18 +2551,18 @@
         <v>6.24</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B57" s="2">
         <v>2.36</v>
@@ -2417,21 +2575,21 @@
         <v>4.72</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B58" s="2">
         <f>1.94+2.29</f>
@@ -2445,18 +2603,18 @@
         <v>4.2300000000000004</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B59" s="2">
         <v>3.49</v>
@@ -2469,18 +2627,18 @@
         <v>3.49</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B60" s="2">
         <v>2.99</v>
@@ -2493,18 +2651,18 @@
         <v>5.98</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B61" s="2">
         <v>10</v>
@@ -2517,45 +2675,48 @@
         <v>30</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" s="22" customFormat="1">
-      <c r="A62" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B62" s="23">
-        <v>269</v>
-      </c>
-      <c r="C62" s="22">
-        <v>1</v>
-      </c>
-      <c r="D62" s="23">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B62" s="2">
+        <v>235.21</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1</v>
+      </c>
+      <c r="D62" s="2">
         <f t="shared" si="2"/>
-        <v>269</v>
-      </c>
-      <c r="E62" s="23"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="H62" s="23"/>
-      <c r="I62" s="22" t="s">
-        <v>84</v>
+        <v>235.21</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B63" s="2">
         <v>0</v>
@@ -2568,49 +2729,50 @@
         <v>0</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" s="22" customFormat="1">
-      <c r="A64" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B64" s="23">
-        <v>14.95</v>
-      </c>
-      <c r="C64" s="22">
-        <v>1</v>
-      </c>
-      <c r="D64" s="23">
-        <f t="shared" si="1"/>
-        <v>14.95</v>
-      </c>
-      <c r="E64" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="F64" s="23"/>
-      <c r="G64" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="H64" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="I64" s="22" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B64" s="2">
+        <v>12.95</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" s="1" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B65" s="2">
         <v>10.57</v>
@@ -2623,21 +2785,21 @@
         <v>10.57</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B66" s="2">
         <v>9.9000000000000005E-2</v>
@@ -2650,21 +2812,24 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B67" s="2">
         <v>0.18</v>
@@ -2677,21 +2842,24 @@
         <v>0.72</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="B68" s="2">
         <v>0.22</v>
@@ -2704,21 +2872,24 @@
         <v>0.22</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B69" s="2">
         <v>50</v>
@@ -2731,21 +2902,21 @@
         <v>50</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70" s="1" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B70" s="2">
         <v>1.99</v>
@@ -2758,1005 +2929,1207 @@
         <v>1.99</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" s="24" customFormat="1">
-      <c r="A71" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="B71" s="25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B71" s="2">
         <v>8.9499999999999993</v>
       </c>
-      <c r="C71" s="24">
-        <v>1</v>
-      </c>
-      <c r="D71" s="25">
+      <c r="C71" s="1">
+        <v>1</v>
+      </c>
+      <c r="D71" s="2">
         <f t="shared" si="1"/>
         <v>8.9499999999999993</v>
       </c>
-      <c r="E71" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="F71" s="25"/>
-      <c r="G71" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="H71" s="25"/>
-      <c r="I71" s="24" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" s="24" customFormat="1">
-      <c r="A72" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="B72" s="25">
+      <c r="E71" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B72" s="2">
         <v>2.95</v>
       </c>
-      <c r="C72" s="24">
+      <c r="C72" s="1">
         <v>3</v>
       </c>
-      <c r="D72" s="25">
+      <c r="D72" s="2">
         <f t="shared" si="1"/>
         <v>8.8500000000000014</v>
       </c>
-      <c r="E72" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="F72" s="25"/>
-      <c r="G72" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="H72" s="25"/>
-      <c r="I72" s="24" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" s="24" customFormat="1">
-      <c r="A73" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="B73" s="25">
+      <c r="E72" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B73" s="2">
         <v>19.95</v>
       </c>
-      <c r="C73" s="24">
-        <v>1</v>
-      </c>
-      <c r="D73" s="25">
+      <c r="C73" s="1">
+        <v>1</v>
+      </c>
+      <c r="D73" s="2">
         <f t="shared" si="1"/>
         <v>19.95</v>
       </c>
-      <c r="E73" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="F73" s="25"/>
-      <c r="G73" s="25" t="s">
+      <c r="E73" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B74" s="2">
+        <v>14.47</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1</v>
+      </c>
+      <c r="D74" s="2">
+        <f t="shared" si="1"/>
+        <v>14.47</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B75" s="2">
+        <v>2.56</v>
+      </c>
+      <c r="C75" s="1">
+        <v>5</v>
+      </c>
+      <c r="D75" s="2">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="H73" s="25"/>
-      <c r="I73" s="24" t="s">
+      <c r="B76" s="2">
+        <v>3.72</v>
+      </c>
+      <c r="C76" s="1">
+        <v>5</v>
+      </c>
+      <c r="D76" s="2">
+        <f t="shared" si="1"/>
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B77" s="2">
+        <v>8.69</v>
+      </c>
+      <c r="C77" s="1">
+        <v>1</v>
+      </c>
+      <c r="D77" s="2">
+        <f t="shared" si="1"/>
+        <v>8.69</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I77" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
-      <c r="C75" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D75" s="11">
-        <f>SUM(D52:D73)</f>
-        <v>2239.9489999999992</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="20">
-      <c r="A77" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
-      <c r="A78" s="17" t="s">
+    <row r="78" spans="1:9">
+      <c r="A78" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B78" s="2">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="C78" s="1">
+        <v>1</v>
+      </c>
+      <c r="D78" s="2">
+        <f t="shared" si="1"/>
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="C80" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D80" s="11">
+        <f>SUM(D52:D78)</f>
+        <v>2254.2189999999991</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="20">
+      <c r="A82" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B78" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C78" s="17" t="s">
+      <c r="B83" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D78" s="18" t="s">
+      <c r="D83" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E78" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F78" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="G78" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H78" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="I78" s="17" t="s">
+      <c r="E83" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F83" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G83" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H83" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I83" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J78" s="19"/>
-    </row>
-    <row r="79" spans="1:10">
-      <c r="A79" s="1" t="s">
+      <c r="J83" s="19"/>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" s="2">
+        <v>56.75</v>
+      </c>
+      <c r="C84" s="1">
+        <v>1</v>
+      </c>
+      <c r="D84" s="2">
+        <f>C84*B84</f>
+        <v>56.75</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B79" s="2">
-        <v>56.75</v>
-      </c>
-      <c r="C79" s="1">
-        <v>1</v>
-      </c>
-      <c r="D79" s="2">
-        <f>C79*B79</f>
-        <v>56.75</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
-      <c r="A80" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B80" s="2">
+      <c r="B85" s="2">
         <v>49</v>
       </c>
-      <c r="C80" s="1">
-        <v>1</v>
-      </c>
-      <c r="D80" s="2">
-        <f>C80*B80</f>
+      <c r="C85" s="1">
+        <v>1</v>
+      </c>
+      <c r="D85" s="2">
+        <f>C85*B85</f>
         <v>49</v>
       </c>
-      <c r="E80" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G80" s="2" t="s">
+      <c r="E85" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" s="19" customFormat="1">
+      <c r="A86" s="1"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="C87" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" s="19" customFormat="1">
-      <c r="A81" s="1"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-    </row>
-    <row r="82" spans="1:10">
-      <c r="C82" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D82" s="11">
-        <f>SUM(D79:D80)</f>
+      <c r="D87" s="11">
+        <f>SUM(D84:D85)</f>
         <v>105.75</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="20">
-      <c r="A84" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
-      <c r="A85" s="17" t="s">
+    <row r="89" spans="1:10" ht="20">
+      <c r="A89" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B85" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C85" s="17" t="s">
+      <c r="B90" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D85" s="18" t="s">
+      <c r="D90" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E85" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F85" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="G85" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H85" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="I85" s="17" t="s">
+      <c r="E90" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F90" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G90" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H90" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I90" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J85" s="19"/>
-    </row>
-    <row r="86" spans="1:10" s="22" customFormat="1">
-      <c r="A86" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="B86" s="23">
+      <c r="J90" s="19"/>
+    </row>
+    <row r="91" spans="1:10" s="22" customFormat="1">
+      <c r="A91" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B91" s="23">
         <v>50</v>
       </c>
-      <c r="C86" s="22">
-        <v>1</v>
-      </c>
-      <c r="D86" s="23">
-        <f>C86*B86</f>
+      <c r="C91" s="22">
+        <v>1</v>
+      </c>
+      <c r="D91" s="23">
+        <f>C91*B91</f>
         <v>50</v>
       </c>
-      <c r="E86" s="23"/>
-      <c r="F86" s="23"/>
-      <c r="G86" s="23" t="s">
+      <c r="E91" s="23"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="H91" s="23"/>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B92" s="2">
+        <v>15.99</v>
+      </c>
+      <c r="C92" s="1">
+        <v>5</v>
+      </c>
+      <c r="D92" s="2">
+        <f>C92*B92</f>
+        <v>79.95</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B93" s="2">
+        <v>10</v>
+      </c>
+      <c r="C93" s="1">
+        <v>1</v>
+      </c>
+      <c r="D93" s="2">
+        <f>C93*B93</f>
+        <v>10</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" s="19" customFormat="1">
+      <c r="A95" s="1"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D95" s="11">
+        <f>SUM(D91:D93)</f>
+        <v>139.94999999999999</v>
+      </c>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+    </row>
+    <row r="97" spans="1:10" ht="20">
+      <c r="A97" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E98" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F98" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G98" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H98" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I98" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J98" s="19"/>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B99" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="C99" s="1">
+        <v>200</v>
+      </c>
+      <c r="D99" s="2">
+        <f>C99*B99</f>
+        <v>126</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G99" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="H86" s="23"/>
-    </row>
-    <row r="87" spans="1:10">
-      <c r="A87" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B87" s="2">
-        <v>15.99</v>
-      </c>
-      <c r="C87" s="1">
-        <v>5</v>
-      </c>
-      <c r="D87" s="2">
-        <f>C87*B87</f>
-        <v>79.95</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I87" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10">
-      <c r="A88" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B88" s="2">
-        <v>10</v>
-      </c>
-      <c r="C88" s="1">
-        <v>1</v>
-      </c>
-      <c r="D88" s="2">
-        <f>C88*B88</f>
-        <v>10</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H88" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" s="19" customFormat="1">
-      <c r="A90" s="1"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D90" s="11">
-        <f>SUM(D86:D88)</f>
-        <v>139.94999999999999</v>
-      </c>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
-      <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-    </row>
-    <row r="92" spans="1:10" ht="20">
-      <c r="A92" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10">
-      <c r="A93" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B93" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C93" s="17" t="s">
+      <c r="I99" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B100" s="2">
+        <v>7.27</v>
+      </c>
+      <c r="C100" s="1">
         <v>2</v>
       </c>
-      <c r="D93" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E93" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F93" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="G93" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H93" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="I93" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J93" s="19"/>
-    </row>
-    <row r="94" spans="1:10" s="24" customFormat="1">
-      <c r="A94" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B94" s="25">
-        <v>0.63</v>
-      </c>
-      <c r="C94" s="24">
-        <v>200</v>
-      </c>
-      <c r="D94" s="25">
-        <f>C94*B94</f>
-        <v>126</v>
-      </c>
-      <c r="E94" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="F94" s="25"/>
-      <c r="G94" s="25" t="s">
+      <c r="D100" s="2">
+        <f t="shared" ref="D100:D104" si="3">C100*B100</f>
+        <v>14.54</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" s="24" customFormat="1">
+      <c r="A101" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="B101" s="25">
+        <v>10.45</v>
+      </c>
+      <c r="C101" s="24">
+        <v>1</v>
+      </c>
+      <c r="D101" s="25">
+        <f t="shared" si="3"/>
+        <v>10.45</v>
+      </c>
+      <c r="E101" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F101" s="25"/>
+      <c r="G101" s="25"/>
+      <c r="H101" s="25"/>
+    </row>
+    <row r="102" spans="1:10" s="19" customFormat="1">
+      <c r="A102" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H94" s="25"/>
-      <c r="I94" s="24" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10">
-      <c r="A95" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B95" s="2">
-        <v>7.27</v>
-      </c>
-      <c r="C95" s="1">
-        <v>2</v>
-      </c>
-      <c r="D95" s="2">
-        <f t="shared" ref="D95:D98" si="3">C95*B95</f>
-        <v>14.54</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G95" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" s="19" customFormat="1">
-      <c r="A96" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B96" s="2">
+      <c r="B102" s="2">
         <v>89.9</v>
       </c>
-      <c r="C96" s="1">
-        <v>1</v>
-      </c>
-      <c r="D96" s="2">
+      <c r="C102" s="1">
+        <v>1</v>
+      </c>
+      <c r="D102" s="2">
         <f t="shared" si="3"/>
         <v>89.9</v>
       </c>
-      <c r="E96" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J96" s="1"/>
-    </row>
-    <row r="97" spans="1:10">
-      <c r="A97" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B97" s="2">
+      <c r="E102" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J102" s="1"/>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B103" s="2">
         <v>6.45</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C103" s="1">
         <v>3</v>
       </c>
-      <c r="D97" s="2">
+      <c r="D103" s="2">
         <f t="shared" si="3"/>
         <v>19.350000000000001</v>
       </c>
-      <c r="E97" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10">
-      <c r="A98" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B98" s="2">
+      <c r="E103" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B104" s="2">
         <f>18.95+4.95-5</f>
         <v>18.899999999999999</v>
       </c>
-      <c r="C98" s="1">
-        <v>1</v>
-      </c>
-      <c r="D98" s="2">
+      <c r="C104" s="1">
+        <v>1</v>
+      </c>
+      <c r="D104" s="2">
         <f t="shared" si="3"/>
         <v>18.899999999999999</v>
       </c>
-      <c r="E98" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" s="22" customFormat="1">
-      <c r="A99" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="B99" s="23"/>
-      <c r="D99" s="23"/>
-      <c r="E99" s="23"/>
-      <c r="F99" s="23"/>
-      <c r="G99" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="H99" s="23"/>
-      <c r="I99" s="22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10">
-      <c r="A100" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B100" s="2">
+      <c r="E104" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" s="24" customFormat="1">
+      <c r="A105" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="B105" s="25">
+        <f>5.72*0.8</f>
+        <v>4.5759999999999996</v>
+      </c>
+      <c r="C105" s="24">
+        <v>30</v>
+      </c>
+      <c r="D105" s="25">
+        <f>C105*B105</f>
+        <v>137.28</v>
+      </c>
+      <c r="E105" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F105" s="25"/>
+      <c r="G105" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="H105" s="25"/>
+      <c r="I105" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B106" s="2">
         <v>5.9</v>
       </c>
-      <c r="C100" s="1">
-        <v>1</v>
-      </c>
-      <c r="D100" s="2">
-        <f t="shared" ref="D100:D106" si="4">C100*B100</f>
+      <c r="C106" s="1">
+        <v>1</v>
+      </c>
+      <c r="D106" s="2">
+        <f t="shared" ref="D106:D112" si="4">C106*B106</f>
         <v>5.9</v>
       </c>
-      <c r="E100" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10">
-      <c r="A101" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B101" s="2">
+      <c r="E106" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B107" s="2">
         <v>16.71</v>
       </c>
-      <c r="C101" s="1">
-        <v>1</v>
-      </c>
-      <c r="D101" s="2">
+      <c r="C107" s="1">
+        <v>1</v>
+      </c>
+      <c r="D107" s="2">
         <f t="shared" si="4"/>
         <v>16.71</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I101" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10">
-      <c r="A102" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B102" s="2">
+      <c r="E107" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="A108" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B108" s="2">
         <v>5.2</v>
       </c>
-      <c r="C102" s="1">
+      <c r="C108" s="1">
         <v>2</v>
       </c>
-      <c r="D102" s="2">
+      <c r="D108" s="2">
         <f t="shared" si="4"/>
         <v>10.4</v>
       </c>
-      <c r="E102" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G102" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I102" s="1" t="s">
+      <c r="E108" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="103" spans="1:10">
-      <c r="A103" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B103" s="2">
+      <c r="B109" s="2">
         <v>9.5</v>
       </c>
-      <c r="C103" s="1">
+      <c r="C109" s="1">
         <v>2</v>
       </c>
-      <c r="D103" s="2">
+      <c r="D109" s="2">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="E103" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G103" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H103" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="I103" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10">
-      <c r="A104" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B104" s="2">
+      <c r="E109" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="A110" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B110" s="2">
         <v>5.26</v>
       </c>
-      <c r="C104" s="1">
-        <v>1</v>
-      </c>
-      <c r="D104" s="2">
+      <c r="C110" s="1">
+        <v>1</v>
+      </c>
+      <c r="D110" s="2">
         <f t="shared" si="4"/>
         <v>5.26</v>
       </c>
-      <c r="E104" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H104" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I104" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10">
-      <c r="A105" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B105" s="2">
-        <v>3.72</v>
-      </c>
-      <c r="C105" s="1">
-        <v>5</v>
-      </c>
-      <c r="D105" s="2">
+      <c r="E110" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B111" s="2">
+        <v>2.17</v>
+      </c>
+      <c r="C111" s="1">
+        <v>1</v>
+      </c>
+      <c r="D111" s="2">
         <f t="shared" si="4"/>
-        <v>18.600000000000001</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H105" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="I105" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10">
-      <c r="A106" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B106" s="2">
+        <v>2.17</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="A112" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B112" s="2">
         <v>8.08</v>
       </c>
-      <c r="C106" s="1">
-        <v>1</v>
-      </c>
-      <c r="D106" s="2">
+      <c r="C112" s="1">
+        <v>1</v>
+      </c>
+      <c r="D112" s="2">
         <f t="shared" si="4"/>
         <v>8.08</v>
       </c>
-      <c r="E106" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G106" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10">
-      <c r="A108" s="10"/>
-      <c r="C108" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D108" s="11">
-        <f>SUM(D94:D106)</f>
-        <v>352.63999999999993</v>
-      </c>
-      <c r="I108" s="15"/>
-    </row>
-    <row r="109" spans="1:10">
-      <c r="A109" s="20"/>
-      <c r="B109" s="21"/>
-      <c r="C109" s="20"/>
-      <c r="D109" s="21"/>
-      <c r="E109" s="21"/>
-      <c r="F109" s="21"/>
-      <c r="G109" s="21"/>
-      <c r="H109" s="21"/>
-      <c r="I109" s="20"/>
-    </row>
-    <row r="110" spans="1:10" ht="20">
-      <c r="A110" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10">
-      <c r="A111" s="17" t="s">
+      <c r="E112" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114" s="10"/>
+      <c r="C114" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D114" s="11">
+        <f>SUM(D99:D112)</f>
+        <v>483.93999999999988</v>
+      </c>
+      <c r="I114" s="15"/>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115" s="20"/>
+      <c r="B115" s="21"/>
+      <c r="C115" s="20"/>
+      <c r="D115" s="21"/>
+      <c r="E115" s="21"/>
+      <c r="F115" s="21"/>
+      <c r="G115" s="21"/>
+      <c r="H115" s="21"/>
+      <c r="I115" s="20"/>
+    </row>
+    <row r="116" spans="1:10" ht="20">
+      <c r="A116" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B111" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C111" s="17" t="s">
+      <c r="B117" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D111" s="18" t="s">
+      <c r="D117" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E111" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F111" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="G111" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H111" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="I111" s="17" t="s">
+      <c r="E117" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F117" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G117" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H117" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I117" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J111" s="19"/>
-    </row>
-    <row r="112" spans="1:10">
-      <c r="A112" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B112" s="2">
-        <v>0</v>
-      </c>
-      <c r="C112" s="1">
-        <v>1</v>
-      </c>
-      <c r="D112" s="2">
-        <v>0</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G112" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H112" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10">
-      <c r="A113" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B113" s="2">
-        <v>0</v>
-      </c>
-      <c r="C113" s="1">
-        <v>1</v>
-      </c>
-      <c r="D113" s="2">
-        <v>0</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G113" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H113" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J113" s="15"/>
-    </row>
-    <row r="114" spans="1:10" s="24" customFormat="1">
-      <c r="A114" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="B114" s="25">
-        <v>149.99</v>
-      </c>
-      <c r="C114" s="24">
-        <v>1</v>
-      </c>
-      <c r="D114" s="25">
-        <f>C114*B114</f>
-        <v>149.99</v>
-      </c>
-      <c r="E114" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="F114" s="25"/>
-      <c r="G114" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="I114" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="J114" s="26"/>
-    </row>
-    <row r="115" spans="1:10">
-      <c r="A115" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B115" s="2">
-        <v>28.75</v>
-      </c>
-      <c r="C115" s="1">
-        <v>1</v>
-      </c>
-      <c r="D115" s="2">
-        <f>C115*B115</f>
-        <v>28.75</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G115" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H115" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="I115" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" s="24" customFormat="1">
-      <c r="A116" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="B116" s="25">
-        <v>8.99</v>
-      </c>
-      <c r="C116" s="24">
-        <v>1</v>
-      </c>
-      <c r="D116" s="25">
-        <f>C116*B116</f>
-        <v>8.99</v>
-      </c>
-      <c r="E116" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="F116" s="25"/>
-      <c r="G116" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="H116" s="25"/>
-      <c r="I116" s="24" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" s="19" customFormat="1">
-      <c r="A117" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B117" s="2">
-        <v>0</v>
-      </c>
-      <c r="C117" s="1">
-        <v>2</v>
-      </c>
-      <c r="D117" s="2">
-        <v>0</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F117" s="2"/>
-      <c r="G117" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H117" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="I117" s="1"/>
-      <c r="J117" s="1"/>
+      <c r="J117" s="19"/>
     </row>
     <row r="118" spans="1:10">
       <c r="A118" s="1" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="B118" s="2">
         <v>0</v>
       </c>
       <c r="C118" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D118" s="2">
         <v>0</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>53</v>
+        <v>39</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
     </row>
     <row r="119" spans="1:10">
       <c r="A119" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B119" s="2">
+        <v>0</v>
+      </c>
+      <c r="C119" s="1">
+        <v>1</v>
+      </c>
+      <c r="D119" s="2">
+        <v>0</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J119" s="15"/>
+    </row>
+    <row r="120" spans="1:10">
+      <c r="A120" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B120" s="2">
+        <v>149.99</v>
+      </c>
+      <c r="C120" s="1">
+        <v>1</v>
+      </c>
+      <c r="D120" s="2">
+        <f>C120*B120</f>
+        <v>149.99</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H120" s="1"/>
+      <c r="I120" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="J120" s="15"/>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B121" s="2">
+        <v>28.75</v>
+      </c>
+      <c r="C121" s="1">
+        <v>1</v>
+      </c>
+      <c r="D121" s="2">
+        <f>C121*B121</f>
+        <v>28.75</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H121" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I121" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
+      <c r="A122" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B122" s="2">
+        <v>8.99</v>
+      </c>
+      <c r="C122" s="1">
+        <v>1</v>
+      </c>
+      <c r="D122" s="2">
+        <f>C122*B122</f>
+        <v>8.99</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I122" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" s="19" customFormat="1">
+      <c r="A123" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B123" s="2">
+        <v>0</v>
+      </c>
+      <c r="C123" s="1">
+        <v>2</v>
+      </c>
+      <c r="D123" s="2">
+        <v>0</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F123" s="2"/>
+      <c r="G123" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H123" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I123" s="1"/>
+      <c r="J123" s="1"/>
+    </row>
+    <row r="124" spans="1:10">
+      <c r="A124" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B124" s="2">
+        <v>0</v>
+      </c>
+      <c r="C124" s="1">
+        <v>2</v>
+      </c>
+      <c r="D124" s="2">
+        <v>0</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H124" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
+      <c r="A125" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B125" s="2">
         <v>9</v>
       </c>
-      <c r="C119" s="1">
-        <v>1</v>
-      </c>
-      <c r="D119" s="2">
-        <f>C119*B119</f>
+      <c r="C125" s="1">
+        <v>1</v>
+      </c>
+      <c r="D125" s="2">
+        <f>C125*B125</f>
         <v>9</v>
       </c>
-      <c r="E119" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G119" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" s="15" customFormat="1">
-      <c r="A120" s="1"/>
-      <c r="B120" s="2"/>
-      <c r="C120" s="1"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="2"/>
-      <c r="F120" s="2"/>
-      <c r="G120" s="2"/>
-      <c r="H120" s="2"/>
-      <c r="I120" s="1"/>
-      <c r="J120" s="1"/>
-    </row>
-    <row r="121" spans="1:10">
-      <c r="C121" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D121" s="11">
-        <f>SUM(D112:D118)</f>
-        <v>187.73000000000002</v>
+      <c r="E125" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
+      <c r="A126" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B126" s="2">
+        <v>11.8</v>
+      </c>
+      <c r="C126" s="1">
+        <v>1</v>
+      </c>
+      <c r="D126" s="2">
+        <f>C126*B126</f>
+        <v>11.8</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" s="15" customFormat="1">
+      <c r="A127" s="1"/>
+      <c r="B127" s="2"/>
+      <c r="C127" s="1"/>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+      <c r="G127" s="2"/>
+      <c r="H127" s="2"/>
+      <c r="I127" s="1"/>
+      <c r="J127" s="1"/>
+    </row>
+    <row r="128" spans="1:10">
+      <c r="C128" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D128" s="11">
+        <f>SUM(D118:D126)</f>
+        <v>208.53000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final items arrived before travel
</commit_message>
<xml_diff>
--- a/DetailedBudget.xlsx
+++ b/DetailedBudget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7160" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="15780" yWindow="0" windowWidth="13040" windowHeight="16140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="194">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -48,9 +48,6 @@
     <t>http://www.amazon.com/Royal-Bingo-Supplies-Wooden-Game/dp/B00GGHMRTI/ref=sr_1_2?ie=UTF8&amp;qid=1436456392&amp;sr=8-2&amp;keywords=bingo+cage&amp;refinements=p_85%3A2470955011</t>
   </si>
   <si>
-    <t>Plywood for furniture</t>
-  </si>
-  <si>
     <t>Wood glue</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
     <t>Airbnb</t>
   </si>
   <si>
-    <t>Hand and power tools</t>
-  </si>
-  <si>
     <t>Local lumberyard</t>
   </si>
   <si>
@@ -598,6 +592,15 @@
   </si>
   <si>
     <t>Shipped</t>
+  </si>
+  <si>
+    <t>Plywood for furniture (8 sheets at 12 x 2200 x 1220mm)</t>
+  </si>
+  <si>
+    <t>Circular saw rental</t>
+  </si>
+  <si>
+    <t>iZettle reader</t>
   </si>
 </sst>
 </file>
@@ -681,7 +684,7 @@
       <name val="Open Sans"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -691,6 +694,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1002,7 +1011,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1036,6 +1045,9 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="296">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1662,10 +1674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J130"/>
+  <dimension ref="A1:J131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1684,37 +1696,37 @@
   <sheetData>
     <row r="1" spans="1:9" ht="34">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="20">
       <c r="E2" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:9" s="10" customFormat="1" ht="20">
       <c r="A3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6">
-        <f>D21+D33+D41+D50+D82+D89+D97+D116+D130</f>
-        <v>12845.179</v>
+        <f>D21+D33+D41+D50+D82+D89+D97+D116+D131</f>
+        <v>12833.086200000002</v>
       </c>
       <c r="E3" s="7">
         <v>0.64</v>
       </c>
       <c r="F3" s="8">
         <f>D3*E3</f>
-        <v>8220.9145600000011</v>
+        <v>8213.1751680000016</v>
       </c>
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:9" ht="20">
       <c r="A4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="5"/>
@@ -1732,20 +1744,20 @@
     </row>
     <row r="5" spans="1:9" ht="20">
       <c r="A5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6">
         <f>D4-D3</f>
-        <v>-345.17900000000009</v>
+        <v>-333.08620000000155</v>
       </c>
       <c r="E5" s="7">
         <v>0.64</v>
       </c>
       <c r="F5" s="8">
         <f>D5*E5</f>
-        <v>-220.91456000000005</v>
+        <v>-213.17516800000101</v>
       </c>
       <c r="H5" s="9"/>
     </row>
@@ -1781,7 +1793,7 @@
     </row>
     <row r="9" spans="1:9" ht="20">
       <c r="A9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="19" customFormat="1">
@@ -1798,16 +1810,16 @@
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>4</v>
@@ -1815,7 +1827,7 @@
     </row>
     <row r="11" spans="1:9" s="15" customFormat="1">
       <c r="A11" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2">
         <v>850</v>
@@ -1828,20 +1840,20 @@
         <v>850</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" s="15" customFormat="1">
       <c r="A12" s="15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B12" s="2">
         <v>145</v>
@@ -1859,24 +1871,31 @@
       <c r="H12" s="2"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="B13" s="2">
-        <v>200</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2">
+    <row r="13" spans="1:9" s="25" customFormat="1">
+      <c r="A13" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" s="26">
+        <f>98.5*1.64</f>
+        <v>161.54</v>
+      </c>
+      <c r="C13" s="25">
+        <v>1</v>
+      </c>
+      <c r="D13" s="26">
         <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
+        <v>161.54</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="2">
         <v>550</v>
@@ -1889,18 +1908,18 @@
         <v>550</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="2">
         <v>600</v>
@@ -1915,7 +1934,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B16" s="2">
         <v>60</v>
@@ -1930,7 +1949,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B17" s="2">
         <v>2025</v>
@@ -1943,18 +1962,18 @@
         <v>2025</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2">
         <v>3000</v>
@@ -1967,15 +1986,15 @@
         <v>3000</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B19" s="2">
         <v>15</v>
@@ -1988,27 +2007,27 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="C21" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="11">
         <f>SUM(D11:D19)</f>
-        <v>7590</v>
+        <v>7551.54</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="20">
       <c r="A23" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="19" customFormat="1">
@@ -2025,16 +2044,16 @@
         <v>3</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I24" s="17" t="s">
         <v>4</v>
@@ -2042,7 +2061,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B25" s="2">
         <v>74.7</v>
@@ -2055,12 +2074,12 @@
         <v>1045.8</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2">
         <v>0</v>
@@ -2072,15 +2091,15 @@
         <v>0</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="22" customFormat="1">
       <c r="A27" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B27" s="23">
         <v>100</v>
@@ -2099,7 +2118,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
@@ -2111,15 +2130,15 @@
         <v>0</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="22" customFormat="1">
       <c r="A29" s="22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B29" s="23">
         <v>100</v>
@@ -2132,36 +2151,38 @@
         <v>200</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F29" s="23"/>
       <c r="G29" s="23"/>
       <c r="H29" s="23" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="22" customFormat="1">
-      <c r="A30" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="B30" s="23">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="25" customFormat="1">
+      <c r="A30" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B30" s="26">
         <v>200</v>
       </c>
-      <c r="C30" s="22">
-        <v>1</v>
-      </c>
-      <c r="D30" s="23">
+      <c r="C30" s="25">
+        <v>1</v>
+      </c>
+      <c r="D30" s="26">
         <f>C30*B30</f>
         <v>200</v>
       </c>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
+      <c r="E30" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B31" s="2">
         <v>60</v>
@@ -2174,12 +2195,12 @@
         <v>60</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="C33" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" s="11">
         <f>SUM(D25:D31)</f>
@@ -2188,7 +2209,7 @@
     </row>
     <row r="35" spans="1:9" ht="20">
       <c r="A35" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -2213,16 +2234,16 @@
         <v>3</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I36" s="17" t="s">
         <v>4</v>
@@ -2243,16 +2264,16 @@
         <v>12.9</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>6</v>
@@ -2260,7 +2281,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B38" s="2">
         <v>0.48</v>
@@ -2273,13 +2294,13 @@
         <v>2.88</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2297,13 +2318,13 @@
         <v>30</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>8</v>
@@ -2311,7 +2332,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="C41" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D41" s="11">
         <f>SUM(D37:D39)</f>
@@ -2320,7 +2341,7 @@
     </row>
     <row r="43" spans="1:9" ht="20">
       <c r="A43" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="19" customFormat="1">
@@ -2337,45 +2358,50 @@
         <v>3</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I44" s="17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" s="2">
-        <v>40</v>
-      </c>
-      <c r="C45" s="1">
-        <v>10</v>
-      </c>
-      <c r="D45" s="2">
+    <row r="45" spans="1:9" s="25" customFormat="1">
+      <c r="A45" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="B45" s="26">
+        <f>(182.4*1.64)/8</f>
+        <v>37.391999999999996</v>
+      </c>
+      <c r="C45" s="25">
+        <v>8</v>
+      </c>
+      <c r="D45" s="26">
         <f>C45*B45</f>
-        <v>400</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>54</v>
+        <v>299.13599999999997</v>
+      </c>
+      <c r="E45" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="H45" s="26" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46" s="2">
         <v>0</v>
@@ -2388,15 +2414,15 @@
         <v>0</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B47" s="2">
         <v>11.21</v>
@@ -2409,53 +2435,57 @@
         <v>11.21</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="2">
-        <v>0</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1</v>
-      </c>
-      <c r="D48" s="2">
-        <v>0</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>169</v>
-      </c>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="25" customFormat="1">
+      <c r="A48" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="B48" s="26">
+        <f>77.58*1.64</f>
+        <v>127.23119999999999</v>
+      </c>
+      <c r="C48" s="25">
+        <v>1</v>
+      </c>
+      <c r="D48" s="26">
+        <f>C48*B48</f>
+        <v>127.23119999999999</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="H48" s="26"/>
     </row>
     <row r="50" spans="1:9">
       <c r="C50" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D50" s="11">
         <f>SUM(D45:D48)</f>
-        <v>411.21</v>
+        <v>437.57719999999995</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="20">
       <c r="A52" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="19" customFormat="1">
@@ -2472,16 +2502,16 @@
         <v>3</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F53" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H53" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I53" s="17" t="s">
         <v>4</v>
@@ -2489,7 +2519,7 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B54" s="2">
         <v>1500</v>
@@ -2502,18 +2532,18 @@
         <v>1500</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B55" s="2">
         <v>280</v>
@@ -2526,18 +2556,18 @@
         <v>280</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B56" s="2">
         <v>13</v>
@@ -2550,21 +2580,21 @@
         <v>13</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B57" s="2">
         <v>6.99</v>
@@ -2576,21 +2606,21 @@
         <v>6.99</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B58" s="2">
         <v>6.24</v>
@@ -2603,18 +2633,18 @@
         <v>6.24</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B59" s="2">
         <v>2.36</v>
@@ -2627,21 +2657,21 @@
         <v>4.72</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B60" s="2">
         <f>1.94+2.29</f>
@@ -2655,18 +2685,18 @@
         <v>4.2300000000000004</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B61" s="2">
         <v>3.49</v>
@@ -2679,18 +2709,18 @@
         <v>3.49</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B62" s="2">
         <v>2.99</v>
@@ -2703,18 +2733,18 @@
         <v>5.98</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B63" s="2">
         <v>10</v>
@@ -2727,21 +2757,21 @@
         <v>30</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B64" s="2">
         <v>235.21</v>
@@ -2754,21 +2784,21 @@
         <v>235.21</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B65" s="2">
         <v>0</v>
@@ -2781,21 +2811,21 @@
         <v>0</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B66" s="2">
         <v>12.95</v>
@@ -2804,27 +2834,27 @@
         <v>1</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B67" s="2">
         <v>10.57</v>
@@ -2837,21 +2867,21 @@
         <v>10.57</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B68" s="2">
         <v>9.9000000000000005E-2</v>
@@ -2864,24 +2894,24 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B69" s="2">
         <v>0.18</v>
@@ -2894,24 +2924,24 @@
         <v>0.72</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H69" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B70" s="2">
         <v>0.22</v>
@@ -2924,24 +2954,24 @@
         <v>0.22</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B71" s="2">
         <v>50</v>
@@ -2954,21 +2984,21 @@
         <v>50</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B72" s="2">
         <v>1.99</v>
@@ -2981,18 +3011,18 @@
         <v>1.99</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B73" s="2">
         <v>8.9499999999999993</v>
@@ -3005,21 +3035,21 @@
         <v>8.9499999999999993</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B74" s="2">
         <v>2.95</v>
@@ -3032,21 +3062,21 @@
         <v>8.8500000000000014</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B75" s="2">
         <v>19.95</v>
@@ -3059,21 +3089,21 @@
         <v>19.95</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B76" s="2">
         <v>14.47</v>
@@ -3086,21 +3116,21 @@
         <v>14.47</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B77" s="2">
         <v>2.56</v>
@@ -3113,24 +3143,24 @@
         <v>12.8</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B78" s="2">
         <v>3.72</v>
@@ -3143,24 +3173,24 @@
         <v>18.600000000000001</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B79" s="2">
         <v>8.69</v>
@@ -3173,24 +3203,24 @@
         <v>8.69</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B80" s="2">
         <v>8.4499999999999993</v>
@@ -3203,21 +3233,21 @@
         <v>8.4499999999999993</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="C82" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D82" s="11">
         <f>SUM(D54:D80)</f>
@@ -3226,7 +3256,7 @@
     </row>
     <row r="84" spans="1:10" ht="20">
       <c r="A84" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -3243,16 +3273,16 @@
         <v>3</v>
       </c>
       <c r="E85" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F85" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G85" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H85" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I85" s="17" t="s">
         <v>4</v>
@@ -3261,7 +3291,7 @@
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B86" s="2">
         <v>56.75</v>
@@ -3274,21 +3304,21 @@
         <v>56.75</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B87" s="2">
         <v>49</v>
@@ -3301,13 +3331,13 @@
         <v>49</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="88" spans="1:10" s="19" customFormat="1">
@@ -3324,7 +3354,7 @@
     </row>
     <row r="89" spans="1:10">
       <c r="C89" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D89" s="11">
         <f>SUM(D86:D87)</f>
@@ -3333,7 +3363,7 @@
     </row>
     <row r="91" spans="1:10" ht="20">
       <c r="A91" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -3350,16 +3380,16 @@
         <v>3</v>
       </c>
       <c r="E92" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F92" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G92" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H92" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I92" s="17" t="s">
         <v>4</v>
@@ -3368,7 +3398,7 @@
     </row>
     <row r="93" spans="1:10" s="22" customFormat="1">
       <c r="A93" s="22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B93" s="23">
         <v>50</v>
@@ -3383,13 +3413,13 @@
       <c r="E93" s="23"/>
       <c r="F93" s="23"/>
       <c r="G93" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H93" s="23"/>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B94" s="2">
         <v>15.99</v>
@@ -3402,21 +3432,21 @@
         <v>79.95</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B95" s="2">
         <v>10</v>
@@ -3429,23 +3459,23 @@
         <v>10</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="97" spans="1:10" s="19" customFormat="1">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="C97" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D97" s="11">
         <f>SUM(D93:D95)</f>
@@ -3460,7 +3490,7 @@
     </row>
     <row r="99" spans="1:10" ht="20">
       <c r="A99" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -3477,16 +3507,16 @@
         <v>3</v>
       </c>
       <c r="E100" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F100" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G100" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H100" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I100" s="17" t="s">
         <v>4</v>
@@ -3495,7 +3525,7 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B101" s="2">
         <v>0.63</v>
@@ -3508,21 +3538,21 @@
         <v>126</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B102" s="2">
         <v>7.27</v>
@@ -3535,21 +3565,21 @@
         <v>14.54</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B103" s="2">
         <v>10.45</v>
@@ -3562,18 +3592,18 @@
         <v>10.45</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="104" spans="1:10" s="19" customFormat="1">
       <c r="A104" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B104" s="2">
         <v>89.9</v>
@@ -3586,25 +3616,25 @@
         <v>89.9</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J104" s="1"/>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B105" s="2">
         <v>6.45</v>
@@ -3617,21 +3647,21 @@
         <v>19.350000000000001</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B106" s="2">
         <f>18.95+4.95-5</f>
@@ -3645,24 +3675,24 @@
         <v>18.899999999999999</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B107" s="2">
         <f>5.72*0.8</f>
@@ -3676,21 +3706,21 @@
         <v>137.28</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="108" spans="1:10">
       <c r="A108" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B108" s="2">
         <v>5.9</v>
@@ -3703,18 +3733,18 @@
         <v>5.9</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B109" s="2">
         <v>16.71</v>
@@ -3727,21 +3757,21 @@
         <v>16.71</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B110" s="2">
         <v>5.2</v>
@@ -3754,21 +3784,21 @@
         <v>10.4</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="111" spans="1:10">
       <c r="A111" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B111" s="2">
         <v>9.5</v>
@@ -3781,24 +3811,24 @@
         <v>19</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G111" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I111" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="H111" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I111" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="112" spans="1:10">
       <c r="A112" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B112" s="2">
         <v>5.26</v>
@@ -3811,24 +3841,24 @@
         <v>5.26</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="113" spans="1:10">
       <c r="A113" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B113" s="2">
         <v>2.17</v>
@@ -3841,24 +3871,24 @@
         <v>2.17</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="114" spans="1:10">
       <c r="A114" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B114" s="2">
         <v>8.08</v>
@@ -3871,19 +3901,19 @@
         <v>8.08</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="116" spans="1:10">
       <c r="A116" s="10"/>
       <c r="C116" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D116" s="11">
         <f>SUM(D101:D114)</f>
@@ -3904,7 +3934,7 @@
     </row>
     <row r="118" spans="1:10" ht="20">
       <c r="A118" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="119" spans="1:10">
@@ -3921,16 +3951,16 @@
         <v>3</v>
       </c>
       <c r="E119" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F119" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G119" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H119" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I119" s="17" t="s">
         <v>4</v>
@@ -3939,7 +3969,7 @@
     </row>
     <row r="120" spans="1:10">
       <c r="A120" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B120" s="2">
         <v>0</v>
@@ -3951,21 +3981,21 @@
         <v>0</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="121" spans="1:10">
       <c r="A121" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B121" s="2">
         <v>0</v>
@@ -3977,22 +4007,22 @@
         <v>0</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J121" s="15"/>
     </row>
     <row r="122" spans="1:10">
       <c r="A122" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B122" s="2">
         <v>149.99</v>
@@ -4005,23 +4035,23 @@
         <v>149.99</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H122" s="1"/>
       <c r="I122" s="24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J122" s="15"/>
     </row>
     <row r="123" spans="1:10">
       <c r="A123" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B123" s="2">
         <v>28.75</v>
@@ -4034,24 +4064,24 @@
         <v>28.75</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="124" spans="1:10">
       <c r="A124" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B124" s="2">
         <v>8.99</v>
@@ -4064,21 +4094,21 @@
         <v>8.99</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="125" spans="1:10" s="19" customFormat="1">
       <c r="A125" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B125" s="2">
         <v>0</v>
@@ -4090,21 +4120,21 @@
         <v>0</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F125" s="2"/>
       <c r="G125" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I125" s="1"/>
       <c r="J125" s="1"/>
     </row>
     <row r="126" spans="1:10">
       <c r="A126" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B126" s="2">
         <v>0</v>
@@ -4116,18 +4146,18 @@
         <v>0</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="127" spans="1:10">
       <c r="A127" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B127" s="2">
         <v>9</v>
@@ -4140,18 +4170,18 @@
         <v>9</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="128" spans="1:10">
       <c r="A128" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B128" s="2">
         <v>11.8</v>
@@ -4164,35 +4194,57 @@
         <v>11.8</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10" s="15" customFormat="1">
-      <c r="A129" s="1"/>
-      <c r="B129" s="2"/>
-      <c r="C129" s="1"/>
-      <c r="D129" s="2"/>
-      <c r="E129" s="2"/>
-      <c r="F129" s="2"/>
-      <c r="G129" s="2"/>
-      <c r="H129" s="2"/>
-      <c r="I129" s="1"/>
-      <c r="J129" s="1"/>
-    </row>
-    <row r="130" spans="1:10">
-      <c r="C130" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D130" s="11">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" s="25" customFormat="1">
+      <c r="A129" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="B129" s="26">
+        <f>34.8*1.64</f>
+        <v>57.071999999999989</v>
+      </c>
+      <c r="C129" s="25">
+        <v>1</v>
+      </c>
+      <c r="D129" s="26">
+        <f>C129*B129</f>
+        <v>57.071999999999989</v>
+      </c>
+      <c r="E129" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F129" s="26"/>
+      <c r="G129" s="26"/>
+      <c r="H129" s="26"/>
+    </row>
+    <row r="130" spans="1:10" s="15" customFormat="1">
+      <c r="A130" s="1"/>
+      <c r="B130" s="2"/>
+      <c r="C130" s="1"/>
+      <c r="D130" s="2"/>
+      <c r="E130" s="2"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+      <c r="H130" s="2"/>
+      <c r="I130" s="1"/>
+      <c r="J130" s="1"/>
+    </row>
+    <row r="131" spans="1:10">
+      <c r="C131" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D131" s="11">
         <f>SUM(D120:D128)</f>
         <v>208.53000000000003</v>
       </c>

</xml_diff>